<commit_message>
Update automatico via Actualizar 06-17-2020 04-30-18
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Panama/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1086" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3A00BDFD-6592-4557-A331-694DE3DD7A76}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="0" windowWidth="13296" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:R541"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G547" sqref="G547"/>
+      <pane ySplit="3" topLeftCell="A525" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E544" sqref="E544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9314,10 +9314,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-20-2020 02-06-29
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Panama/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1086" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3A00BDFD-6592-4557-A331-694DE3DD7A76}"/>
+  <xr:revisionPtr revIDLastSave="1087" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A2C46382-D909-410C-AA4C-EDC27ECB3BFB}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="0" windowWidth="13296" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:R541"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A525" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E544" sqref="E544"/>
+      <pane ySplit="3" topLeftCell="A526" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A551" sqref="A551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3291,7 +3291,9 @@
       </c>
       <c r="M43" s="21"/>
       <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
+      <c r="O43" s="2">
+        <v>533206.50499999989</v>
+      </c>
       <c r="P43" s="2">
         <v>403.34</v>
       </c>
@@ -9314,10 +9316,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-26-2020 23-14-12
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Panama/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1095" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{71CF25EA-636C-4D02-959D-20FE2C60326D}"/>
+  <xr:revisionPtr revIDLastSave="1105" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E5BF6134-799B-4670-B31C-6A016063464B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8412" yWindow="0" windowWidth="14616" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="99">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1063,6 +1063,56 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF5D7B9D"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1207,56 +1257,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF5D7B9D"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9E2F3"/>
@@ -1300,13 +1300,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H550" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H550" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H555" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A3:H555" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Banano" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Harina de Pescado" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Banano" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Harina de Pescado" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Gasolina Superior"/>
     <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular"/>
     <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel"/>
@@ -1317,18 +1317,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R46" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R46" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="13" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="10">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8FC1825F-E2AC-4830-AA41-5B12F2C15972}" name="Índice Mensual de Actividad Económica "/>
-    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="4" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="3" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="2" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="9" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="8" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="7" dataCellStyle="Millares"/>
     <tableColumn id="8" xr3:uid="{1A570E63-F800-45DF-9E5A-B8961BEFE222}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{7E984A16-0976-4747-9D31-12709D8A9C2E}" name="Ingesos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1337,7 +1337,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="6">
   <autoFilter ref="A1:U23" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1360,7 +1360,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1632,11 +1632,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R550"/>
+  <dimension ref="A1:R555"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A531" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A556" sqref="A556"/>
+      <pane ySplit="3" topLeftCell="A539" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A560" sqref="A560"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3377,7 +3377,7 @@
         <v>24</v>
       </c>
       <c r="L46" s="9" t="str">
-        <f t="shared" ref="L46" si="2">+K46&amp;", "&amp;J46</f>
+        <f t="shared" ref="L46:L47" si="2">+K46&amp;", "&amp;J46</f>
         <v>Julio, 2020</v>
       </c>
       <c r="M46" s="21"/>
@@ -3399,13 +3399,20 @@
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
       <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21"/>
+      <c r="J47" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L47" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v>Agosto, 2020</v>
+      </c>
       <c r="M47" s="21"/>
-      <c r="N47" s="21"/>
-      <c r="O47" s="21"/>
-      <c r="P47" s="21"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
       <c r="Q47" s="21"/>
       <c r="R47" s="21"/>
     </row>
@@ -8701,8 +8708,12 @@
         <v>43952</v>
       </c>
       <c r="B490" s="21"/>
-      <c r="C490" s="21"/>
-      <c r="D490" s="21"/>
+      <c r="C490" s="21">
+        <v>1.3</v>
+      </c>
+      <c r="D490" s="23">
+        <v>1392.96</v>
+      </c>
       <c r="E490" s="21"/>
       <c r="F490" s="21"/>
       <c r="G490" s="21"/>
@@ -9386,6 +9397,46 @@
       <c r="B550" s="25"/>
       <c r="C550" s="25"/>
       <c r="D550" s="25"/>
+    </row>
+    <row r="551" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A551" s="8">
+        <v>44013</v>
+      </c>
+      <c r="B551" s="25"/>
+      <c r="C551" s="25"/>
+      <c r="D551" s="25"/>
+    </row>
+    <row r="552" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A552" s="8">
+        <v>44014</v>
+      </c>
+      <c r="B552" s="25"/>
+      <c r="C552" s="25"/>
+      <c r="D552" s="25"/>
+    </row>
+    <row r="553" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A553" s="8">
+        <v>44015</v>
+      </c>
+      <c r="B553" s="25"/>
+      <c r="C553" s="25"/>
+      <c r="D553" s="25"/>
+    </row>
+    <row r="554" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A554" s="8">
+        <v>44016</v>
+      </c>
+      <c r="B554" s="25"/>
+      <c r="C554" s="25"/>
+      <c r="D554" s="25"/>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A555" s="8">
+        <v>44017</v>
+      </c>
+      <c r="B555" s="25"/>
+      <c r="C555" s="25"/>
+      <c r="D555" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -9406,10 +9457,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-01-2020 03-25-55
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1105" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E5BF6134-799B-4670-B31C-6A016063464B}"/>
   <bookViews>
-    <workbookView xWindow="8412" yWindow="0" windowWidth="14616" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7992" yWindow="0" windowWidth="15024" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1063,56 +1063,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF5D7B9D"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1257,6 +1207,56 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF5D7B9D"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9E2F3"/>
@@ -1300,13 +1300,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H555" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H555" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A3:H555" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Banano" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Harina de Pescado" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Banano" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Harina de Pescado" dataDxfId="9"/>
     <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Gasolina Superior"/>
     <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular"/>
     <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel"/>
@@ -1317,18 +1317,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="13" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8FC1825F-E2AC-4830-AA41-5B12F2C15972}" name="Índice Mensual de Actividad Económica "/>
-    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="9" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="8" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="7" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="3" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="2" dataCellStyle="Millares"/>
     <tableColumn id="8" xr3:uid="{1A570E63-F800-45DF-9E5A-B8961BEFE222}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{7E984A16-0976-4747-9D31-12709D8A9C2E}" name="Ingesos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1337,7 +1337,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="1">
   <autoFilter ref="A1:U23" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1360,7 +1360,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:R555"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A539" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A560" sqref="A560"/>
+      <pane ySplit="3" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A558" sqref="A558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9460,7 +9460,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-04-2020 01-38-05
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Panama/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1105" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E5BF6134-799B-4670-B31C-6A016063464B}"/>
+  <xr:revisionPtr revIDLastSave="1120" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B79EDFAF-0483-4B14-804E-3977D007B83E}"/>
   <bookViews>
-    <workbookView xWindow="7992" yWindow="0" windowWidth="15024" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8208" yWindow="0" windowWidth="14808" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:R555"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A558" sqref="A558"/>
+      <pane ySplit="3" topLeftCell="A537" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A561" sqref="A561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3173,7 +3173,7 @@
         <v>Enero, 2020</v>
       </c>
       <c r="M40" s="24">
-        <v>340.19246193075492</v>
+        <v>339.56602505061431</v>
       </c>
       <c r="N40" s="2">
         <v>51503.478000000003</v>
@@ -3210,7 +3210,7 @@
         <v>Febrero, 2020</v>
       </c>
       <c r="M41" s="24">
-        <v>334.16091635711257</v>
+        <v>333.99133203105765</v>
       </c>
       <c r="N41" s="2">
         <v>54227.436999999991</v>
@@ -3247,7 +3247,7 @@
         <v>Marzo, 2020</v>
       </c>
       <c r="M42" s="24">
-        <v>369.50921717470578</v>
+        <v>366.43683999641081</v>
       </c>
       <c r="N42" s="2">
         <v>69413.402000000002</v>
@@ -3289,8 +3289,12 @@
         <f t="shared" si="0"/>
         <v>Abril, 2020</v>
       </c>
-      <c r="M43" s="21"/>
-      <c r="N43" s="2"/>
+      <c r="M43" s="24">
+        <v>217.92340191398858</v>
+      </c>
+      <c r="N43" s="2">
+        <v>59005.919000000002</v>
+      </c>
       <c r="O43" s="2">
         <v>533206.50499999989</v>
       </c>
@@ -3322,11 +3326,13 @@
         <f t="shared" si="0"/>
         <v>Mayo, 2020</v>
       </c>
-      <c r="M44" s="21"/>
+      <c r="M44" s="24"/>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="21"/>
+      <c r="P44" s="2">
+        <v>375.5</v>
+      </c>
+      <c r="Q44" s="2"/>
       <c r="R44" s="21"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
@@ -3351,11 +3357,11 @@
         <f t="shared" ref="L45" si="1">+K45&amp;", "&amp;J45</f>
         <v>Junio, 2020</v>
       </c>
-      <c r="M45" s="21"/>
+      <c r="M45" s="24"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
-      <c r="Q45" s="21"/>
+      <c r="Q45" s="2"/>
       <c r="R45" s="21"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
@@ -3380,11 +3386,11 @@
         <f t="shared" ref="L46:L47" si="2">+K46&amp;", "&amp;J46</f>
         <v>Julio, 2020</v>
       </c>
-      <c r="M46" s="21"/>
+      <c r="M46" s="24"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
-      <c r="Q46" s="21"/>
+      <c r="Q46" s="2"/>
       <c r="R46" s="21"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
@@ -3409,11 +3415,11 @@
         <f t="shared" si="2"/>
         <v>Agosto, 2020</v>
       </c>
-      <c r="M47" s="21"/>
+      <c r="M47" s="24"/>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
-      <c r="Q47" s="21"/>
+      <c r="Q47" s="2"/>
       <c r="R47" s="21"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
@@ -9350,7 +9356,7 @@
       <c r="C544" s="25"/>
       <c r="D544" s="25"/>
     </row>
-    <row r="545" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A545" s="8">
         <v>44007</v>
       </c>
@@ -9358,7 +9364,7 @@
       <c r="C545" s="25"/>
       <c r="D545" s="25"/>
     </row>
-    <row r="546" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A546" s="8">
         <v>44008</v>
       </c>
@@ -9366,15 +9372,24 @@
       <c r="C546" s="25"/>
       <c r="D546" s="25"/>
     </row>
-    <row r="547" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A547" s="8">
         <v>44009</v>
       </c>
       <c r="B547" s="25"/>
       <c r="C547" s="25"/>
       <c r="D547" s="25"/>
-    </row>
-    <row r="548" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E547">
+        <v>2.35</v>
+      </c>
+      <c r="F547">
+        <v>2.29</v>
+      </c>
+      <c r="G547">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="548" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A548" s="8">
         <v>44010</v>
       </c>
@@ -9382,7 +9397,7 @@
       <c r="C548" s="25"/>
       <c r="D548" s="25"/>
     </row>
-    <row r="549" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A549" s="8">
         <v>44011</v>
       </c>
@@ -9390,7 +9405,7 @@
       <c r="C549" s="25"/>
       <c r="D549" s="25"/>
     </row>
-    <row r="550" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A550" s="8">
         <v>44012</v>
       </c>
@@ -9398,7 +9413,7 @@
       <c r="C550" s="25"/>
       <c r="D550" s="25"/>
     </row>
-    <row r="551" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A551" s="8">
         <v>44013</v>
       </c>
@@ -9406,7 +9421,7 @@
       <c r="C551" s="25"/>
       <c r="D551" s="25"/>
     </row>
-    <row r="552" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A552" s="8">
         <v>44014</v>
       </c>
@@ -9414,7 +9429,7 @@
       <c r="C552" s="25"/>
       <c r="D552" s="25"/>
     </row>
-    <row r="553" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A553" s="8">
         <v>44015</v>
       </c>
@@ -9422,7 +9437,7 @@
       <c r="C553" s="25"/>
       <c r="D553" s="25"/>
     </row>
-    <row r="554" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A554" s="8">
         <v>44016</v>
       </c>
@@ -9430,7 +9445,7 @@
       <c r="C554" s="25"/>
       <c r="D554" s="25"/>
     </row>
-    <row r="555" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A555" s="8">
         <v>44017</v>
       </c>
@@ -9460,7 +9475,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-08-2020 01-52-07
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Panama/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1120" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B79EDFAF-0483-4B14-804E-3977D007B83E}"/>
+  <xr:revisionPtr revIDLastSave="1121" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D9CC28B-5D1C-42DE-A8E9-577EDE986383}"/>
   <bookViews>
-    <workbookView xWindow="8208" yWindow="0" windowWidth="14808" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -8714,12 +8714,8 @@
         <v>43952</v>
       </c>
       <c r="B490" s="21"/>
-      <c r="C490" s="21">
-        <v>1.3</v>
-      </c>
-      <c r="D490" s="23">
-        <v>1392.96</v>
-      </c>
+      <c r="C490" s="25"/>
+      <c r="D490" s="25"/>
       <c r="E490" s="21"/>
       <c r="F490" s="21"/>
       <c r="G490" s="21"/>
@@ -9101,8 +9097,12 @@
         <v>43982</v>
       </c>
       <c r="B520" s="21"/>
-      <c r="C520" s="21"/>
-      <c r="D520" s="21"/>
+      <c r="C520" s="21">
+        <v>1.3</v>
+      </c>
+      <c r="D520" s="23">
+        <v>1392.96</v>
+      </c>
       <c r="E520" s="21"/>
       <c r="F520" s="21"/>
       <c r="G520" s="21"/>
@@ -9475,7 +9475,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-11-2020 06-03-17
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1121" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D9CC28B-5D1C-42DE-A8E9-577EDE986383}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5784" yWindow="0" windowWidth="17220" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:R555"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A537" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A561" sqref="A561"/>
+      <pane ySplit="3" topLeftCell="A543" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A562" sqref="A562"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9475,7 +9475,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-15-2020 02-15-04
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Panama/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1121" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D9CC28B-5D1C-42DE-A8E9-577EDE986383}"/>
+  <xr:revisionPtr revIDLastSave="1130" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{12AE38F6-9B62-422C-A42D-79C59F4CE46D}"/>
   <bookViews>
-    <workbookView xWindow="5784" yWindow="0" windowWidth="17220" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7464" yWindow="696" windowWidth="15552" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1300,8 +1300,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H555" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H555" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H569" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H569" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1632,11 +1632,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R555"/>
+  <dimension ref="A1:R569"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A543" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A562" sqref="A562"/>
+      <pane ySplit="3" topLeftCell="A553" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E571" sqref="E571"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9444,6 +9444,15 @@
       <c r="B554" s="25"/>
       <c r="C554" s="25"/>
       <c r="D554" s="25"/>
+      <c r="E554">
+        <v>2.35</v>
+      </c>
+      <c r="F554" s="21">
+        <v>2.29</v>
+      </c>
+      <c r="G554" s="21">
+        <v>1.9</v>
+      </c>
     </row>
     <row r="555" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A555" s="8">
@@ -9452,6 +9461,127 @@
       <c r="B555" s="25"/>
       <c r="C555" s="25"/>
       <c r="D555" s="25"/>
+    </row>
+    <row r="556" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A556" s="8">
+        <v>44018</v>
+      </c>
+      <c r="B556" s="25"/>
+      <c r="C556" s="25"/>
+      <c r="D556" s="25"/>
+    </row>
+    <row r="557" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A557" s="8">
+        <v>44019</v>
+      </c>
+      <c r="B557" s="25"/>
+      <c r="C557" s="25"/>
+      <c r="D557" s="25"/>
+    </row>
+    <row r="558" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A558" s="8">
+        <v>44020</v>
+      </c>
+      <c r="B558" s="25"/>
+      <c r="C558" s="25"/>
+      <c r="D558" s="25"/>
+    </row>
+    <row r="559" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A559" s="8">
+        <v>44021</v>
+      </c>
+      <c r="B559" s="25"/>
+      <c r="C559" s="25"/>
+      <c r="D559" s="25"/>
+    </row>
+    <row r="560" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A560" s="8">
+        <v>44022</v>
+      </c>
+      <c r="B560" s="25"/>
+      <c r="C560" s="25"/>
+      <c r="D560" s="25"/>
+    </row>
+    <row r="561" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A561" s="8">
+        <v>44023</v>
+      </c>
+      <c r="B561" s="25"/>
+      <c r="C561" s="25"/>
+      <c r="D561" s="25"/>
+      <c r="E561">
+        <v>2.42</v>
+      </c>
+      <c r="F561">
+        <v>2.35</v>
+      </c>
+      <c r="G561">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A562" s="8">
+        <v>44024</v>
+      </c>
+      <c r="B562" s="25"/>
+      <c r="C562" s="25"/>
+      <c r="D562" s="25"/>
+    </row>
+    <row r="563" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A563" s="8">
+        <v>44025</v>
+      </c>
+      <c r="B563" s="25"/>
+      <c r="C563" s="25"/>
+      <c r="D563" s="25"/>
+    </row>
+    <row r="564" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A564" s="8">
+        <v>44026</v>
+      </c>
+      <c r="B564" s="25"/>
+      <c r="C564" s="25"/>
+      <c r="D564" s="25"/>
+    </row>
+    <row r="565" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A565" s="8">
+        <v>44027</v>
+      </c>
+      <c r="B565" s="25"/>
+      <c r="C565" s="25"/>
+      <c r="D565" s="25"/>
+    </row>
+    <row r="566" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A566" s="8">
+        <v>44028</v>
+      </c>
+      <c r="B566" s="25"/>
+      <c r="C566" s="25"/>
+      <c r="D566" s="25"/>
+    </row>
+    <row r="567" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A567" s="8">
+        <v>44029</v>
+      </c>
+      <c r="B567" s="25"/>
+      <c r="C567" s="25"/>
+      <c r="D567" s="25"/>
+    </row>
+    <row r="568" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A568" s="8">
+        <v>44030</v>
+      </c>
+      <c r="B568" s="25"/>
+      <c r="C568" s="25"/>
+      <c r="D568" s="25"/>
+    </row>
+    <row r="569" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A569" s="8">
+        <v>44031</v>
+      </c>
+      <c r="B569" s="25"/>
+      <c r="C569" s="25"/>
+      <c r="D569" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -9475,7 +9605,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-25-2020 02-57-09
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944d5b9328a00097/Proyectos/Data intelligence/Covid-19/Panama/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Panama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1136" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C564F5E4-A314-4E45-A556-9CB75E961416}"/>
+  <xr:revisionPtr revIDLastSave="1136" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{C564F5E4-A314-4E45-A556-9CB75E961416}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10128" yWindow="1248" windowWidth="12912" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:R576"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A561" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E583" sqref="E583"/>
+      <pane ySplit="3" topLeftCell="A554" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A579" sqref="A579"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9669,7 +9669,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-01-2020 00-51-49
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Panama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1138" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{A8BC490A-F996-4519-867B-75E8D1B1E77B}"/>
+  <xr:revisionPtr revIDLastSave="1138" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A8BC490A-F996-4519-867B-75E8D1B1E77B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8736" yWindow="0" windowWidth="14268" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
     <sheet name="Fuentes" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1632,9 +1634,9 @@
   </sheetPr>
   <dimension ref="A1:R576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A561" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A584" sqref="A584"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9667,7 +9669,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-08-2020 00-41-11
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Panama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1157" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{711844A7-F7C0-4915-9CCB-E9F71D8A4B8D}"/>
+  <xr:revisionPtr revIDLastSave="1159" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E8D56E48-A941-4EFA-89C7-97213D807BD6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1635,8 +1635,8 @@
   <dimension ref="A1:R590"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A574" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A595" sqref="A595"/>
+      <pane ySplit="3" topLeftCell="A577" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A602" sqref="A602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3326,7 +3326,9 @@
         <f t="shared" si="0"/>
         <v>Mayo, 2020</v>
       </c>
-      <c r="M44" s="24"/>
+      <c r="M44" s="24">
+        <v>193.83678840082644</v>
+      </c>
       <c r="N44" s="2">
         <v>44765.543999999994</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-12-2020 02-00-51
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Panama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1159" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E8D56E48-A941-4EFA-89C7-97213D807BD6}"/>
+  <xr:revisionPtr revIDLastSave="1166" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{75E0FB4E-1BD3-4B0D-9C64-AC55FEF162A5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1300,8 +1300,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H590" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H590" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H597" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H597" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1632,11 +1632,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R590"/>
+  <dimension ref="A1:R597"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A577" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A602" sqref="A602"/>
+      <pane ySplit="3" topLeftCell="A580" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A605" sqref="A605"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9710,8 +9710,12 @@
         <v>44043</v>
       </c>
       <c r="B581" s="25"/>
-      <c r="C581" s="25"/>
-      <c r="D581" s="25"/>
+      <c r="C581" s="25">
+        <v>1.27</v>
+      </c>
+      <c r="D581" s="23">
+        <v>1486.92</v>
+      </c>
     </row>
     <row r="582" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A582" s="8">
@@ -9785,6 +9789,15 @@
       <c r="B589" s="25"/>
       <c r="C589" s="25"/>
       <c r="D589" s="25"/>
+      <c r="E589">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="F589">
+        <v>2.37</v>
+      </c>
+      <c r="G589">
+        <v>2.06</v>
+      </c>
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A590" s="8">
@@ -9793,6 +9806,62 @@
       <c r="B590" s="25"/>
       <c r="C590" s="25"/>
       <c r="D590" s="25"/>
+    </row>
+    <row r="591" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A591" s="8">
+        <v>44053</v>
+      </c>
+      <c r="B591" s="25"/>
+      <c r="C591" s="25"/>
+      <c r="D591" s="25"/>
+    </row>
+    <row r="592" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A592" s="8">
+        <v>44054</v>
+      </c>
+      <c r="B592" s="25"/>
+      <c r="C592" s="25"/>
+      <c r="D592" s="25"/>
+    </row>
+    <row r="593" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A593" s="8">
+        <v>44055</v>
+      </c>
+      <c r="B593" s="25"/>
+      <c r="C593" s="25"/>
+      <c r="D593" s="25"/>
+    </row>
+    <row r="594" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A594" s="8">
+        <v>44056</v>
+      </c>
+      <c r="B594" s="25"/>
+      <c r="C594" s="25"/>
+      <c r="D594" s="25"/>
+    </row>
+    <row r="595" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A595" s="8">
+        <v>44057</v>
+      </c>
+      <c r="B595" s="25"/>
+      <c r="C595" s="25"/>
+      <c r="D595" s="25"/>
+    </row>
+    <row r="596" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A596" s="8">
+        <v>44058</v>
+      </c>
+      <c r="B596" s="25"/>
+      <c r="C596" s="25"/>
+      <c r="D596" s="25"/>
+    </row>
+    <row r="597" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A597" s="8">
+        <v>44059</v>
+      </c>
+      <c r="B597" s="25"/>
+      <c r="C597" s="25"/>
+      <c r="D597" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -9816,7 +9885,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-19-2020 14-43-52
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1167" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE2DBC69-7A9C-4BE7-BCC4-3539132476DE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="0" windowWidth="14904" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1633,7 +1633,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A581" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B599" sqref="B599"/>
+      <selection pane="bottomLeft" activeCell="E599" sqref="E599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9882,7 +9882,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-22-2020 02-08-05
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Panama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1167" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE2DBC69-7A9C-4BE7-BCC4-3539132476DE}"/>
+  <xr:revisionPtr revIDLastSave="1172" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{52F32E3F-6AEB-4AD3-90ED-0123C5807AF2}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="0" windowWidth="14904" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1297,8 +1297,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H597" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H597" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H604" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H604" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1629,11 +1629,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R597"/>
+  <dimension ref="A1:R604"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A581" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E599" sqref="E599"/>
+      <pane ySplit="3" topLeftCell="A595" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A606" sqref="A606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9820,7 +9820,7 @@
       <c r="C592" s="25"/>
       <c r="D592" s="25"/>
     </row>
-    <row r="593" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A593" s="8">
         <v>44055</v>
       </c>
@@ -9828,7 +9828,7 @@
       <c r="C593" s="25"/>
       <c r="D593" s="25"/>
     </row>
-    <row r="594" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A594" s="8">
         <v>44056</v>
       </c>
@@ -9836,7 +9836,7 @@
       <c r="C594" s="25"/>
       <c r="D594" s="25"/>
     </row>
-    <row r="595" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A595" s="8">
         <v>44057</v>
       </c>
@@ -9844,21 +9844,86 @@
       <c r="C595" s="25"/>
       <c r="D595" s="25"/>
     </row>
-    <row r="596" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A596" s="8">
         <v>44058</v>
       </c>
       <c r="B596" s="25"/>
       <c r="C596" s="25"/>
       <c r="D596" s="25"/>
-    </row>
-    <row r="597" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E596">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="F596">
+        <v>2.37</v>
+      </c>
+      <c r="G596">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="597" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A597" s="8">
         <v>44059</v>
       </c>
       <c r="B597" s="25"/>
       <c r="C597" s="25"/>
       <c r="D597" s="25"/>
+    </row>
+    <row r="598" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A598" s="8">
+        <v>44060</v>
+      </c>
+      <c r="B598" s="25"/>
+      <c r="C598" s="25"/>
+      <c r="D598" s="25"/>
+    </row>
+    <row r="599" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A599" s="8">
+        <v>44061</v>
+      </c>
+      <c r="B599" s="25"/>
+      <c r="C599" s="25"/>
+      <c r="D599" s="25"/>
+    </row>
+    <row r="600" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A600" s="8">
+        <v>44062</v>
+      </c>
+      <c r="B600" s="25"/>
+      <c r="C600" s="25"/>
+      <c r="D600" s="25"/>
+    </row>
+    <row r="601" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A601" s="8">
+        <v>44063</v>
+      </c>
+      <c r="B601" s="25"/>
+      <c r="C601" s="25"/>
+      <c r="D601" s="25"/>
+    </row>
+    <row r="602" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A602" s="8">
+        <v>44064</v>
+      </c>
+      <c r="B602" s="25"/>
+      <c r="C602" s="25"/>
+      <c r="D602" s="25"/>
+    </row>
+    <row r="603" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A603" s="8">
+        <v>44065</v>
+      </c>
+      <c r="B603" s="25"/>
+      <c r="C603" s="25"/>
+      <c r="D603" s="25"/>
+    </row>
+    <row r="604" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A604" s="8">
+        <v>44066</v>
+      </c>
+      <c r="B604" s="25"/>
+      <c r="C604" s="25"/>
+      <c r="D604" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -9882,7 +9947,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-29-2020 00-38-35
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1175" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FF0E637-7B0E-4D03-81D3-F58E5B1703C5}"/>
   <bookViews>
-    <workbookView xWindow="11484" yWindow="0" windowWidth="11544" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:R611"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A597" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A621" sqref="A621"/>
+      <pane ySplit="3" topLeftCell="A593" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A618" sqref="A618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10007,10 +10007,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-02-2020 00-48-24
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Panama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1175" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FF0E637-7B0E-4D03-81D3-F58E5B1703C5}"/>
+  <xr:revisionPtr revIDLastSave="1180" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84ECCE2D-CE7E-4190-BB38-F8F49EF9A5DB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="98">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1314,8 +1314,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R47" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R47" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R48" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R48" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:R611"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A593" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A618" sqref="A618"/>
+      <pane ySplit="3" topLeftCell="A594" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A619" sqref="A619"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3256,7 +3256,9 @@
         <v>425.56</v>
       </c>
       <c r="Q42" s="2"/>
-      <c r="R42" s="21"/>
+      <c r="R42" s="21">
+        <v>-56.3</v>
+      </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
@@ -3368,7 +3370,7 @@
         <v>523101.42599999998</v>
       </c>
       <c r="P45" s="2">
-        <v>376.09</v>
+        <v>367.61</v>
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="21"/>
@@ -3398,7 +3400,9 @@
       <c r="M46" s="24"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
+      <c r="P46" s="2">
+        <v>367.61</v>
+      </c>
       <c r="Q46" s="2"/>
       <c r="R46" s="21"/>
     </row>
@@ -3443,13 +3447,20 @@
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="21"/>
+      <c r="J48" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K48" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L48" s="9" t="str">
+        <f t="shared" ref="L48" si="3">+K48&amp;", "&amp;J48</f>
+        <v>Septiembre, 2020</v>
+      </c>
       <c r="M48" s="21"/>
-      <c r="N48" s="21"/>
-      <c r="O48" s="21"/>
-      <c r="P48" s="21"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
       <c r="Q48" s="21"/>
       <c r="R48" s="21"/>
     </row>
@@ -10010,7 +10021,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-05-2020 02-08-30
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reyes.rodriguezucv@gmail.com\OneDrive\Proyectos\Data intelligence\Covid-19\Panama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1180" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84ECCE2D-CE7E-4190-BB38-F8F49EF9A5DB}"/>
+  <xr:revisionPtr revIDLastSave="1182" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1FE479EE-9943-4D2A-B825-FB84725F8614}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1633,7 +1633,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A594" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A619" sqref="A619"/>
+      <selection pane="bottomLeft" activeCell="A616" sqref="A616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10021,7 +10021,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-11-2020 22-41-42
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1182" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1FE479EE-9943-4D2A-B825-FB84725F8614}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1632,7 +1632,7 @@
   <dimension ref="A1:R611"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A596" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A600" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A621" sqref="A621"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-17-2020 22-39-05
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:R632"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A620" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A635" sqref="A635"/>
+      <pane ySplit="3" topLeftCell="A624" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A634" sqref="A634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10243,7 +10243,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-26-2020 00-40-13
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1217" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E3C2CAAC-FF8D-4A8D-8BE2-8DEE7706844D}"/>
+  <xr:revisionPtr revIDLastSave="1219" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{11B8B756-3FC1-4FFC-A332-833C8A6E9252}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:R639"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A626" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A646" sqref="A646"/>
+      <pane ySplit="3" topLeftCell="A632" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B641" sqref="B641"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 09-30-2020 00-41-54
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1219" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{11B8B756-3FC1-4FFC-A332-833C8A6E9252}"/>
+  <xr:revisionPtr revIDLastSave="1221" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5FF551ED-A17E-4E65-854A-1BC346941723}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:R639"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A632" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B641" sqref="B641"/>
+      <pane ySplit="3" topLeftCell="A630" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A645" sqref="A645"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10026,8 +10026,12 @@
         <v>44074</v>
       </c>
       <c r="B612" s="25"/>
-      <c r="C612" s="25"/>
-      <c r="D612" s="25"/>
+      <c r="C612" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="D612" s="23">
+        <v>1479.92</v>
+      </c>
       <c r="H612" s="21"/>
     </row>
     <row r="613" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-03-2020 00-38-47
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1221" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5FF551ED-A17E-4E65-854A-1BC346941723}"/>
+  <xr:revisionPtr revIDLastSave="1225" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0EFF54CE-C568-488C-87E4-6ED193B5B111}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1297,8 +1297,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H639" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H639" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H646" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H646" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1629,11 +1629,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R639"/>
+  <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A630" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A645" sqref="A645"/>
+      <pane ySplit="3" topLeftCell="A635" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A650" sqref="A650"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3434,8 +3434,12 @@
       </c>
       <c r="M47" s="24"/>
       <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
+      <c r="O47" s="2">
+        <v>584213.68099999998</v>
+      </c>
+      <c r="P47" s="2">
+        <v>368.93</v>
+      </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="21"/>
     </row>
@@ -10289,6 +10293,62 @@
       <c r="B639" s="25"/>
       <c r="C639" s="25"/>
       <c r="D639" s="25"/>
+    </row>
+    <row r="640" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A640" s="8">
+        <v>44102</v>
+      </c>
+      <c r="B640" s="25"/>
+      <c r="C640" s="25"/>
+      <c r="D640" s="25"/>
+    </row>
+    <row r="641" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A641" s="8">
+        <v>44103</v>
+      </c>
+      <c r="B641" s="25"/>
+      <c r="C641" s="25"/>
+      <c r="D641" s="25"/>
+    </row>
+    <row r="642" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A642" s="8">
+        <v>44104</v>
+      </c>
+      <c r="B642" s="25"/>
+      <c r="C642" s="25"/>
+      <c r="D642" s="25"/>
+    </row>
+    <row r="643" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A643" s="8">
+        <v>44105</v>
+      </c>
+      <c r="B643" s="25"/>
+      <c r="C643" s="25"/>
+      <c r="D643" s="25"/>
+    </row>
+    <row r="644" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A644" s="8">
+        <v>44106</v>
+      </c>
+      <c r="B644" s="25"/>
+      <c r="C644" s="25"/>
+      <c r="D644" s="25"/>
+    </row>
+    <row r="645" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A645" s="8">
+        <v>44107</v>
+      </c>
+      <c r="B645" s="25"/>
+      <c r="C645" s="25"/>
+      <c r="D645" s="25"/>
+    </row>
+    <row r="646" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A646" s="8">
+        <v>44108</v>
+      </c>
+      <c r="B646" s="25"/>
+      <c r="C646" s="25"/>
+      <c r="D646" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -10312,7 +10372,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-06-2020 22-40-43
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A635" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A650" sqref="A650"/>
+      <pane ySplit="3" topLeftCell="A627" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A652" sqref="A652"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10372,7 +10372,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-10-2020 02-10-23
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1225" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0EFF54CE-C568-488C-87E4-6ED193B5B111}"/>
+  <xr:revisionPtr revIDLastSave="1227" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{081292B3-B85A-4AE1-8142-69A0920BB157}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A627" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A652" sqref="A652"/>
+      <pane ySplit="3" topLeftCell="A637" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A651" sqref="A651"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10372,7 +10372,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-14-2020 02-11-06
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1227" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{081292B3-B85A-4AE1-8142-69A0920BB157}"/>
+  <xr:revisionPtr revIDLastSave="1229" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BFF08B96-EBCC-40F9-9F41-21F0A6898C10}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1633,7 +1633,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A637" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A651" sqref="A651"/>
+      <selection pane="bottomLeft" activeCell="A652" sqref="A652"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10372,7 +10372,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-17-2020 00-39-33
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1229" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BFF08B96-EBCC-40F9-9F41-21F0A6898C10}"/>
+  <xr:revisionPtr revIDLastSave="1232" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84A208AE-9049-463B-A1A2-0370A4BBBF3A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A637" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A652" sqref="A652"/>
+      <pane ySplit="3" topLeftCell="A639" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A647" sqref="A647"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3433,7 +3433,9 @@
         <v>Agosto, 2020</v>
       </c>
       <c r="M47" s="24"/>
-      <c r="N47" s="2"/>
+      <c r="N47" s="2">
+        <v>50175.788</v>
+      </c>
       <c r="O47" s="2">
         <v>584213.68099999998</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-21-2020 00-38-41
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1232" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84A208AE-9049-463B-A1A2-0370A4BBBF3A}"/>
+  <xr:revisionPtr revIDLastSave="1234" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F5DEC077-4BD9-4801-8323-47DFEAA96334}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1632,8 +1632,8 @@
   <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A639" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A647" sqref="A647"/>
+      <pane ySplit="3" topLeftCell="A634" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A649" sqref="A649"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-24-2020 00-40-06
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1234" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F5DEC077-4BD9-4801-8323-47DFEAA96334}"/>
+  <xr:revisionPtr revIDLastSave="1241" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AD706504-121F-4092-9509-1C4BC16EDFF2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="102">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -361,6 +361,18 @@
   <si>
     <t>configuración regional de EE.UU.</t>
   </si>
+  <si>
+    <t>Combustible Gasolina Superior (USD/Galón)</t>
+  </si>
+  <si>
+    <t>Combustible Regular (USD/Galón)</t>
+  </si>
+  <si>
+    <t>Combustible Diesel (USD/Galón)</t>
+  </si>
+  <si>
+    <t>https://sen.hn/informe-estadistico-semanal-de-cchac/</t>
+  </si>
 </sst>
 </file>
 
@@ -373,7 +385,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +602,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -916,7 +936,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -963,8 +983,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1009,8 +1030,9 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="46" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="47">
     <cellStyle name="20% - Énfasis1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="28" builtinId="38" customBuiltin="1"/>
@@ -1042,6 +1064,7 @@
     <cellStyle name="Énfasis5" xfId="35" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis6" xfId="39" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="46" builtinId="8"/>
     <cellStyle name="Hipervínculo 2" xfId="44" xr:uid="{D1D5AC69-E029-407D-8457-44EF34D97FF6}"/>
     <cellStyle name="Incorrecto" xfId="8" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1632,8 +1655,8 @@
   <dimension ref="A1:R646"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A634" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A649" sqref="A649"/>
+      <pane ySplit="3" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A648" sqref="A648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10287,6 +10310,15 @@
       <c r="B638" s="25"/>
       <c r="C638" s="25"/>
       <c r="D638" s="25"/>
+      <c r="E638">
+        <v>2.48</v>
+      </c>
+      <c r="F638" s="21">
+        <v>2.41</v>
+      </c>
+      <c r="G638" s="21">
+        <v>1.99</v>
+      </c>
     </row>
     <row r="639" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A639" s="8">
@@ -10371,10 +10403,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10597,7 +10629,7 @@
         <v>53</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>67</v>
@@ -10654,7 +10686,7 @@
         <v>53</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>67</v>
@@ -10711,7 +10743,7 @@
         <v>53</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>67</v>
@@ -11113,10 +11145,18 @@
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="16"/>
+      <c r="C14" s="12">
+        <v>7</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>101</v>
+      </c>
       <c r="G14" s="12"/>
       <c r="H14" s="13"/>
       <c r="I14" s="12"/>
@@ -12332,12 +12372,13 @@
     <hyperlink ref="H10" r:id="rId22" display="cie_inec@contraloria.gob.pa" xr:uid="{89F510B2-5C68-4D03-A1F1-EFFB3447A280}"/>
     <hyperlink ref="F6" r:id="rId23" xr:uid="{A63B55D0-3F47-4A34-8619-62920F88C6BD}"/>
     <hyperlink ref="F4:F5" r:id="rId24" display="http://www.energia.gob.pa/precios/?tag=255" xr:uid="{CC5C4EC3-A3ED-46B0-9857-4D54C9FB54E0}"/>
+    <hyperlink ref="F14" r:id="rId25" xr:uid="{3987BD5B-4929-4737-915E-69B483BD1681}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId25"/>
+  <legacyDrawing r:id="rId26"/>
   <tableParts count="1">
-    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 10-28-2020 00-40-32
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1241" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AD706504-121F-4092-9509-1C4BC16EDFF2}"/>
+  <xr:revisionPtr revIDLastSave="1243" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0CCFF9A-361A-4295-826F-BE83E689C715}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1654,9 +1654,9 @@
   </sheetPr>
   <dimension ref="A1:R646"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A648" sqref="A648"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10349,8 +10349,12 @@
         <v>44104</v>
       </c>
       <c r="B642" s="25"/>
-      <c r="C642" s="25"/>
-      <c r="D642" s="25"/>
+      <c r="C642" s="25">
+        <v>1.24</v>
+      </c>
+      <c r="D642" s="23">
+        <v>1477.77</v>
+      </c>
     </row>
     <row r="643" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A643" s="8">
@@ -10403,10 +10407,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-28-2020 02-09-44
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1654,9 +1654,9 @@
   </sheetPr>
   <dimension ref="A1:R646"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O48" sqref="O48"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A638" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A653" sqref="A653"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10410,7 +10410,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 10-31-2020 00-39-08
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1243" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0CCFF9A-361A-4295-826F-BE83E689C715}"/>
+  <xr:revisionPtr revIDLastSave="1245" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A9C0D8ED-0392-426A-A9AA-5C9A6111CF84}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1320,8 +1320,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H646" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H646" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H653" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H653" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1652,11 +1652,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R646"/>
+  <dimension ref="A1:R653"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A638" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A653" sqref="A653"/>
+      <pane ySplit="3" topLeftCell="A644" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A659" sqref="A659"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10388,6 +10388,62 @@
       <c r="C646" s="25"/>
       <c r="D646" s="25"/>
     </row>
+    <row r="647" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A647" s="8">
+        <v>44109</v>
+      </c>
+      <c r="B647" s="25"/>
+      <c r="C647" s="25"/>
+      <c r="D647" s="25"/>
+    </row>
+    <row r="648" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A648" s="8">
+        <v>44110</v>
+      </c>
+      <c r="B648" s="25"/>
+      <c r="C648" s="25"/>
+      <c r="D648" s="25"/>
+    </row>
+    <row r="649" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A649" s="8">
+        <v>44111</v>
+      </c>
+      <c r="B649" s="25"/>
+      <c r="C649" s="25"/>
+      <c r="D649" s="25"/>
+    </row>
+    <row r="650" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A650" s="8">
+        <v>44112</v>
+      </c>
+      <c r="B650" s="25"/>
+      <c r="C650" s="25"/>
+      <c r="D650" s="25"/>
+    </row>
+    <row r="651" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A651" s="8">
+        <v>44113</v>
+      </c>
+      <c r="B651" s="25"/>
+      <c r="C651" s="25"/>
+      <c r="D651" s="25"/>
+    </row>
+    <row r="652" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A652" s="8">
+        <v>44114</v>
+      </c>
+      <c r="B652" s="25"/>
+      <c r="C652" s="25"/>
+      <c r="D652" s="25"/>
+    </row>
+    <row r="653" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A653" s="8">
+        <v>44115</v>
+      </c>
+      <c r="B653" s="25"/>
+      <c r="C653" s="25"/>
+      <c r="D653" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -10410,7 +10466,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-04-2020 02-09-29
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1245" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A9C0D8ED-0392-426A-A9AA-5C9A6111CF84}"/>
+  <xr:revisionPtr revIDLastSave="1258" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE584541-2E57-41F7-8D5F-EF0D0A951267}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1320,8 +1320,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H653" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H653" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H674" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H674" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1652,11 +1652,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R653"/>
+  <dimension ref="A1:R674"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A644" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A659" sqref="A659"/>
+      <pane ySplit="3" topLeftCell="A662" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A677" sqref="A677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10444,6 +10444,201 @@
       <c r="C653" s="25"/>
       <c r="D653" s="25"/>
     </row>
+    <row r="654" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A654" s="8">
+        <v>44116</v>
+      </c>
+      <c r="B654" s="25"/>
+      <c r="C654" s="25"/>
+      <c r="D654" s="25"/>
+    </row>
+    <row r="655" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A655" s="8">
+        <v>44117</v>
+      </c>
+      <c r="B655" s="25"/>
+      <c r="C655" s="25"/>
+      <c r="D655" s="25"/>
+    </row>
+    <row r="656" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A656" s="8">
+        <v>44118</v>
+      </c>
+      <c r="B656" s="25"/>
+      <c r="C656" s="25"/>
+      <c r="D656" s="25"/>
+    </row>
+    <row r="657" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A657" s="8">
+        <v>44119</v>
+      </c>
+      <c r="B657" s="25"/>
+      <c r="C657" s="25"/>
+      <c r="D657" s="25"/>
+    </row>
+    <row r="658" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A658" s="8">
+        <v>44120</v>
+      </c>
+      <c r="B658" s="25"/>
+      <c r="C658" s="25"/>
+      <c r="D658" s="25"/>
+    </row>
+    <row r="659" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A659" s="8">
+        <v>44121</v>
+      </c>
+      <c r="B659" s="25"/>
+      <c r="C659" s="25"/>
+      <c r="D659" s="25"/>
+      <c r="E659" s="21">
+        <v>2.46</v>
+      </c>
+      <c r="F659" s="21">
+        <v>2.38</v>
+      </c>
+      <c r="G659" s="21">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="660" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A660" s="8">
+        <v>44122</v>
+      </c>
+      <c r="B660" s="25"/>
+      <c r="C660" s="25"/>
+      <c r="D660" s="25"/>
+    </row>
+    <row r="661" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A661" s="8">
+        <v>44123</v>
+      </c>
+      <c r="B661" s="25"/>
+      <c r="C661" s="25"/>
+      <c r="D661" s="25"/>
+    </row>
+    <row r="662" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A662" s="8">
+        <v>44124</v>
+      </c>
+      <c r="B662" s="25"/>
+      <c r="C662" s="25"/>
+      <c r="D662" s="25"/>
+    </row>
+    <row r="663" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A663" s="8">
+        <v>44125</v>
+      </c>
+      <c r="B663" s="25"/>
+      <c r="C663" s="25"/>
+      <c r="D663" s="25"/>
+    </row>
+    <row r="664" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A664" s="8">
+        <v>44126</v>
+      </c>
+      <c r="B664" s="25"/>
+      <c r="C664" s="25"/>
+      <c r="D664" s="25"/>
+    </row>
+    <row r="665" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A665" s="8">
+        <v>44127</v>
+      </c>
+      <c r="B665" s="25"/>
+      <c r="C665" s="25"/>
+      <c r="D665" s="25"/>
+    </row>
+    <row r="666" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A666" s="8">
+        <v>44128</v>
+      </c>
+      <c r="B666" s="25"/>
+      <c r="C666" s="25"/>
+      <c r="D666" s="25"/>
+      <c r="E666" s="21">
+        <v>2.46</v>
+      </c>
+      <c r="F666" s="21">
+        <v>2.38</v>
+      </c>
+      <c r="G666" s="21">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="667" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A667" s="8">
+        <v>44129</v>
+      </c>
+      <c r="B667" s="25"/>
+      <c r="C667" s="25"/>
+      <c r="D667" s="25"/>
+    </row>
+    <row r="668" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A668" s="8">
+        <v>44130</v>
+      </c>
+      <c r="B668" s="25"/>
+      <c r="C668" s="25"/>
+      <c r="D668" s="25"/>
+    </row>
+    <row r="669" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A669" s="8">
+        <v>44131</v>
+      </c>
+      <c r="B669" s="25"/>
+      <c r="C669" s="25"/>
+      <c r="D669" s="25"/>
+    </row>
+    <row r="670" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A670" s="8">
+        <v>44132</v>
+      </c>
+      <c r="B670" s="25"/>
+      <c r="C670" s="25"/>
+      <c r="D670" s="25"/>
+    </row>
+    <row r="671" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A671" s="8">
+        <v>44133</v>
+      </c>
+      <c r="B671" s="25"/>
+      <c r="C671" s="25"/>
+      <c r="D671" s="25"/>
+    </row>
+    <row r="672" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A672" s="8">
+        <v>44134</v>
+      </c>
+      <c r="B672" s="25"/>
+      <c r="C672" s="25"/>
+      <c r="D672" s="25"/>
+    </row>
+    <row r="673" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A673" s="8">
+        <v>44135</v>
+      </c>
+      <c r="B673" s="25"/>
+      <c r="C673" s="25"/>
+      <c r="D673" s="25"/>
+      <c r="E673">
+        <v>2.42</v>
+      </c>
+      <c r="F673">
+        <v>2.37</v>
+      </c>
+      <c r="G673">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="674" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A674" s="8">
+        <v>44136</v>
+      </c>
+      <c r="B674" s="25"/>
+      <c r="C674" s="25"/>
+      <c r="D674" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -10466,7 +10661,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-08-2020 13-53-11
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1258" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE584541-2E57-41F7-8D5F-EF0D0A951267}"/>
+  <xr:revisionPtr revIDLastSave="1266" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8BA6CCCF-6C43-44F0-B9DF-826863657E24}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="102">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1320,8 +1320,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H674" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H674" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H681" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H681" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1337,8 +1337,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R48" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R48" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R49" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R49" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
@@ -1652,11 +1652,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R674"/>
+  <dimension ref="A1:R681"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A662" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A677" sqref="A677"/>
+      <pane ySplit="3" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A688" sqref="A688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3393,7 +3393,7 @@
         <v>523101.42599999998</v>
       </c>
       <c r="P45" s="2">
-        <v>367.61</v>
+        <v>376.09</v>
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="21"/>
@@ -3487,17 +3487,21 @@
         <v>26</v>
       </c>
       <c r="L48" s="9" t="str">
-        <f t="shared" ref="L48" si="3">+K48&amp;", "&amp;J48</f>
+        <f t="shared" ref="L48:L49" si="3">+K48&amp;", "&amp;J48</f>
         <v>Septiembre, 2020</v>
       </c>
       <c r="M48" s="21"/>
       <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
+      <c r="O48" s="2">
+        <v>652482.00699999998</v>
+      </c>
+      <c r="P48" s="2">
+        <v>367.09</v>
+      </c>
       <c r="Q48" s="21"/>
       <c r="R48" s="21"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>43511</v>
       </c>
@@ -3507,8 +3511,21 @@
       <c r="E49" s="21"/>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J49" s="9">
+        <v>2020</v>
+      </c>
+      <c r="K49" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L49" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>Octubre, 2020</v>
+      </c>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>43512</v>
       </c>
@@ -3525,7 +3542,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>43513</v>
       </c>
@@ -3536,7 +3553,7 @@
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>43514</v>
       </c>
@@ -3547,7 +3564,7 @@
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>43515</v>
       </c>
@@ -3558,7 +3575,7 @@
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>43516</v>
       </c>
@@ -3569,7 +3586,7 @@
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>43517</v>
       </c>
@@ -3580,7 +3597,7 @@
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>43518</v>
       </c>
@@ -3591,7 +3608,7 @@
       <c r="F56" s="21"/>
       <c r="G56" s="21"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>43519</v>
       </c>
@@ -3608,7 +3625,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>43520</v>
       </c>
@@ -3619,7 +3636,7 @@
       <c r="F58" s="21"/>
       <c r="G58" s="21"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>43521</v>
       </c>
@@ -3630,7 +3647,7 @@
       <c r="F59" s="21"/>
       <c r="G59" s="21"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>43522</v>
       </c>
@@ -3641,7 +3658,7 @@
       <c r="F60" s="21"/>
       <c r="G60" s="21"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>43523</v>
       </c>
@@ -3652,7 +3669,7 @@
       <c r="F61" s="21"/>
       <c r="G61" s="21"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>43524</v>
       </c>
@@ -3667,7 +3684,7 @@
       <c r="F62" s="21"/>
       <c r="G62" s="21"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>43525</v>
       </c>
@@ -3678,7 +3695,7 @@
       <c r="F63" s="21"/>
       <c r="G63" s="21"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>43526</v>
       </c>
@@ -10638,6 +10655,62 @@
       <c r="B674" s="25"/>
       <c r="C674" s="25"/>
       <c r="D674" s="25"/>
+    </row>
+    <row r="675" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A675" s="8">
+        <v>44137</v>
+      </c>
+      <c r="B675" s="25"/>
+      <c r="C675" s="25"/>
+      <c r="D675" s="25"/>
+    </row>
+    <row r="676" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A676" s="8">
+        <v>44138</v>
+      </c>
+      <c r="B676" s="25"/>
+      <c r="C676" s="25"/>
+      <c r="D676" s="25"/>
+    </row>
+    <row r="677" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A677" s="8">
+        <v>44139</v>
+      </c>
+      <c r="B677" s="25"/>
+      <c r="C677" s="25"/>
+      <c r="D677" s="25"/>
+    </row>
+    <row r="678" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A678" s="8">
+        <v>44140</v>
+      </c>
+      <c r="B678" s="25"/>
+      <c r="C678" s="25"/>
+      <c r="D678" s="25"/>
+    </row>
+    <row r="679" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A679" s="8">
+        <v>44141</v>
+      </c>
+      <c r="B679" s="25"/>
+      <c r="C679" s="25"/>
+      <c r="D679" s="25"/>
+    </row>
+    <row r="680" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A680" s="8">
+        <v>44142</v>
+      </c>
+      <c r="B680" s="25"/>
+      <c r="C680" s="25"/>
+      <c r="D680" s="25"/>
+    </row>
+    <row r="681" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A681" s="8">
+        <v>44143</v>
+      </c>
+      <c r="B681" s="25"/>
+      <c r="C681" s="25"/>
+      <c r="D681" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -10661,7 +10734,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-10-2020 22-39-01
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1266" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8BA6CCCF-6C43-44F0-B9DF-826863657E24}"/>
+  <xr:revisionPtr revIDLastSave="1271" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B51F616F-2682-4445-8198-376A47BAD7BC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1656,7 +1656,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A688" sqref="A688"/>
+      <selection pane="bottomLeft" activeCell="A684" sqref="A684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10703,6 +10703,15 @@
       <c r="B680" s="25"/>
       <c r="C680" s="25"/>
       <c r="D680" s="25"/>
+      <c r="E680" s="21">
+        <v>2.42</v>
+      </c>
+      <c r="F680" s="21">
+        <v>2.37</v>
+      </c>
+      <c r="G680" s="21">
+        <v>1.97</v>
+      </c>
     </row>
     <row r="681" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A681" s="8">
@@ -10734,7 +10743,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-14-2020 00-30-54
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1271" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B51F616F-2682-4445-8198-376A47BAD7BC}"/>
+  <xr:revisionPtr revIDLastSave="1274" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2AE17112-F7FF-42A4-8358-15C1580612C8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45" yWindow="135" windowWidth="17220" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -385,7 +385,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,14 +602,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -936,7 +928,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -983,9 +975,8 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1030,9 +1021,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="46" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="46">
     <cellStyle name="20% - Énfasis1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="28" builtinId="38" customBuiltin="1"/>
@@ -1064,7 +1054,6 @@
     <cellStyle name="Énfasis5" xfId="35" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis6" xfId="39" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="10" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="46" builtinId="8"/>
     <cellStyle name="Hipervínculo 2" xfId="44" xr:uid="{D1D5AC69-E029-407D-8457-44EF34D97FF6}"/>
     <cellStyle name="Incorrecto" xfId="8" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1320,8 +1309,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H681" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H681" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H688" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H688" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1652,11 +1641,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R681"/>
+  <dimension ref="A1:R688"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A684" sqref="A684"/>
+      <pane ySplit="3" topLeftCell="A676" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E681" sqref="E681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10721,6 +10710,62 @@
       <c r="C681" s="25"/>
       <c r="D681" s="25"/>
     </row>
+    <row r="682" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A682" s="8">
+        <v>44144</v>
+      </c>
+      <c r="B682" s="25"/>
+      <c r="C682" s="25"/>
+      <c r="D682" s="25"/>
+    </row>
+    <row r="683" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A683" s="8">
+        <v>44145</v>
+      </c>
+      <c r="B683" s="25"/>
+      <c r="C683" s="25"/>
+      <c r="D683" s="25"/>
+    </row>
+    <row r="684" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A684" s="8">
+        <v>44146</v>
+      </c>
+      <c r="B684" s="25"/>
+      <c r="C684" s="25"/>
+      <c r="D684" s="25"/>
+    </row>
+    <row r="685" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A685" s="8">
+        <v>44147</v>
+      </c>
+      <c r="B685" s="25"/>
+      <c r="C685" s="25"/>
+      <c r="D685" s="25"/>
+    </row>
+    <row r="686" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A686" s="8">
+        <v>44148</v>
+      </c>
+      <c r="B686" s="25"/>
+      <c r="C686" s="25"/>
+      <c r="D686" s="25"/>
+    </row>
+    <row r="687" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A687" s="8">
+        <v>44149</v>
+      </c>
+      <c r="B687" s="25"/>
+      <c r="C687" s="25"/>
+      <c r="D687" s="25"/>
+    </row>
+    <row r="688" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A688" s="8">
+        <v>44150</v>
+      </c>
+      <c r="B688" s="25"/>
+      <c r="C688" s="25"/>
+      <c r="D688" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -10740,10 +10785,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11491,7 +11536,7 @@
       <c r="E14" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="16" t="s">
         <v>101</v>
       </c>
       <c r="G14" s="12"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-14-2020 02-01-09
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1644,8 +1644,8 @@
   <dimension ref="A1:R688"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A676" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E681" sqref="E681"/>
+      <pane ySplit="3" topLeftCell="A680" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A695" sqref="A695"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10788,7 +10788,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-18-2020 02-00-40
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1274" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2AE17112-F7FF-42A4-8358-15C1580612C8}"/>
+  <xr:revisionPtr revIDLastSave="1275" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45A34D75-11CD-4B8D-97DB-543D75B3F6F3}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="135" windowWidth="17220" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1644,8 +1644,8 @@
   <dimension ref="A1:R688"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A680" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A695" sqref="A695"/>
+      <pane ySplit="3" topLeftCell="A677" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A692" sqref="A692"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3480,7 +3480,9 @@
         <v>Septiembre, 2020</v>
       </c>
       <c r="M48" s="21"/>
-      <c r="N48" s="2"/>
+      <c r="N48" s="2">
+        <v>51815.226999999999</v>
+      </c>
       <c r="O48" s="2">
         <v>652482.00699999998</v>
       </c>
@@ -10788,7 +10790,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-21-2020 00-31-28
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1644,8 +1644,8 @@
   <dimension ref="A1:R688"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A677" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A692" sqref="A692"/>
+      <pane ySplit="3" topLeftCell="A676" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A691" sqref="A691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10787,10 +10787,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-25-2020 00-31-26
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1275" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45A34D75-11CD-4B8D-97DB-543D75B3F6F3}"/>
+  <xr:revisionPtr revIDLastSave="1286" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A72986E-4E1E-42AD-B2CF-D5D3E331C32B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1309,8 +1309,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H688" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H688" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H702" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H702" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1641,11 +1641,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R688"/>
+  <dimension ref="A1:R702"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A676" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A691" sqref="A691"/>
+      <pane ySplit="3" topLeftCell="A687" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E702" sqref="E702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10627,8 +10627,12 @@
         <v>44135</v>
       </c>
       <c r="B673" s="25"/>
-      <c r="C673" s="25"/>
-      <c r="D673" s="25"/>
+      <c r="C673" s="25">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D673" s="23">
+        <v>1438.22</v>
+      </c>
       <c r="E673">
         <v>2.42</v>
       </c>
@@ -10759,6 +10763,15 @@
       <c r="B687" s="25"/>
       <c r="C687" s="25"/>
       <c r="D687" s="25"/>
+      <c r="E687">
+        <v>2.31</v>
+      </c>
+      <c r="F687">
+        <v>2.25</v>
+      </c>
+      <c r="G687">
+        <v>1.92</v>
+      </c>
     </row>
     <row r="688" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A688" s="8">
@@ -10767,6 +10780,127 @@
       <c r="B688" s="25"/>
       <c r="C688" s="25"/>
       <c r="D688" s="25"/>
+    </row>
+    <row r="689" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A689" s="8">
+        <v>44151</v>
+      </c>
+      <c r="B689" s="25"/>
+      <c r="C689" s="25"/>
+      <c r="D689" s="25"/>
+    </row>
+    <row r="690" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A690" s="8">
+        <v>44152</v>
+      </c>
+      <c r="B690" s="25"/>
+      <c r="C690" s="25"/>
+      <c r="D690" s="25"/>
+    </row>
+    <row r="691" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A691" s="8">
+        <v>44153</v>
+      </c>
+      <c r="B691" s="25"/>
+      <c r="C691" s="25"/>
+      <c r="D691" s="25"/>
+    </row>
+    <row r="692" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A692" s="8">
+        <v>44154</v>
+      </c>
+      <c r="B692" s="25"/>
+      <c r="C692" s="25"/>
+      <c r="D692" s="25"/>
+    </row>
+    <row r="693" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A693" s="8">
+        <v>44155</v>
+      </c>
+      <c r="B693" s="25"/>
+      <c r="C693" s="25"/>
+      <c r="D693" s="25"/>
+    </row>
+    <row r="694" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A694" s="8">
+        <v>44156</v>
+      </c>
+      <c r="B694" s="25"/>
+      <c r="C694" s="25"/>
+      <c r="D694" s="25"/>
+      <c r="E694" s="21">
+        <v>2.31</v>
+      </c>
+      <c r="F694" s="21">
+        <v>2.25</v>
+      </c>
+      <c r="G694" s="21">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="695" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A695" s="8">
+        <v>44157</v>
+      </c>
+      <c r="B695" s="25"/>
+      <c r="C695" s="25"/>
+      <c r="D695" s="25"/>
+    </row>
+    <row r="696" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A696" s="8">
+        <v>44158</v>
+      </c>
+      <c r="B696" s="25"/>
+      <c r="C696" s="25"/>
+      <c r="D696" s="25"/>
+    </row>
+    <row r="697" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A697" s="8">
+        <v>44159</v>
+      </c>
+      <c r="B697" s="25"/>
+      <c r="C697" s="25"/>
+      <c r="D697" s="25"/>
+    </row>
+    <row r="698" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A698" s="8">
+        <v>44160</v>
+      </c>
+      <c r="B698" s="25"/>
+      <c r="C698" s="25"/>
+      <c r="D698" s="25"/>
+    </row>
+    <row r="699" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A699" s="8">
+        <v>44161</v>
+      </c>
+      <c r="B699" s="25"/>
+      <c r="C699" s="25"/>
+      <c r="D699" s="25"/>
+    </row>
+    <row r="700" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A700" s="8">
+        <v>44162</v>
+      </c>
+      <c r="B700" s="25"/>
+      <c r="C700" s="25"/>
+      <c r="D700" s="25"/>
+    </row>
+    <row r="701" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A701" s="8">
+        <v>44163</v>
+      </c>
+      <c r="B701" s="25"/>
+      <c r="C701" s="25"/>
+      <c r="D701" s="25"/>
+    </row>
+    <row r="702" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A702" s="8">
+        <v>44164</v>
+      </c>
+      <c r="B702" s="25"/>
+      <c r="C702" s="25"/>
+      <c r="D702" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -10790,7 +10924,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-25-2020 02-01-04
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1286" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A72986E-4E1E-42AD-B2CF-D5D3E331C32B}"/>
+  <xr:revisionPtr revIDLastSave="1287" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FFACA9D6-CAFF-4D67-AF8F-57143861C00D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1644,8 +1644,8 @@
   <dimension ref="A1:R702"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A687" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E702" sqref="E702"/>
+      <pane ySplit="3" topLeftCell="A689" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G702" sqref="G702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3182,7 +3182,7 @@
         <v>Enero, 2020</v>
       </c>
       <c r="M40" s="24">
-        <v>339.56602505061431</v>
+        <v>339.61158109834963</v>
       </c>
       <c r="N40" s="2">
         <v>51503.478000000003</v>
@@ -3219,7 +3219,7 @@
         <v>Febrero, 2020</v>
       </c>
       <c r="M41" s="24">
-        <v>333.99133203105765</v>
+        <v>334.01742836097281</v>
       </c>
       <c r="N41" s="2">
         <v>54227.436999999991</v>
@@ -3256,7 +3256,7 @@
         <v>Marzo, 2020</v>
       </c>
       <c r="M42" s="24">
-        <v>366.43683999641081</v>
+        <v>366.38633514958934</v>
       </c>
       <c r="N42" s="2">
         <v>69413.402000000002</v>
@@ -3301,7 +3301,7 @@
         <v>Abril, 2020</v>
       </c>
       <c r="M43" s="24">
-        <v>217.92340191398858</v>
+        <v>245.00732997578669</v>
       </c>
       <c r="N43" s="2">
         <v>59005.919000000002</v>
@@ -3338,7 +3338,7 @@
         <v>Mayo, 2020</v>
       </c>
       <c r="M44" s="24">
-        <v>193.83678840082644</v>
+        <v>225.38759592718446</v>
       </c>
       <c r="N44" s="2">
         <v>44765.543999999994</v>
@@ -3374,7 +3374,9 @@
         <f t="shared" ref="L45" si="1">+K45&amp;", "&amp;J45</f>
         <v>Junio, 2020</v>
       </c>
-      <c r="M45" s="24"/>
+      <c r="M45" s="24">
+        <v>238.98816111041066</v>
+      </c>
       <c r="N45" s="2">
         <v>56461.284</v>
       </c>
@@ -3409,7 +3411,9 @@
         <f t="shared" ref="L46:L47" si="2">+K46&amp;", "&amp;J46</f>
         <v>Julio, 2020</v>
       </c>
-      <c r="M46" s="24"/>
+      <c r="M46" s="24">
+        <v>222.70585963798015</v>
+      </c>
       <c r="N46" s="2">
         <v>52641.306000000011</v>
       </c>
@@ -3444,7 +3448,9 @@
         <f t="shared" si="2"/>
         <v>Agosto, 2020</v>
       </c>
-      <c r="M47" s="24"/>
+      <c r="M47" s="24">
+        <v>240.42959604465955</v>
+      </c>
       <c r="N47" s="2">
         <v>50175.788</v>
       </c>
@@ -10924,7 +10930,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 11-28-2020 00-30-38
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1287" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FFACA9D6-CAFF-4D67-AF8F-57143861C00D}"/>
+  <xr:revisionPtr revIDLastSave="1290" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{90B3B6B8-5F27-4BAF-8EC0-1F18D75DE23A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1644,8 +1644,8 @@
   <dimension ref="A1:R702"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A689" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G702" sqref="G702"/>
+      <pane ySplit="3" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A705" sqref="A705"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3387,7 +3387,9 @@
         <v>376.09</v>
       </c>
       <c r="Q45" s="2"/>
-      <c r="R45" s="21"/>
+      <c r="R45" s="21">
+        <v>-4.5</v>
+      </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
@@ -10930,7 +10932,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-04-2020 22-30-35
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1292" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3B516BC8-3D1F-2544-8D0B-D6E4F57DABD6}"/>
+  <xr:revisionPtr revIDLastSave="1296" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6317D5D6-EBC6-9741-B46E-5DFD14B8A7B5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1644,8 +1644,8 @@
   <dimension ref="A1:R702"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A701" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F702" sqref="F702"/>
+      <pane ySplit="3" topLeftCell="A698" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C702" sqref="C702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10929,10 +10929,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.98828125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-12-2020 02-00-57
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1304" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E42625C7-D8C7-4A64-8C2E-64D038E7EE3C}"/>
+  <xr:revisionPtr revIDLastSave="1306" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{28101860-F039-4B97-A3F8-A6BE3AA7CF13}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1645,7 +1645,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A694" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C702" sqref="C702"/>
+      <selection pane="bottomLeft" activeCell="E702" sqref="E702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-16-2020 00-30-55
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1306" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{28101860-F039-4B97-A3F8-A6BE3AA7CF13}"/>
+  <xr:revisionPtr revIDLastSave="1308" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{754C5733-7498-4231-9ABF-E6DF9E3243FF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1644,7 +1644,7 @@
   <dimension ref="A1:R702"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A694" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E702" sqref="E702"/>
     </sheetView>
   </sheetViews>
@@ -10946,10 +10946,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-18-2020 22-31-03
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1308" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{754C5733-7498-4231-9ABF-E6DF9E3243FF}"/>
+  <xr:revisionPtr revIDLastSave="1310" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F0F808F-91B9-487C-B32C-DC3105E20D78}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1644,7 +1644,7 @@
   <dimension ref="A1:R702"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A688" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E702" sqref="E702"/>
     </sheetView>
   </sheetViews>
@@ -10949,7 +10949,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-19-2020 00-30-51
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1310" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F0F808F-91B9-487C-B32C-DC3105E20D78}"/>
+  <xr:revisionPtr revIDLastSave="1322" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5EE93B57-0D31-49CE-B25C-B3992DF64163}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1644,8 +1644,8 @@
   <dimension ref="A1:R702"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A688" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E702" sqref="E702"/>
+      <pane ySplit="3" topLeftCell="A693" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F702" sqref="F702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2721,7 +2721,7 @@
         <v>331.32889999999998</v>
       </c>
       <c r="N28" s="2">
-        <v>43482.339</v>
+        <v>43308.890000000007</v>
       </c>
       <c r="O28" s="2">
         <v>1111219.905</v>
@@ -2758,7 +2758,7 @@
         <v>328.63400000000001</v>
       </c>
       <c r="N29" s="2">
-        <v>52653.085999999996</v>
+        <v>51395.210000000006</v>
       </c>
       <c r="O29" s="2">
         <v>1038882.9299999999</v>
@@ -2795,7 +2795,7 @@
         <v>364.33889770244838</v>
       </c>
       <c r="N30" s="2">
-        <v>60651.198999999993</v>
+        <v>60634.097999999991</v>
       </c>
       <c r="O30" s="2">
         <v>1017322.97</v>
@@ -2834,7 +2834,7 @@
         <v>333.48007691186666</v>
       </c>
       <c r="N31" s="2">
-        <v>68424.034</v>
+        <v>68221.039000000004</v>
       </c>
       <c r="O31" s="2">
         <v>1160800.395</v>
@@ -2908,7 +2908,7 @@
         <v>343.69303369887035</v>
       </c>
       <c r="N33" s="2">
-        <v>56420.404000000002</v>
+        <v>86458.164999999994</v>
       </c>
       <c r="O33" s="2">
         <v>1161410.8489999999</v>
@@ -2951,7 +2951,7 @@
         <v>322.31220289308749</v>
       </c>
       <c r="N34" s="2">
-        <v>77405.130999999994</v>
+        <v>275466.90400000004</v>
       </c>
       <c r="O34" s="2">
         <v>1114362.077</v>
@@ -2988,7 +2988,7 @@
         <v>339.43098738157141</v>
       </c>
       <c r="N35" s="2">
-        <v>63098.324999999997</v>
+        <v>149332.53999999998</v>
       </c>
       <c r="O35" s="2">
         <v>1042562.5420000001</v>
@@ -3033,7 +3033,7 @@
         <v>334.79059757082905</v>
       </c>
       <c r="N36" s="2">
-        <v>61629.516000000003</v>
+        <v>214166.18599999999</v>
       </c>
       <c r="O36" s="2">
         <v>973233.25699999998</v>
@@ -3072,7 +3072,7 @@
         <v>357.60777156513046</v>
       </c>
       <c r="N37" s="2">
-        <v>63678.347000000002</v>
+        <v>223565.72999999995</v>
       </c>
       <c r="O37" s="2">
         <v>1168093.5159999998</v>
@@ -3185,7 +3185,7 @@
         <v>339.61158109834963</v>
       </c>
       <c r="N40" s="2">
-        <v>51503.478000000003</v>
+        <v>157509.23899999997</v>
       </c>
       <c r="O40" s="2">
         <v>913121.64900000009</v>
@@ -3222,7 +3222,7 @@
         <v>334.01742836097281</v>
       </c>
       <c r="N41" s="2">
-        <v>54227.436999999991</v>
+        <v>184085.48299999998</v>
       </c>
       <c r="O41" s="2">
         <v>750772.66500000004</v>
@@ -3259,7 +3259,7 @@
         <v>366.38633514958934</v>
       </c>
       <c r="N42" s="2">
-        <v>69413.402000000002</v>
+        <v>181206.992</v>
       </c>
       <c r="O42" s="2">
         <v>787744.87099999993</v>
@@ -3304,7 +3304,7 @@
         <v>245.00732997578669</v>
       </c>
       <c r="N43" s="2">
-        <v>59005.919000000002</v>
+        <v>89167.92</v>
       </c>
       <c r="O43" s="2">
         <v>533206.50500000012</v>
@@ -3341,7 +3341,7 @@
         <v>225.38759592718446</v>
       </c>
       <c r="N44" s="2">
-        <v>44765.543999999994</v>
+        <v>78383.502000000008</v>
       </c>
       <c r="O44" s="2">
         <v>493292.21799999999</v>
@@ -3378,7 +3378,7 @@
         <v>238.98816111041066</v>
       </c>
       <c r="N45" s="2">
-        <v>56461.284</v>
+        <v>107559.02799999998</v>
       </c>
       <c r="O45" s="2">
         <v>523101.42599999998</v>
@@ -3417,7 +3417,7 @@
         <v>222.70585963798015</v>
       </c>
       <c r="N46" s="2">
-        <v>52641.306000000011</v>
+        <v>91433.98000000001</v>
       </c>
       <c r="O46" s="2">
         <v>556779.63899999997</v>
@@ -3454,7 +3454,7 @@
         <v>240.42959604465955</v>
       </c>
       <c r="N47" s="2">
-        <v>50175.788</v>
+        <v>188088.80299999999</v>
       </c>
       <c r="O47" s="2">
         <v>584213.68099999998</v>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="M48" s="21"/>
       <c r="N48" s="2">
-        <v>51815.226999999999</v>
+        <v>226098.86000000007</v>
       </c>
       <c r="O48" s="2">
         <v>652482.00699999998</v>
@@ -3520,7 +3520,9 @@
         <f t="shared" si="3"/>
         <v>Octubre, 2020</v>
       </c>
-      <c r="N49" s="2"/>
+      <c r="N49" s="2">
+        <v>146935.70398999998</v>
+      </c>
       <c r="O49" s="2">
         <v>726934.16200000001</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-23-2020 00-30-42
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1322" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5EE93B57-0D31-49CE-B25C-B3992DF64163}"/>
+  <xr:revisionPtr revIDLastSave="1326" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ACA2D15F-A047-4B09-B264-EF4317AB10F0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1309,8 +1309,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H702" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H702" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H709" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H709" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1641,11 +1641,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R702"/>
+  <dimension ref="A1:R709"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A693" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F702" sqref="F702"/>
+      <pane ySplit="3" topLeftCell="A694" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A709" sqref="A709"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10929,6 +10929,66 @@
       <c r="C702" s="25"/>
       <c r="D702" s="25"/>
     </row>
+    <row r="703" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A703" s="8">
+        <v>44165</v>
+      </c>
+      <c r="B703" s="25"/>
+      <c r="C703" s="25">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D703" s="23">
+        <v>1442.77</v>
+      </c>
+    </row>
+    <row r="704" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A704" s="8">
+        <v>44166</v>
+      </c>
+      <c r="B704" s="25"/>
+      <c r="C704" s="25"/>
+      <c r="D704" s="25"/>
+    </row>
+    <row r="705" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A705" s="8">
+        <v>44167</v>
+      </c>
+      <c r="B705" s="25"/>
+      <c r="C705" s="25"/>
+      <c r="D705" s="25"/>
+    </row>
+    <row r="706" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A706" s="8">
+        <v>44168</v>
+      </c>
+      <c r="B706" s="25"/>
+      <c r="C706" s="25"/>
+      <c r="D706" s="25"/>
+    </row>
+    <row r="707" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A707" s="8">
+        <v>44169</v>
+      </c>
+      <c r="B707" s="25"/>
+      <c r="C707" s="25"/>
+      <c r="D707" s="25"/>
+    </row>
+    <row r="708" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A708" s="8">
+        <v>44170</v>
+      </c>
+      <c r="B708" s="25"/>
+      <c r="C708" s="25"/>
+      <c r="D708" s="25"/>
+    </row>
+    <row r="709" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A709" s="8">
+        <v>44171</v>
+      </c>
+      <c r="B709" s="25"/>
+      <c r="C709" s="25"/>
+      <c r="D709" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -10948,10 +11008,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-24-2020 20-31-07
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1326" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ACA2D15F-A047-4B09-B264-EF4317AB10F0}"/>
+  <xr:revisionPtr revIDLastSave="1328" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE51FB2A-24F4-4280-A75B-A074EF010CC1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1644,8 +1644,8 @@
   <dimension ref="A1:R709"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A694" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A709" sqref="A709"/>
+      <pane ySplit="3" topLeftCell="A696" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C709" sqref="C709"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11011,7 +11011,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-29-2020 22-30-57
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1328" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE51FB2A-24F4-4280-A75B-A074EF010CC1}"/>
+  <xr:revisionPtr revIDLastSave="1332" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2AD27EE-3077-4C5C-B00B-EE1F7FA0AC0E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1644,8 +1644,8 @@
   <dimension ref="A1:R709"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A696" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C709" sqref="C709"/>
+      <pane ySplit="3" topLeftCell="A697" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H709" sqref="H709"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,7 +3375,7 @@
         <v>Junio, 2020</v>
       </c>
       <c r="M45" s="24">
-        <v>238.98816111041066</v>
+        <v>239.10946995623192</v>
       </c>
       <c r="N45" s="2">
         <v>107559.02799999998</v>
@@ -3414,7 +3414,7 @@
         <v>Julio, 2020</v>
       </c>
       <c r="M46" s="24">
-        <v>222.70585963798015</v>
+        <v>223.13587473103388</v>
       </c>
       <c r="N46" s="2">
         <v>91433.98000000001</v>
@@ -3451,7 +3451,7 @@
         <v>Agosto, 2020</v>
       </c>
       <c r="M47" s="24">
-        <v>240.42959604465955</v>
+        <v>239.65563601447195</v>
       </c>
       <c r="N47" s="2">
         <v>188088.80299999999</v>
@@ -3487,7 +3487,9 @@
         <f t="shared" ref="L48:L49" si="3">+K48&amp;", "&amp;J48</f>
         <v>Septiembre, 2020</v>
       </c>
-      <c r="M48" s="21"/>
+      <c r="M48" s="24">
+        <v>260.08302350187762</v>
+      </c>
       <c r="N48" s="2">
         <v>226098.86000000007</v>
       </c>
@@ -3520,6 +3522,9 @@
         <f t="shared" si="3"/>
         <v>Octubre, 2020</v>
       </c>
+      <c r="M49" s="24">
+        <v>296.95084413583675</v>
+      </c>
       <c r="N49" s="2">
         <v>146935.70398999998</v>
       </c>
@@ -3556,6 +3561,7 @@
         <f t="shared" ref="L50" si="4">+K50&amp;", "&amp;J50</f>
         <v>Noviembre, 2020</v>
       </c>
+      <c r="M50" s="24"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
@@ -11011,7 +11017,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 12-31-2020 20-31-17
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1332" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2AD27EE-3077-4C5C-B00B-EE1F7FA0AC0E}"/>
+  <xr:revisionPtr revIDLastSave="1354" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CCDCBE00-F7D9-4355-B5B7-C960C9CDEFC9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>https://sen.hn/informe-estadistico-semanal-de-cchac/</t>
+  </si>
+  <si>
+    <t>https://www.energia.gob.pa/documentos/</t>
+  </si>
+  <si>
+    <t>https://www.energia.gob.pa/archivos/?mdocs-cat=mdocs-cat-9</t>
   </si>
 </sst>
 </file>
@@ -1309,8 +1315,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H709" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H709" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H734" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H734" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1641,11 +1647,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:R709"/>
+  <dimension ref="A1:R734"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A697" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H709" sqref="H709"/>
+      <pane ySplit="3" topLeftCell="A726" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D734" sqref="D734"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3499,7 +3505,9 @@
       <c r="P48" s="2">
         <v>367.09</v>
       </c>
-      <c r="Q48" s="21"/>
+      <c r="Q48" s="21">
+        <v>18.5</v>
+      </c>
       <c r="R48" s="21"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -10926,6 +10934,15 @@
       <c r="B701" s="25"/>
       <c r="C701" s="25"/>
       <c r="D701" s="25"/>
+      <c r="E701">
+        <v>2.34</v>
+      </c>
+      <c r="F701">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G701">
+        <v>2.0099999999999998</v>
+      </c>
     </row>
     <row r="702" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A702" s="8">
@@ -10955,7 +10972,7 @@
       <c r="C704" s="25"/>
       <c r="D704" s="25"/>
     </row>
-    <row r="705" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A705" s="8">
         <v>44167</v>
       </c>
@@ -10963,7 +10980,7 @@
       <c r="C705" s="25"/>
       <c r="D705" s="25"/>
     </row>
-    <row r="706" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A706" s="8">
         <v>44168</v>
       </c>
@@ -10971,7 +10988,7 @@
       <c r="C706" s="25"/>
       <c r="D706" s="25"/>
     </row>
-    <row r="707" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="707" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A707" s="8">
         <v>44169</v>
       </c>
@@ -10979,21 +10996,248 @@
       <c r="C707" s="25"/>
       <c r="D707" s="25"/>
     </row>
-    <row r="708" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="708" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A708" s="8">
         <v>44170</v>
       </c>
       <c r="B708" s="25"/>
       <c r="C708" s="25"/>
       <c r="D708" s="25"/>
-    </row>
-    <row r="709" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E708" s="21">
+        <v>2.34</v>
+      </c>
+      <c r="F708" s="21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G708" s="21">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="709" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A709" s="8">
         <v>44171</v>
       </c>
       <c r="B709" s="25"/>
       <c r="C709" s="25"/>
       <c r="D709" s="25"/>
+    </row>
+    <row r="710" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A710" s="8">
+        <v>44172</v>
+      </c>
+      <c r="B710" s="25"/>
+      <c r="C710" s="25"/>
+      <c r="D710" s="25"/>
+    </row>
+    <row r="711" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A711" s="8">
+        <v>44173</v>
+      </c>
+      <c r="B711" s="25"/>
+      <c r="C711" s="25"/>
+      <c r="D711" s="25"/>
+    </row>
+    <row r="712" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A712" s="8">
+        <v>44174</v>
+      </c>
+      <c r="B712" s="25"/>
+      <c r="C712" s="25"/>
+      <c r="D712" s="25"/>
+    </row>
+    <row r="713" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A713" s="8">
+        <v>44175</v>
+      </c>
+      <c r="B713" s="25"/>
+      <c r="C713" s="25"/>
+      <c r="D713" s="25"/>
+    </row>
+    <row r="714" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A714" s="8">
+        <v>44176</v>
+      </c>
+      <c r="B714" s="25"/>
+      <c r="C714" s="25"/>
+      <c r="D714" s="25"/>
+    </row>
+    <row r="715" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A715" s="8">
+        <v>44177</v>
+      </c>
+      <c r="B715" s="25"/>
+      <c r="C715" s="25"/>
+      <c r="D715" s="25"/>
+      <c r="E715">
+        <v>2.44</v>
+      </c>
+      <c r="F715">
+        <v>2.38</v>
+      </c>
+      <c r="G715">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="716" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A716" s="8">
+        <v>44178</v>
+      </c>
+      <c r="B716" s="25"/>
+      <c r="C716" s="25"/>
+      <c r="D716" s="25"/>
+    </row>
+    <row r="717" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A717" s="8">
+        <v>44179</v>
+      </c>
+      <c r="B717" s="25"/>
+      <c r="C717" s="25"/>
+      <c r="D717" s="25"/>
+    </row>
+    <row r="718" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A718" s="8">
+        <v>44180</v>
+      </c>
+      <c r="B718" s="25"/>
+      <c r="C718" s="25"/>
+      <c r="D718" s="25"/>
+    </row>
+    <row r="719" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A719" s="8">
+        <v>44181</v>
+      </c>
+      <c r="B719" s="25"/>
+      <c r="C719" s="25"/>
+      <c r="D719" s="25"/>
+    </row>
+    <row r="720" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A720" s="8">
+        <v>44182</v>
+      </c>
+      <c r="B720" s="25"/>
+      <c r="C720" s="25"/>
+      <c r="D720" s="25"/>
+    </row>
+    <row r="721" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A721" s="8">
+        <v>44183</v>
+      </c>
+      <c r="B721" s="25"/>
+      <c r="C721" s="25"/>
+      <c r="D721" s="25"/>
+    </row>
+    <row r="722" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A722" s="8">
+        <v>44184</v>
+      </c>
+      <c r="B722" s="25"/>
+      <c r="C722" s="25"/>
+      <c r="D722" s="25"/>
+      <c r="E722" s="21">
+        <v>2.44</v>
+      </c>
+      <c r="F722" s="21">
+        <v>2.38</v>
+      </c>
+      <c r="G722">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="723" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A723" s="8">
+        <v>44185</v>
+      </c>
+      <c r="B723" s="25"/>
+      <c r="C723" s="25"/>
+      <c r="D723" s="25"/>
+    </row>
+    <row r="724" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A724" s="8">
+        <v>44186</v>
+      </c>
+      <c r="B724" s="25"/>
+      <c r="C724" s="25"/>
+      <c r="D724" s="25"/>
+    </row>
+    <row r="725" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A725" s="8">
+        <v>44187</v>
+      </c>
+      <c r="B725" s="25"/>
+      <c r="C725" s="25"/>
+      <c r="D725" s="25"/>
+    </row>
+    <row r="726" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A726" s="8">
+        <v>44188</v>
+      </c>
+      <c r="B726" s="25"/>
+      <c r="C726" s="25"/>
+      <c r="D726" s="25"/>
+    </row>
+    <row r="727" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A727" s="8">
+        <v>44189</v>
+      </c>
+      <c r="B727" s="25"/>
+      <c r="C727" s="25"/>
+      <c r="D727" s="25"/>
+    </row>
+    <row r="728" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A728" s="8">
+        <v>44190</v>
+      </c>
+      <c r="B728" s="25"/>
+      <c r="C728" s="25"/>
+      <c r="D728" s="25"/>
+    </row>
+    <row r="729" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A729" s="8">
+        <v>44191</v>
+      </c>
+      <c r="B729" s="25"/>
+      <c r="C729" s="25"/>
+      <c r="D729" s="25"/>
+    </row>
+    <row r="730" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A730" s="8">
+        <v>44192</v>
+      </c>
+      <c r="B730" s="25"/>
+      <c r="C730" s="25"/>
+      <c r="D730" s="25"/>
+    </row>
+    <row r="731" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A731" s="8">
+        <v>44193</v>
+      </c>
+      <c r="B731" s="25"/>
+      <c r="C731" s="25"/>
+      <c r="D731" s="25"/>
+    </row>
+    <row r="732" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A732" s="8">
+        <v>44194</v>
+      </c>
+      <c r="B732" s="25"/>
+      <c r="C732" s="25"/>
+      <c r="D732" s="25"/>
+    </row>
+    <row r="733" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A733" s="8">
+        <v>44195</v>
+      </c>
+      <c r="B733" s="25"/>
+      <c r="C733" s="25"/>
+      <c r="D733" s="25"/>
+    </row>
+    <row r="734" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A734" s="8">
+        <v>44196</v>
+      </c>
+      <c r="B734" s="25"/>
+      <c r="C734" s="25"/>
+      <c r="D734" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -11014,10 +11258,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11784,10 +12028,18 @@
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="16"/>
+      <c r="C15" s="12">
+        <v>7</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>102</v>
+      </c>
       <c r="G15" s="12"/>
       <c r="H15" s="13"/>
       <c r="I15" s="12"/>
@@ -11804,10 +12056,18 @@
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="16"/>
+      <c r="C16" s="12">
+        <v>7</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>103</v>
+      </c>
       <c r="G16" s="12"/>
       <c r="H16" s="13"/>
       <c r="I16" s="12"/>
@@ -12984,12 +13244,14 @@
     <hyperlink ref="F6" r:id="rId23" xr:uid="{A63B55D0-3F47-4A34-8619-62920F88C6BD}"/>
     <hyperlink ref="F4:F5" r:id="rId24" display="http://www.energia.gob.pa/precios/?tag=255" xr:uid="{CC5C4EC3-A3ED-46B0-9857-4D54C9FB54E0}"/>
     <hyperlink ref="F14" r:id="rId25" xr:uid="{3987BD5B-4929-4737-915E-69B483BD1681}"/>
+    <hyperlink ref="F15" r:id="rId26" xr:uid="{01B53A43-B238-4058-8A26-7C758549C1CF}"/>
+    <hyperlink ref="F16" r:id="rId27" xr:uid="{8BFBE07F-D5BE-43FE-8735-438DA46BE249}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId26"/>
+  <legacyDrawing r:id="rId28"/>
   <tableParts count="1">
-    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 01-06-2021 00-30-56
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1354" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CCDCBE00-F7D9-4355-B5B7-C960C9CDEFC9}"/>
+  <xr:revisionPtr revIDLastSave="1356" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{534A9165-AD15-4584-80A0-79FBA546E2E8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1650,8 +1650,8 @@
   <dimension ref="A1:R734"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A726" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D734" sqref="D734"/>
+      <pane ySplit="3" topLeftCell="A724" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E734" sqref="E734"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11258,10 +11258,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-12-2021 20-30-58
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23711"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1376" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{36142012-1FF7-44CF-9AA8-28D466C602F7}"/>
+  <xr:revisionPtr revIDLastSave="1378" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D089A9F7-8958-41E7-AC70-2BE5D13B2C9C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1654,8 +1654,8 @@
   <dimension ref="A1:R734"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="H31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P40" sqref="P40"/>
+      <pane ySplit="3" topLeftCell="L47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -11939,7 +11939,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-15-2021 20-31-28
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23713"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1378" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D089A9F7-8958-41E7-AC70-2BE5D13B2C9C}"/>
+  <xr:revisionPtr revIDLastSave="1380" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C0FA98FB-AB4A-4F3B-B0CE-DD7BD6CA4F44}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1654,8 +1654,8 @@
   <dimension ref="A1:R734"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="L47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M50" sqref="M50"/>
+      <pane ySplit="3" topLeftCell="A717" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C734" sqref="C734"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-22-2021 22-31-01
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1394" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EE329F2A-B2FC-4FF1-9070-A24BAA0EF81D}"/>
+  <xr:revisionPtr revIDLastSave="1396" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B7805C8D-8C9E-464C-A384-31C54AE26BAF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1082,6 +1082,22 @@
   <dxfs count="17">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1209,22 +1225,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1335,18 +1335,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R52" totalsRowShown="0" headerRowDxfId="6" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R52" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R52" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8FC1825F-E2AC-4830-AA41-5B12F2C15972}" name="Índice Mensual de Actividad Económica "/>
-    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="2" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="1" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="0" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="3" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="2" dataCellStyle="Millares"/>
     <tableColumn id="8" xr3:uid="{1A570E63-F800-45DF-9E5A-B8961BEFE222}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{7E984A16-0976-4747-9D31-12709D8A9C2E}" name="Ingesos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1355,7 +1355,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="1">
   <autoFilter ref="A1:U23" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1378,7 +1378,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1654,7 +1654,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A736" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A751" sqref="A751"/>
+      <selection pane="bottomLeft" activeCell="F748" sqref="F748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11671,7 +11671,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-27-2021 00-30-48
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1396" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B7805C8D-8C9E-464C-A384-31C54AE26BAF}"/>
+  <xr:revisionPtr revIDLastSave="1417" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{404A48F5-56C8-42C4-A9A3-FAB9A68976A0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="105">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1081,6 +1081,56 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF5D7B9D"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1225,56 +1275,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF5D7B9D"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9E2F3"/>
@@ -1318,13 +1318,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H748" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H748" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H772" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A3:H772" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Banano" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Harina de Pescado" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Banano" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Harina de Pescado" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Gasolina Superior"/>
     <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular"/>
     <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel"/>
@@ -1335,18 +1335,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R52" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R52" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R53" totalsRowShown="0" headerRowDxfId="13" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R53" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="10">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8FC1825F-E2AC-4830-AA41-5B12F2C15972}" name="Índice Mensual de Actividad Económica "/>
-    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="4" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="3" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="2" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="9" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="8" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="7" dataCellStyle="Millares"/>
     <tableColumn id="8" xr3:uid="{1A570E63-F800-45DF-9E5A-B8961BEFE222}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{7E984A16-0976-4747-9D31-12709D8A9C2E}" name="Ingesos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1355,7 +1355,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="6">
   <autoFilter ref="A1:U23" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1378,7 +1378,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1650,11 +1650,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W748"/>
+  <dimension ref="A1:W772"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A736" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F748" sqref="F748"/>
+      <pane ySplit="3" topLeftCell="A758" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B771" sqref="B771"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3722,7 +3722,7 @@
         <v>Septiembre, 2020</v>
       </c>
       <c r="M48" s="24">
-        <v>260.08302350187762</v>
+        <v>260.31128588533551</v>
       </c>
       <c r="N48" s="2">
         <v>226098.86000000007</v>
@@ -3764,7 +3764,7 @@
         <v>Octubre, 2020</v>
       </c>
       <c r="M49" s="24">
-        <v>296.95084413583675</v>
+        <v>297.6383833861118</v>
       </c>
       <c r="N49" s="2">
         <v>146935.70398999998</v>
@@ -3807,7 +3807,9 @@
         <f t="shared" ref="L50" si="4">+K50&amp;", "&amp;J50</f>
         <v>Noviembre, 2020</v>
       </c>
-      <c r="M50" s="24"/>
+      <c r="M50" s="24">
+        <v>296.77843816013888</v>
+      </c>
       <c r="N50" s="2">
         <v>102213.84199999998</v>
       </c>
@@ -3886,6 +3888,19 @@
       <c r="E53" s="21"/>
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
+      <c r="J53" s="9">
+        <v>2022</v>
+      </c>
+      <c r="K53" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L53" s="9" t="str">
+        <f>+K53&amp;", "&amp;J53</f>
+        <v>Febrero, 2022</v>
+      </c>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
@@ -11553,7 +11568,7 @@
         <v>2.21</v>
       </c>
     </row>
-    <row r="737" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="737" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A737" s="8">
         <v>44199</v>
       </c>
@@ -11561,7 +11576,7 @@
       <c r="C737" s="25"/>
       <c r="D737" s="25"/>
     </row>
-    <row r="738" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="738" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A738" s="8">
         <v>44200</v>
       </c>
@@ -11569,7 +11584,7 @@
       <c r="C738" s="25"/>
       <c r="D738" s="25"/>
     </row>
-    <row r="739" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="739" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A739" s="8">
         <v>44201</v>
       </c>
@@ -11577,7 +11592,7 @@
       <c r="C739" s="25"/>
       <c r="D739" s="25"/>
     </row>
-    <row r="740" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A740" s="8">
         <v>44202</v>
       </c>
@@ -11585,7 +11600,7 @@
       <c r="C740" s="25"/>
       <c r="D740" s="25"/>
     </row>
-    <row r="741" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="741" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A741" s="8">
         <v>44203</v>
       </c>
@@ -11593,15 +11608,24 @@
       <c r="C741" s="25"/>
       <c r="D741" s="25"/>
     </row>
-    <row r="742" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="742" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A742" s="8">
         <v>44204</v>
       </c>
       <c r="B742" s="25"/>
       <c r="C742" s="25"/>
       <c r="D742" s="25"/>
-    </row>
-    <row r="743" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E742">
+        <v>2.62</v>
+      </c>
+      <c r="F742">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G742">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="743" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A743" s="8">
         <v>44205</v>
       </c>
@@ -11609,7 +11633,7 @@
       <c r="C743" s="25"/>
       <c r="D743" s="25"/>
     </row>
-    <row r="744" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="744" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A744" s="8">
         <v>44206</v>
       </c>
@@ -11617,7 +11641,7 @@
       <c r="C744" s="25"/>
       <c r="D744" s="25"/>
     </row>
-    <row r="745" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="745" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A745" s="8">
         <v>44207</v>
       </c>
@@ -11625,7 +11649,7 @@
       <c r="C745" s="25"/>
       <c r="D745" s="25"/>
     </row>
-    <row r="746" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="746" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A746" s="8">
         <v>44208</v>
       </c>
@@ -11633,7 +11657,7 @@
       <c r="C746" s="25"/>
       <c r="D746" s="25"/>
     </row>
-    <row r="747" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="747" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A747" s="8">
         <v>44209</v>
       </c>
@@ -11641,13 +11665,223 @@
       <c r="C747" s="25"/>
       <c r="D747" s="25"/>
     </row>
-    <row r="748" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="748" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A748" s="8">
         <v>44210</v>
       </c>
       <c r="B748" s="25"/>
       <c r="C748" s="25"/>
       <c r="D748" s="25"/>
+    </row>
+    <row r="749" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A749" s="8">
+        <v>44211</v>
+      </c>
+      <c r="B749" s="25"/>
+      <c r="C749" s="25"/>
+      <c r="D749" s="25"/>
+    </row>
+    <row r="750" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A750" s="8">
+        <v>44212</v>
+      </c>
+      <c r="B750" s="25"/>
+      <c r="C750" s="25"/>
+      <c r="D750" s="25"/>
+      <c r="E750" s="21">
+        <v>2.62</v>
+      </c>
+      <c r="F750" s="21">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G750" s="21">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="751" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A751" s="8">
+        <v>44213</v>
+      </c>
+      <c r="B751" s="25"/>
+      <c r="C751" s="25"/>
+      <c r="D751" s="25"/>
+    </row>
+    <row r="752" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A752" s="8">
+        <v>44214</v>
+      </c>
+      <c r="B752" s="25"/>
+      <c r="C752" s="25"/>
+      <c r="D752" s="25"/>
+    </row>
+    <row r="753" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A753" s="8">
+        <v>44215</v>
+      </c>
+      <c r="B753" s="25"/>
+      <c r="C753" s="25"/>
+      <c r="D753" s="25"/>
+    </row>
+    <row r="754" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A754" s="8">
+        <v>44216</v>
+      </c>
+      <c r="B754" s="25"/>
+      <c r="C754" s="25"/>
+      <c r="D754" s="25"/>
+    </row>
+    <row r="755" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A755" s="8">
+        <v>44217</v>
+      </c>
+      <c r="B755" s="25"/>
+      <c r="C755" s="25"/>
+      <c r="D755" s="25"/>
+    </row>
+    <row r="756" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A756" s="8">
+        <v>44218</v>
+      </c>
+      <c r="B756" s="25"/>
+      <c r="C756" s="25"/>
+      <c r="D756" s="25"/>
+    </row>
+    <row r="757" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A757" s="8">
+        <v>44219</v>
+      </c>
+      <c r="B757" s="25"/>
+      <c r="C757" s="25"/>
+      <c r="D757" s="25"/>
+      <c r="E757">
+        <v>2.7</v>
+      </c>
+      <c r="F757">
+        <v>2.64</v>
+      </c>
+      <c r="G757">
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="758" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A758" s="8">
+        <v>44220</v>
+      </c>
+      <c r="B758" s="25"/>
+      <c r="C758" s="25"/>
+      <c r="D758" s="25"/>
+    </row>
+    <row r="759" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A759" s="8">
+        <v>44221</v>
+      </c>
+      <c r="B759" s="25"/>
+      <c r="C759" s="25"/>
+      <c r="D759" s="25"/>
+    </row>
+    <row r="760" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A760" s="8">
+        <v>44222</v>
+      </c>
+      <c r="B760" s="25"/>
+      <c r="C760" s="25"/>
+      <c r="D760" s="25"/>
+    </row>
+    <row r="761" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A761" s="8">
+        <v>44223</v>
+      </c>
+      <c r="B761" s="25"/>
+      <c r="C761" s="25"/>
+      <c r="D761" s="25"/>
+    </row>
+    <row r="762" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A762" s="8">
+        <v>44224</v>
+      </c>
+      <c r="B762" s="25"/>
+      <c r="C762" s="25"/>
+      <c r="D762" s="25"/>
+    </row>
+    <row r="763" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A763" s="8">
+        <v>44225</v>
+      </c>
+      <c r="B763" s="25"/>
+      <c r="C763" s="25"/>
+      <c r="D763" s="25"/>
+    </row>
+    <row r="764" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A764" s="8">
+        <v>44226</v>
+      </c>
+      <c r="B764" s="25"/>
+      <c r="C764" s="25"/>
+      <c r="D764" s="25"/>
+    </row>
+    <row r="765" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A765" s="8">
+        <v>44227</v>
+      </c>
+      <c r="B765" s="25"/>
+      <c r="C765" s="25"/>
+      <c r="D765" s="25"/>
+    </row>
+    <row r="766" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A766" s="8">
+        <v>44228</v>
+      </c>
+      <c r="B766" s="25"/>
+      <c r="C766" s="25"/>
+      <c r="D766" s="25"/>
+    </row>
+    <row r="767" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A767" s="8">
+        <v>44229</v>
+      </c>
+      <c r="B767" s="25"/>
+      <c r="C767" s="25"/>
+      <c r="D767" s="25"/>
+    </row>
+    <row r="768" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A768" s="8">
+        <v>44230</v>
+      </c>
+      <c r="B768" s="25"/>
+      <c r="C768" s="25"/>
+      <c r="D768" s="25"/>
+    </row>
+    <row r="769" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A769" s="8">
+        <v>44231</v>
+      </c>
+      <c r="B769" s="25"/>
+      <c r="C769" s="25"/>
+      <c r="D769" s="25"/>
+    </row>
+    <row r="770" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A770" s="8">
+        <v>44232</v>
+      </c>
+      <c r="B770" s="25"/>
+      <c r="C770" s="25"/>
+      <c r="D770" s="25"/>
+    </row>
+    <row r="771" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A771" s="8">
+        <v>44233</v>
+      </c>
+      <c r="B771" s="25"/>
+      <c r="C771" s="25"/>
+      <c r="D771" s="25"/>
+    </row>
+    <row r="772" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A772" s="8">
+        <v>44234</v>
+      </c>
+      <c r="B772" s="25"/>
+      <c r="C772" s="25"/>
+      <c r="D772" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -11671,7 +11905,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 01-28-2021 22-31-01
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1417" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{404A48F5-56C8-42C4-A9A3-FAB9A68976A0}"/>
+  <xr:revisionPtr revIDLastSave="1419" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B4C3D94B-73E0-4C76-918F-D5340DF1DCD6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1081,56 +1081,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF5D7B9D"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1275,6 +1225,56 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF5D7B9D"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9E2F3"/>
@@ -1318,13 +1318,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H772" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H772" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A3:H772" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Banano" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Harina de Pescado" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{D5EAE7FD-5C02-42C1-9C84-A2EEC0E6B542}" name="Precio Banano" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{BB21C496-7E01-4835-902E-A9595CE4A9FC}" name="Precio Harina de Pescado" dataDxfId="9"/>
     <tableColumn id="6" xr3:uid="{1A412D0D-9DDD-4532-ADAC-BC90F0ABB038}" name="Combustible Gasolina Superior"/>
     <tableColumn id="7" xr3:uid="{6C9802FB-03D0-4F94-9942-ED195CC86D50}" name="Combustible Regular"/>
     <tableColumn id="8" xr3:uid="{EBFE959D-24EF-495E-9BE7-BDEC4C8061F8}" name="Combustible Diesel"/>
@@ -1335,18 +1335,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R53" totalsRowShown="0" headerRowDxfId="13" headerRowCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R53" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
   <autoFilter ref="J3:R53" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{B5014004-7BDF-4570-B6E7-9E9E456E9FA9}" name="Fecha" dataDxfId="5">
       <calculatedColumnFormula>+K4&amp;", "&amp;J4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8FC1825F-E2AC-4830-AA41-5B12F2C15972}" name="Índice Mensual de Actividad Económica "/>
-    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="9" dataCellStyle="Millares"/>
-    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="8" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="7" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{9450F662-71AF-4E06-9948-6070A2499352}" name="Valor FOB de las exportaciones de bienes" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{8DA19535-924B-4930-B2B7-A27C68A6BB9A}" name="Valor CIF de las importaciones de bienes" dataDxfId="3" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF46982F-65B8-4AB6-8F8C-0A8885FA66A5}" name="Índice Precios Bolsa de Valores de Panamá" dataDxfId="2" dataCellStyle="Millares"/>
     <tableColumn id="8" xr3:uid="{1A570E63-F800-45DF-9E5A-B8961BEFE222}" name="Tasa de desempleo abierto"/>
     <tableColumn id="9" xr3:uid="{7E984A16-0976-4747-9D31-12709D8A9C2E}" name="Ingesos - Egresos Remesas (Millones USD)"/>
   </tableColumns>
@@ -1355,7 +1355,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D1D3CDDC-AAEE-4879-BF46-5EAF54FB4896}" name="Table_17" displayName="Table_17" ref="A1:U23" headerRowDxfId="1">
   <autoFilter ref="A1:U23" xr:uid="{A4DDB744-8DEA-4F35-AEC9-FB17B2884A09}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{C1E7A7E7-7FD3-4FCB-A528-822BF1431468}" name="ID_Fuente"/>
@@ -1378,7 +1378,7 @@
     <tableColumn id="18" xr3:uid="{BE4CA536-69A1-4E09-B63A-D7282A251F01}" name="País"/>
     <tableColumn id="19" xr3:uid="{15A820D3-8670-4BFD-8BDE-2BD2A5BBCE28}" name="División Administrativa"/>
     <tableColumn id="20" xr3:uid="{19BD7B61-ED33-4BE3-B11A-D96B98260DC0}" name="Formato Descarga"/>
-    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{3F7DFEC3-567C-4830-8528-61B17B47D643}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1654,7 +1654,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A758" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B771" sqref="B771"/>
+      <selection pane="bottomLeft" activeCell="C772" sqref="C772"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11880,7 +11880,6 @@
         <v>44234</v>
       </c>
       <c r="B772" s="25"/>
-      <c r="C772" s="25"/>
       <c r="D772" s="25"/>
     </row>
   </sheetData>
@@ -11905,7 +11904,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 02-20-2021 00-30-28
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1436" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A4CED769-5A61-4F40-9100-B005061671CD}"/>
+  <xr:revisionPtr revIDLastSave="1440" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3D429AFB-02C9-4096-B288-15EFC947680F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>Combustible Gasolina Superior (USD/Galón)</t>
-  </si>
-  <si>
-    <t>http://www.energia.gob.pa/precios/?tag=255</t>
   </si>
   <si>
     <t>Precio en la capital (USD/galón). Combustible Gasolina Superior</t>
@@ -1319,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H779" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H779" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H800" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H800" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1651,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W779"/>
+  <dimension ref="A1:W800"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A765" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B779" sqref="B779"/>
+      <pane ySplit="3" topLeftCell="A789" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B800" sqref="B800"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12819,6 +12816,174 @@
         <v>2.38</v>
       </c>
     </row>
+    <row r="780" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A780" s="8">
+        <v>44242</v>
+      </c>
+      <c r="B780" s="25"/>
+      <c r="C780" s="25"/>
+      <c r="D780" s="25"/>
+    </row>
+    <row r="781" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A781" s="8">
+        <v>44243</v>
+      </c>
+      <c r="B781" s="25"/>
+      <c r="C781" s="25"/>
+      <c r="D781" s="25"/>
+    </row>
+    <row r="782" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A782" s="8">
+        <v>44244</v>
+      </c>
+      <c r="B782" s="25"/>
+      <c r="C782" s="25"/>
+      <c r="D782" s="25"/>
+    </row>
+    <row r="783" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A783" s="8">
+        <v>44245</v>
+      </c>
+      <c r="B783" s="25"/>
+      <c r="C783" s="25"/>
+      <c r="D783" s="25"/>
+    </row>
+    <row r="784" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A784" s="8">
+        <v>44246</v>
+      </c>
+      <c r="B784" s="25"/>
+      <c r="C784" s="25"/>
+      <c r="D784" s="25"/>
+    </row>
+    <row r="785" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A785" s="8">
+        <v>44247</v>
+      </c>
+      <c r="B785" s="25"/>
+      <c r="C785" s="25"/>
+      <c r="D785" s="25"/>
+    </row>
+    <row r="786" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A786" s="8">
+        <v>44248</v>
+      </c>
+      <c r="B786" s="25"/>
+      <c r="C786" s="25"/>
+      <c r="D786" s="25"/>
+    </row>
+    <row r="787" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A787" s="8">
+        <v>44249</v>
+      </c>
+      <c r="B787" s="25"/>
+      <c r="C787" s="25"/>
+      <c r="D787" s="25"/>
+    </row>
+    <row r="788" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A788" s="8">
+        <v>44250</v>
+      </c>
+      <c r="B788" s="25"/>
+      <c r="C788" s="25"/>
+      <c r="D788" s="25"/>
+    </row>
+    <row r="789" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A789" s="8">
+        <v>44251</v>
+      </c>
+      <c r="B789" s="25"/>
+      <c r="C789" s="25"/>
+      <c r="D789" s="25"/>
+    </row>
+    <row r="790" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A790" s="8">
+        <v>44252</v>
+      </c>
+      <c r="B790" s="25"/>
+      <c r="C790" s="25"/>
+      <c r="D790" s="25"/>
+    </row>
+    <row r="791" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A791" s="8">
+        <v>44253</v>
+      </c>
+      <c r="B791" s="25"/>
+      <c r="C791" s="25"/>
+      <c r="D791" s="25"/>
+    </row>
+    <row r="792" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A792" s="8">
+        <v>44254</v>
+      </c>
+      <c r="B792" s="25"/>
+      <c r="C792" s="25"/>
+      <c r="D792" s="25"/>
+    </row>
+    <row r="793" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A793" s="8">
+        <v>44255</v>
+      </c>
+      <c r="B793" s="25"/>
+      <c r="C793" s="25"/>
+      <c r="D793" s="25"/>
+    </row>
+    <row r="794" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A794" s="8">
+        <v>44256</v>
+      </c>
+      <c r="B794" s="25"/>
+      <c r="C794" s="25"/>
+      <c r="D794" s="25"/>
+    </row>
+    <row r="795" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A795" s="8">
+        <v>44257</v>
+      </c>
+      <c r="B795" s="25"/>
+      <c r="C795" s="25"/>
+      <c r="D795" s="25"/>
+    </row>
+    <row r="796" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A796" s="8">
+        <v>44258</v>
+      </c>
+      <c r="B796" s="25"/>
+      <c r="C796" s="25"/>
+      <c r="D796" s="25"/>
+    </row>
+    <row r="797" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A797" s="8">
+        <v>44259</v>
+      </c>
+      <c r="B797" s="25"/>
+      <c r="C797" s="25"/>
+      <c r="D797" s="25"/>
+    </row>
+    <row r="798" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A798" s="8">
+        <v>44260</v>
+      </c>
+      <c r="B798" s="25"/>
+      <c r="C798" s="25"/>
+      <c r="D798" s="25"/>
+    </row>
+    <row r="799" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A799" s="8">
+        <v>44261</v>
+      </c>
+      <c r="B799" s="25"/>
+      <c r="C799" s="25"/>
+      <c r="D799" s="25"/>
+    </row>
+    <row r="800" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A800" s="8">
+        <v>44262</v>
+      </c>
+      <c r="B800" s="25"/>
+      <c r="C800" s="25"/>
+      <c r="D800" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -12841,7 +13006,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13067,19 +13232,19 @@
         <v>69</v>
       </c>
       <c r="F4" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="13" t="s">
         <v>71</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>72</v>
       </c>
       <c r="I4" s="12" t="s">
         <v>59</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="12"/>
@@ -13101,10 +13266,10 @@
         <v>62</v>
       </c>
       <c r="T4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="U4" s="15" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13121,22 +13286,22 @@
         <v>55</v>
       </c>
       <c r="E5" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>77</v>
-      </c>
       <c r="H5" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>59</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="12"/>
@@ -13158,10 +13323,10 @@
         <v>62</v>
       </c>
       <c r="T5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="U5" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="U5" s="15" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13178,22 +13343,22 @@
         <v>55</v>
       </c>
       <c r="E6" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>79</v>
-      </c>
       <c r="H6" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>59</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="12"/>
@@ -13215,10 +13380,10 @@
         <v>62</v>
       </c>
       <c r="T6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="U6" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="U6" s="15" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13226,7 +13391,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="12">
         <v>7</v>
@@ -13235,22 +13400,22 @@
         <v>55</v>
       </c>
       <c r="E7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="G7" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="H7" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>84</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>59</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="12"/>
@@ -13272,7 +13437,7 @@
         <v>62</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U7" s="15"/>
     </row>
@@ -13281,7 +13446,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="12">
         <v>7</v>
@@ -13293,19 +13458,19 @@
         <v>13</v>
       </c>
       <c r="F8" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>88</v>
-      </c>
       <c r="H8" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>59</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="12"/>
@@ -13327,7 +13492,7 @@
         <v>62</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U8" s="15"/>
     </row>
@@ -13336,7 +13501,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="12">
         <v>7</v>
@@ -13348,19 +13513,19 @@
         <v>14</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>59</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="12"/>
@@ -13382,7 +13547,7 @@
         <v>62</v>
       </c>
       <c r="T9" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U9" s="15"/>
     </row>
@@ -13391,7 +13556,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="12">
         <v>7</v>
@@ -13403,19 +13568,19 @@
         <v>15</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>59</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="12"/>
@@ -13437,7 +13602,7 @@
         <v>62</v>
       </c>
       <c r="T10" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U10" s="15"/>
     </row>
@@ -13446,7 +13611,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="12">
         <v>7</v>
@@ -13458,19 +13623,19 @@
         <v>16</v>
       </c>
       <c r="F11" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="H11" s="13" t="s">
         <v>92</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>93</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>59</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="12" t="s">
@@ -13494,10 +13659,10 @@
         <v>62</v>
       </c>
       <c r="T11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="U11" s="15" t="s">
         <v>74</v>
-      </c>
-      <c r="U11" s="15" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13505,7 +13670,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="12">
         <v>7</v>
@@ -13514,22 +13679,22 @@
         <v>55</v>
       </c>
       <c r="E12" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="H12" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>98</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>59</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="12"/>
@@ -13551,10 +13716,10 @@
         <v>62</v>
       </c>
       <c r="T12" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="U12" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="U12" s="15" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13580,18 +13745,10 @@
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="12">
-        <v>7</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>102</v>
-      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="13"/>
       <c r="I14" s="12"/>
@@ -13608,18 +13765,10 @@
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="12">
-        <v>7</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>103</v>
-      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="13"/>
       <c r="I15" s="12"/>
@@ -13636,18 +13785,10 @@
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="12">
-        <v>7</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>104</v>
-      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="13"/>
       <c r="I16" s="12"/>
@@ -14821,17 +14962,15 @@
     <hyperlink ref="H12" r:id="rId20" xr:uid="{A2CCE213-E64E-4D79-A444-2B2B51E63D8A}"/>
     <hyperlink ref="F11" r:id="rId21" xr:uid="{BAA932D0-528E-473F-B41D-ACBC3F9E9EC1}"/>
     <hyperlink ref="H10" r:id="rId22" display="cie_inec@contraloria.gob.pa" xr:uid="{89F510B2-5C68-4D03-A1F1-EFFB3447A280}"/>
-    <hyperlink ref="F6" r:id="rId23" xr:uid="{A63B55D0-3F47-4A34-8619-62920F88C6BD}"/>
-    <hyperlink ref="F4:F5" r:id="rId24" display="http://www.energia.gob.pa/precios/?tag=255" xr:uid="{CC5C4EC3-A3ED-46B0-9857-4D54C9FB54E0}"/>
-    <hyperlink ref="F14" r:id="rId25" xr:uid="{3987BD5B-4929-4737-915E-69B483BD1681}"/>
-    <hyperlink ref="F15" r:id="rId26" xr:uid="{01B53A43-B238-4058-8A26-7C758549C1CF}"/>
-    <hyperlink ref="F16" r:id="rId27" xr:uid="{8BFBE07F-D5BE-43FE-8735-438DA46BE249}"/>
+    <hyperlink ref="F4" r:id="rId23" xr:uid="{61A2A2A2-9845-4809-98B5-9C141FC78053}"/>
+    <hyperlink ref="F5" r:id="rId24" xr:uid="{0CA49FFA-4006-4994-A52D-23AD67D24C26}"/>
+    <hyperlink ref="F6" r:id="rId25" xr:uid="{0D73098C-4410-497F-8CC5-D2401A5DE46C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId28"/>
+  <legacyDrawing r:id="rId26"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId27"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update automatico via Actualizar 03-02-2021 22-31-11
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1447" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6FDAC1E0-EA6B-4082-8EDA-BAFD5B331F3F}"/>
+  <xr:revisionPtr revIDLastSave="1459" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8BA57ED5-E02D-4ECD-84BE-8B7A68F98013}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1333,8 +1333,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R53" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R53" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R54" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R54" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
@@ -1651,7 +1651,7 @@
   <dimension ref="A1:W807"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A797" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A792" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B807" sqref="B807"/>
     </sheetView>
   </sheetViews>
@@ -3744,7 +3744,9 @@
       <c r="Q48" s="21">
         <v>18.5</v>
       </c>
-      <c r="R48" s="21"/>
+      <c r="R48" s="21">
+        <v>-19.100000000000001</v>
+      </c>
       <c r="S48" s="21"/>
       <c r="T48" s="21"/>
       <c r="U48" s="21"/>
@@ -3906,7 +3908,9 @@
       <c r="M52" s="21"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
+      <c r="P52" s="2">
+        <v>362.07</v>
+      </c>
       <c r="Q52" s="21"/>
       <c r="R52" s="21"/>
       <c r="S52" s="21"/>
@@ -3928,14 +3932,14 @@
       <c r="H53" s="21"/>
       <c r="I53" s="21"/>
       <c r="J53" s="9">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="K53" s="9" t="s">
         <v>19</v>
       </c>
       <c r="L53" s="9" t="str">
         <f>+K53&amp;", "&amp;J53</f>
-        <v>Febrero, 2022</v>
+        <v>Febrero, 2021</v>
       </c>
       <c r="M53" s="21"/>
       <c r="N53" s="2"/>
@@ -3961,13 +3965,20 @@
       <c r="G54" s="21"/>
       <c r="H54" s="21"/>
       <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="21"/>
+      <c r="J54" s="9">
+        <v>2021</v>
+      </c>
+      <c r="K54" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L54" s="9" t="str">
+        <f t="shared" ref="L54" si="6">+K54&amp;", "&amp;J54</f>
+        <v>Marzo, 2021</v>
+      </c>
       <c r="M54" s="21"/>
-      <c r="N54" s="21"/>
-      <c r="O54" s="21"/>
-      <c r="P54" s="21"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
       <c r="Q54" s="21"/>
       <c r="R54" s="21"/>
       <c r="S54" s="21"/>
@@ -13064,7 +13075,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-13-2021 00-30-38
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1464" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{446D474D-9FEB-4338-B9DB-DD035DBCEC22}"/>
+  <xr:revisionPtr revIDLastSave="1466" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{76E1DD32-E7A3-4D66-B204-5C7FFD1B3F53}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H807" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H807" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H814" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H814" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1333,8 +1333,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R54" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R54" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R55" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R55" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W807"/>
+  <dimension ref="A1:W814"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A792" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B807" sqref="B807"/>
+      <pane ySplit="3" topLeftCell="A799" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C814" sqref="C814"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3999,13 +3999,20 @@
       <c r="G55" s="21"/>
       <c r="H55" s="21"/>
       <c r="I55" s="21"/>
-      <c r="J55" s="21"/>
-      <c r="K55" s="21"/>
-      <c r="L55" s="21"/>
+      <c r="J55" s="9">
+        <v>2021</v>
+      </c>
+      <c r="K55" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L55" s="9" t="str">
+        <f>+K55&amp;", "&amp;J55</f>
+        <v>Abril, 2021</v>
+      </c>
       <c r="M55" s="21"/>
-      <c r="N55" s="21"/>
-      <c r="O55" s="21"/>
-      <c r="P55" s="21"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
       <c r="Q55" s="21"/>
       <c r="R55" s="21"/>
       <c r="S55" s="21"/>
@@ -13057,6 +13064,62 @@
       <c r="C807" s="25"/>
       <c r="D807" s="25"/>
     </row>
+    <row r="808" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A808" s="8">
+        <v>44270</v>
+      </c>
+      <c r="B808" s="25"/>
+      <c r="C808" s="25"/>
+      <c r="D808" s="25"/>
+    </row>
+    <row r="809" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A809" s="8">
+        <v>44271</v>
+      </c>
+      <c r="B809" s="25"/>
+      <c r="C809" s="25"/>
+      <c r="D809" s="25"/>
+    </row>
+    <row r="810" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A810" s="8">
+        <v>44272</v>
+      </c>
+      <c r="B810" s="25"/>
+      <c r="C810" s="25"/>
+      <c r="D810" s="25"/>
+    </row>
+    <row r="811" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A811" s="8">
+        <v>44273</v>
+      </c>
+      <c r="B811" s="25"/>
+      <c r="C811" s="25"/>
+      <c r="D811" s="25"/>
+    </row>
+    <row r="812" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A812" s="8">
+        <v>44274</v>
+      </c>
+      <c r="B812" s="25"/>
+      <c r="C812" s="25"/>
+      <c r="D812" s="25"/>
+    </row>
+    <row r="813" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A813" s="8">
+        <v>44275</v>
+      </c>
+      <c r="B813" s="25"/>
+      <c r="C813" s="25"/>
+      <c r="D813" s="25"/>
+    </row>
+    <row r="814" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A814" s="8">
+        <v>44276</v>
+      </c>
+      <c r="B814" s="25"/>
+      <c r="C814" s="25"/>
+      <c r="D814" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -13079,7 +13142,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-17-2021 02-01-22
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1466" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{76E1DD32-E7A3-4D66-B204-5C7FFD1B3F53}"/>
+  <xr:revisionPtr revIDLastSave="1468" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B8E86356-6497-4FF5-98F0-218679B1A515}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1652,7 +1652,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A799" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C814" sqref="C814"/>
+      <selection pane="bottomLeft" activeCell="B814" sqref="B814"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13142,7 +13142,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-19-2021 20-30-45
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1468" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B8E86356-6497-4FF5-98F0-218679B1A515}"/>
+  <xr:revisionPtr revIDLastSave="1470" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2B763E6E-D394-4B85-881A-0D5C4AF2758B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1650,9 +1650,9 @@
   </sheetPr>
   <dimension ref="A1:W814"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A799" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B814" sqref="B814"/>
+      <selection pane="bottomLeft" activeCell="B810" sqref="B810"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13138,11 +13138,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB840748-361D-4458-B100-AAECA785CA65}">
   <dimension ref="A1:Y959"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-20-2021 02-01-04
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1470" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2B763E6E-D394-4B85-881A-0D5C4AF2758B}"/>
+  <xr:revisionPtr revIDLastSave="1472" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5650822A-AB74-4D3B-8305-08DBDA90336A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1650,9 +1650,9 @@
   </sheetPr>
   <dimension ref="A1:W814"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A799" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B810" sqref="B810"/>
+      <selection pane="bottomLeft" activeCell="B814" sqref="B814"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3906,8 +3906,12 @@
         <v>Enero, 2021</v>
       </c>
       <c r="M52" s="21"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
+      <c r="N52" s="2">
+        <v>241506.179</v>
+      </c>
+      <c r="O52" s="2">
+        <v>672024</v>
+      </c>
       <c r="P52" s="2">
         <v>362.07</v>
       </c>
@@ -13138,11 +13142,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB840748-361D-4458-B100-AAECA785CA65}">
   <dimension ref="A1:Y959"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-23-2021 22-30-56
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1472" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5650822A-AB74-4D3B-8305-08DBDA90336A}"/>
+  <xr:revisionPtr revIDLastSave="1476" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0644E223-8A60-4383-8040-E978D8D7F625}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="810" windowWidth="17130" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -375,10 +375,10 @@
     <t>https://sen.hn/informe-estadistico-semanal-de-cchac/</t>
   </si>
   <si>
-    <t>https://www.energia.gob.pa/documentos/</t>
+    <t>https://www.energia.gob.pa/archivos/?mdocs-cat=mdocs-cat-9</t>
   </si>
   <si>
-    <t>https://www.energia.gob.pa/archivos/?mdocs-cat=mdocs-cat-9</t>
+    <t>https://www.acodeco.gob.pa/uploads/pdf/combustibles/</t>
   </si>
 </sst>
 </file>
@@ -1651,8 +1651,8 @@
   <dimension ref="A1:W814"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A799" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B814" sqref="B814"/>
+      <pane ySplit="3" topLeftCell="A779" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E793" sqref="E793"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12880,7 +12880,7 @@
       <c r="C784" s="25"/>
       <c r="D784" s="25"/>
     </row>
-    <row r="785" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="785" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A785" s="8">
         <v>44247</v>
       </c>
@@ -12888,15 +12888,24 @@
       <c r="C785" s="25"/>
       <c r="D785" s="25"/>
     </row>
-    <row r="786" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="786" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A786" s="8">
         <v>44248</v>
       </c>
       <c r="B786" s="25"/>
       <c r="C786" s="25"/>
       <c r="D786" s="25"/>
-    </row>
-    <row r="787" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E786" s="21">
+        <v>2.78</v>
+      </c>
+      <c r="F786" s="21">
+        <v>2.72</v>
+      </c>
+      <c r="G786" s="21">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="787" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A787" s="8">
         <v>44249</v>
       </c>
@@ -12904,7 +12913,7 @@
       <c r="C787" s="25"/>
       <c r="D787" s="25"/>
     </row>
-    <row r="788" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A788" s="8">
         <v>44250</v>
       </c>
@@ -12912,7 +12921,7 @@
       <c r="C788" s="25"/>
       <c r="D788" s="25"/>
     </row>
-    <row r="789" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="789" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A789" s="8">
         <v>44251</v>
       </c>
@@ -12920,7 +12929,7 @@
       <c r="C789" s="25"/>
       <c r="D789" s="25"/>
     </row>
-    <row r="790" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="790" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A790" s="8">
         <v>44252</v>
       </c>
@@ -12928,7 +12937,7 @@
       <c r="C790" s="25"/>
       <c r="D790" s="25"/>
     </row>
-    <row r="791" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="791" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A791" s="8">
         <v>44253</v>
       </c>
@@ -12936,7 +12945,7 @@
       <c r="C791" s="25"/>
       <c r="D791" s="25"/>
     </row>
-    <row r="792" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="792" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A792" s="8">
         <v>44254</v>
       </c>
@@ -12944,7 +12953,7 @@
       <c r="C792" s="25"/>
       <c r="D792" s="25"/>
     </row>
-    <row r="793" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="793" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A793" s="8">
         <v>44255</v>
       </c>
@@ -12956,7 +12965,7 @@
         <v>1473.02</v>
       </c>
     </row>
-    <row r="794" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="794" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A794" s="8">
         <v>44256</v>
       </c>
@@ -12964,7 +12973,7 @@
       <c r="C794" s="25"/>
       <c r="D794" s="25"/>
     </row>
-    <row r="795" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="795" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A795" s="8">
         <v>44257</v>
       </c>
@@ -12972,7 +12981,7 @@
       <c r="C795" s="25"/>
       <c r="D795" s="25"/>
     </row>
-    <row r="796" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="796" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A796" s="8">
         <v>44258</v>
       </c>
@@ -12980,7 +12989,7 @@
       <c r="C796" s="25"/>
       <c r="D796" s="25"/>
     </row>
-    <row r="797" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A797" s="8">
         <v>44259</v>
       </c>
@@ -12988,7 +12997,7 @@
       <c r="C797" s="25"/>
       <c r="D797" s="25"/>
     </row>
-    <row r="798" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A798" s="8">
         <v>44260</v>
       </c>
@@ -12996,7 +13005,7 @@
       <c r="C798" s="25"/>
       <c r="D798" s="25"/>
     </row>
-    <row r="799" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A799" s="8">
         <v>44261</v>
       </c>
@@ -13004,7 +13013,7 @@
       <c r="C799" s="25"/>
       <c r="D799" s="25"/>
     </row>
-    <row r="800" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="800" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A800" s="8">
         <v>44262</v>
       </c>
@@ -13146,7 +13155,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13429,7 +13438,7 @@
         <v>75</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>76</v>
@@ -13486,7 +13495,7 @@
         <v>77</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-24-2021 00-31-10
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1476" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0644E223-8A60-4383-8040-E978D8D7F625}"/>
+  <xr:revisionPtr revIDLastSave="1493" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{90B82218-1515-4B26-85A5-1DD16432F17E}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="810" windowWidth="17130" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="17445" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H814" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H814" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H828" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H828" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1333,8 +1333,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R55" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R55" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R56" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R56" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W814"/>
+  <dimension ref="A1:W828"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A779" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E793" sqref="E793"/>
+      <pane ySplit="3" topLeftCell="A813" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D828" sqref="D828"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2860,7 +2860,7 @@
         <v>Enero, 2019</v>
       </c>
       <c r="M28" s="24">
-        <v>331.32889999999998</v>
+        <v>331.79227842289998</v>
       </c>
       <c r="N28" s="2">
         <v>43308.89</v>
@@ -2902,7 +2902,7 @@
         <v>Febrero, 2019</v>
       </c>
       <c r="M29" s="24">
-        <v>328.63400000000001</v>
+        <v>327.54095469060053</v>
       </c>
       <c r="N29" s="2">
         <v>51395.21</v>
@@ -2944,7 +2944,7 @@
         <v>Marzo, 2019</v>
       </c>
       <c r="M30" s="24">
-        <v>364.33889770244838</v>
+        <v>361.47824828044622</v>
       </c>
       <c r="N30" s="2">
         <v>60634.097999999998</v>
@@ -2988,7 +2988,7 @@
         <v>Abril, 2019</v>
       </c>
       <c r="M31" s="24">
-        <v>333.48007691186666</v>
+        <v>331.69492925226791</v>
       </c>
       <c r="N31" s="2">
         <v>68221.039000000004</v>
@@ -3030,7 +3030,7 @@
         <v>Mayo, 2019</v>
       </c>
       <c r="M32" s="24">
-        <v>328.002921080259</v>
+        <v>329.04436646063061</v>
       </c>
       <c r="N32" s="2">
         <v>63247.701000000001</v>
@@ -3072,7 +3072,7 @@
         <v>Junio, 2019</v>
       </c>
       <c r="M33" s="24">
-        <v>343.69303369887035</v>
+        <v>342.06805496641988</v>
       </c>
       <c r="N33" s="2">
         <v>86458.164999999994</v>
@@ -3120,7 +3120,7 @@
         <v>Julio, 2019</v>
       </c>
       <c r="M34" s="24">
-        <v>322.31220289308749</v>
+        <v>326.88726900591166</v>
       </c>
       <c r="N34" s="2">
         <v>275466.90399999998</v>
@@ -3162,7 +3162,7 @@
         <v>Agosto, 2019</v>
       </c>
       <c r="M35" s="24">
-        <v>339.43098738157141</v>
+        <v>343.03149858744376</v>
       </c>
       <c r="N35" s="2">
         <v>149332.54</v>
@@ -3212,7 +3212,7 @@
         <v>Septiembre, 2019</v>
       </c>
       <c r="M36" s="24">
-        <v>334.79059757082905</v>
+        <v>340.11523926656309</v>
       </c>
       <c r="N36" s="2">
         <v>214166.18599999999</v>
@@ -3256,7 +3256,7 @@
         <v>Octubre, 2019</v>
       </c>
       <c r="M37" s="24">
-        <v>357.60777156513046</v>
+        <v>359.83953761663122</v>
       </c>
       <c r="N37" s="2">
         <v>223565.73</v>
@@ -3298,7 +3298,7 @@
         <v>Noviembre, 2019</v>
       </c>
       <c r="M38" s="24">
-        <v>345.43188779185346</v>
+        <v>346.63259299837517</v>
       </c>
       <c r="N38" s="2">
         <v>103221.327</v>
@@ -3340,7 +3340,7 @@
         <v>Diciembre , 2019</v>
       </c>
       <c r="M39" s="24">
-        <v>345.68285804018092</v>
+        <v>348.26904675965937</v>
       </c>
       <c r="N39" s="2">
         <v>165252.29199999999</v>
@@ -3384,7 +3384,7 @@
         <v>Enero, 2020</v>
       </c>
       <c r="M40" s="24">
-        <v>339.61158109834963</v>
+        <v>345.72501531547721</v>
       </c>
       <c r="N40" s="2">
         <v>157509.239</v>
@@ -3426,7 +3426,7 @@
         <v>Febrero, 2020</v>
       </c>
       <c r="M41" s="24">
-        <v>334.01742836097281</v>
+        <v>338.73174736590823</v>
       </c>
       <c r="N41" s="2">
         <v>184085.48300000001</v>
@@ -3468,7 +3468,7 @@
         <v>Marzo, 2020</v>
       </c>
       <c r="M42" s="24">
-        <v>366.38633514958934</v>
+        <v>364.78145538603928</v>
       </c>
       <c r="N42" s="2">
         <v>181206.992</v>
@@ -3518,7 +3518,7 @@
         <v>Abril, 2020</v>
       </c>
       <c r="M43" s="24">
-        <v>245.00732997578669</v>
+        <v>247.18712829655288</v>
       </c>
       <c r="N43" s="2">
         <v>89167.92</v>
@@ -3560,7 +3560,7 @@
         <v>Mayo, 2020</v>
       </c>
       <c r="M44" s="24">
-        <v>225.38759592718446</v>
+        <v>228.29929707050536</v>
       </c>
       <c r="N44" s="2">
         <v>78383.501999999993</v>
@@ -3602,7 +3602,7 @@
         <v>Junio, 2020</v>
       </c>
       <c r="M45" s="24">
-        <v>239.10946995623192</v>
+        <v>243.00656400193247</v>
       </c>
       <c r="N45" s="2">
         <v>107559.02800000001</v>
@@ -3646,7 +3646,7 @@
         <v>Julio, 2020</v>
       </c>
       <c r="M46" s="24">
-        <v>223.13587473103388</v>
+        <v>241.95295042385374</v>
       </c>
       <c r="N46" s="2">
         <v>91433.98</v>
@@ -3688,7 +3688,7 @@
         <v>Agosto, 2020</v>
       </c>
       <c r="M47" s="24">
-        <v>239.65563601447195</v>
+        <v>251.35003199559037</v>
       </c>
       <c r="N47" s="2">
         <v>188088.80300000001</v>
@@ -3730,7 +3730,7 @@
         <v>Septiembre, 2020</v>
       </c>
       <c r="M48" s="24">
-        <v>260.31128588533551</v>
+        <v>268.97176432623962</v>
       </c>
       <c r="N48" s="2">
         <v>226098.86</v>
@@ -3776,7 +3776,7 @@
         <v>Octubre, 2020</v>
       </c>
       <c r="M49" s="24">
-        <v>297.6383833861118</v>
+        <v>312.11629922642197</v>
       </c>
       <c r="N49" s="2">
         <v>146935.704</v>
@@ -3824,7 +3824,7 @@
         <v>Noviembre, 2020</v>
       </c>
       <c r="M50" s="24">
-        <v>296.77843816013888</v>
+        <v>300.20826455933565</v>
       </c>
       <c r="N50" s="2">
         <v>102213.842</v>
@@ -3865,7 +3865,9 @@
         <f>+K51&amp;", "&amp;J51</f>
         <v>Diciembre, 2020</v>
       </c>
-      <c r="M51" s="21"/>
+      <c r="M51" s="24">
+        <v>316.09856314386326</v>
+      </c>
       <c r="N51" s="2">
         <v>172851.421</v>
       </c>
@@ -3905,7 +3907,9 @@
         <f t="shared" ref="L52" si="5">+K52&amp;", "&amp;J52</f>
         <v>Enero, 2021</v>
       </c>
-      <c r="M52" s="21"/>
+      <c r="M52" s="24">
+        <v>295.15693645642841</v>
+      </c>
       <c r="N52" s="2">
         <v>241506.179</v>
       </c>
@@ -3945,7 +3949,7 @@
         <f>+K53&amp;", "&amp;J53</f>
         <v>Febrero, 2021</v>
       </c>
-      <c r="M53" s="21"/>
+      <c r="M53" s="24"/>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
@@ -3979,7 +3983,7 @@
         <f t="shared" ref="L54" si="6">+K54&amp;", "&amp;J54</f>
         <v>Marzo, 2021</v>
       </c>
-      <c r="M54" s="21"/>
+      <c r="M54" s="24"/>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
@@ -4013,7 +4017,7 @@
         <f>+K55&amp;", "&amp;J55</f>
         <v>Abril, 2021</v>
       </c>
-      <c r="M55" s="21"/>
+      <c r="M55" s="24"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -4037,13 +4041,20 @@
       <c r="G56" s="21"/>
       <c r="H56" s="21"/>
       <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
+      <c r="J56" s="9">
+        <v>2021</v>
+      </c>
+      <c r="K56" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L56" s="9" t="str">
+        <f t="shared" ref="L56" si="7">+K56&amp;", "&amp;J56</f>
+        <v>Mayo, 2021</v>
+      </c>
       <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="21"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
       <c r="Q56" s="21"/>
       <c r="R56" s="21"/>
       <c r="S56" s="21"/>
@@ -12694,7 +12705,7 @@
       <c r="C765" s="25">
         <v>1.24</v>
       </c>
-      <c r="D765" s="25">
+      <c r="D765" s="23">
         <v>1497.16</v>
       </c>
       <c r="E765" s="21"/>
@@ -12961,8 +12972,17 @@
       <c r="C793" s="25">
         <v>1.22</v>
       </c>
-      <c r="D793" s="25">
+      <c r="D793" s="23">
         <v>1473.02</v>
+      </c>
+      <c r="E793">
+        <v>2.84</v>
+      </c>
+      <c r="F793">
+        <v>2.79</v>
+      </c>
+      <c r="G793">
+        <v>2.46</v>
       </c>
     </row>
     <row r="794" spans="1:7" x14ac:dyDescent="0.25">
@@ -13020,6 +13040,15 @@
       <c r="B800" s="25"/>
       <c r="C800" s="25"/>
       <c r="D800" s="25"/>
+      <c r="E800">
+        <v>3.02</v>
+      </c>
+      <c r="F800">
+        <v>2.96</v>
+      </c>
+      <c r="G800">
+        <v>2.61</v>
+      </c>
     </row>
     <row r="801" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A801" s="8">
@@ -13132,6 +13161,118 @@
       <c r="B814" s="25"/>
       <c r="C814" s="25"/>
       <c r="D814" s="25"/>
+    </row>
+    <row r="815" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A815" s="8">
+        <v>44277</v>
+      </c>
+      <c r="B815" s="25"/>
+      <c r="C815" s="25"/>
+      <c r="D815" s="25"/>
+    </row>
+    <row r="816" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A816" s="8">
+        <v>44278</v>
+      </c>
+      <c r="B816" s="25"/>
+      <c r="C816" s="25"/>
+      <c r="D816" s="25"/>
+    </row>
+    <row r="817" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A817" s="8">
+        <v>44279</v>
+      </c>
+      <c r="B817" s="25"/>
+      <c r="C817" s="25"/>
+      <c r="D817" s="25"/>
+    </row>
+    <row r="818" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A818" s="8">
+        <v>44280</v>
+      </c>
+      <c r="B818" s="25"/>
+      <c r="C818" s="25"/>
+      <c r="D818" s="25"/>
+    </row>
+    <row r="819" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A819" s="8">
+        <v>44281</v>
+      </c>
+      <c r="B819" s="25"/>
+      <c r="C819" s="25"/>
+      <c r="D819" s="25"/>
+    </row>
+    <row r="820" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A820" s="8">
+        <v>44282</v>
+      </c>
+      <c r="B820" s="25"/>
+      <c r="C820" s="25"/>
+      <c r="D820" s="25"/>
+    </row>
+    <row r="821" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A821" s="8">
+        <v>44283</v>
+      </c>
+      <c r="B821" s="25"/>
+      <c r="C821" s="25"/>
+      <c r="D821" s="25"/>
+    </row>
+    <row r="822" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A822" s="8">
+        <v>44284</v>
+      </c>
+      <c r="B822" s="25"/>
+      <c r="C822" s="25"/>
+      <c r="D822" s="25"/>
+    </row>
+    <row r="823" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A823" s="8">
+        <v>44285</v>
+      </c>
+      <c r="B823" s="25"/>
+      <c r="C823" s="25"/>
+      <c r="D823" s="25"/>
+    </row>
+    <row r="824" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A824" s="8">
+        <v>44286</v>
+      </c>
+      <c r="B824" s="25"/>
+      <c r="C824" s="25"/>
+      <c r="D824" s="25"/>
+    </row>
+    <row r="825" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A825" s="8">
+        <v>44287</v>
+      </c>
+      <c r="B825" s="25"/>
+      <c r="C825" s="25"/>
+      <c r="D825" s="25"/>
+    </row>
+    <row r="826" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A826" s="8">
+        <v>44288</v>
+      </c>
+      <c r="B826" s="25"/>
+      <c r="C826" s="25"/>
+      <c r="D826" s="25"/>
+    </row>
+    <row r="827" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A827" s="8">
+        <v>44289</v>
+      </c>
+      <c r="B827" s="25"/>
+      <c r="C827" s="25"/>
+      <c r="D827" s="25"/>
+    </row>
+    <row r="828" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A828" s="8">
+        <v>44290</v>
+      </c>
+      <c r="B828" s="25"/>
+      <c r="C828" s="25"/>
+      <c r="D828" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -13152,10 +13293,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-26-2021 20-30-59
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1493" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{90B82218-1515-4B26-85A5-1DD16432F17E}"/>
+  <xr:revisionPtr revIDLastSave="1495" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{23DB1606-FB2D-4E9F-AF35-40CE747437C7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="735" windowWidth="17445" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="780" windowWidth="16905" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1652,7 +1652,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A813" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D828" sqref="D828"/>
+      <selection pane="bottomLeft" activeCell="B828" sqref="B828"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13296,7 +13296,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 03-31-2021 02-01-00
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1495" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{23DB1606-FB2D-4E9F-AF35-40CE747437C7}"/>
+  <xr:revisionPtr revIDLastSave="1499" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{19CB9634-4A29-4D46-920C-00F98FBF817E}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="780" windowWidth="16905" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="16935" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -13293,10 +13293,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-01-2021 22-31-03
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1499" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{19CB9634-4A29-4D46-920C-00F98FBF817E}"/>
+  <xr:revisionPtr revIDLastSave="1502" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C7049C11-908A-4E53-A049-ABC4A346E1C9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="16935" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H828" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H828" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H835" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H835" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W828"/>
+  <dimension ref="A1:W835"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A813" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B828" sqref="B828"/>
+      <pane ySplit="3" topLeftCell="A823" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B835" sqref="B835"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3950,9 +3950,13 @@
         <v>Febrero, 2021</v>
       </c>
       <c r="M53" s="24"/>
-      <c r="N53" s="2"/>
+      <c r="N53" s="2">
+        <v>238513.94700000004</v>
+      </c>
       <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
+      <c r="P53" s="2">
+        <v>361.48</v>
+      </c>
       <c r="Q53" s="21"/>
       <c r="R53" s="21"/>
       <c r="S53" s="21"/>
@@ -13274,6 +13278,62 @@
       <c r="C828" s="25"/>
       <c r="D828" s="25"/>
     </row>
+    <row r="829" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A829" s="8">
+        <v>44291</v>
+      </c>
+      <c r="B829" s="25"/>
+      <c r="C829" s="25"/>
+      <c r="D829" s="25"/>
+    </row>
+    <row r="830" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A830" s="8">
+        <v>44292</v>
+      </c>
+      <c r="B830" s="25"/>
+      <c r="C830" s="25"/>
+      <c r="D830" s="25"/>
+    </row>
+    <row r="831" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A831" s="8">
+        <v>44293</v>
+      </c>
+      <c r="B831" s="25"/>
+      <c r="C831" s="25"/>
+      <c r="D831" s="25"/>
+    </row>
+    <row r="832" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A832" s="8">
+        <v>44294</v>
+      </c>
+      <c r="B832" s="25"/>
+      <c r="C832" s="25"/>
+      <c r="D832" s="25"/>
+    </row>
+    <row r="833" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A833" s="8">
+        <v>44295</v>
+      </c>
+      <c r="B833" s="25"/>
+      <c r="C833" s="25"/>
+      <c r="D833" s="25"/>
+    </row>
+    <row r="834" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A834" s="8">
+        <v>44296</v>
+      </c>
+      <c r="B834" s="25"/>
+      <c r="C834" s="25"/>
+      <c r="D834" s="25"/>
+    </row>
+    <row r="835" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A835" s="8">
+        <v>44297</v>
+      </c>
+      <c r="B835" s="25"/>
+      <c r="C835" s="25"/>
+      <c r="D835" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -13296,7 +13356,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-07-2021 00-30-36
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1502" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C7049C11-908A-4E53-A049-ABC4A346E1C9}"/>
+  <xr:revisionPtr revIDLastSave="1510" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2A52EE1C-2D67-485A-A5C4-5EDA7FB80758}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H835" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H835" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H842" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H842" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W835"/>
+  <dimension ref="A1:W842"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A823" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B835" sqref="B835"/>
+      <pane ySplit="3" topLeftCell="A827" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B842" sqref="B842"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13054,7 +13054,7 @@
         <v>2.61</v>
       </c>
     </row>
-    <row r="801" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A801" s="8">
         <v>44263</v>
       </c>
@@ -13062,7 +13062,7 @@
       <c r="C801" s="25"/>
       <c r="D801" s="25"/>
     </row>
-    <row r="802" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A802" s="8">
         <v>44264</v>
       </c>
@@ -13070,7 +13070,7 @@
       <c r="C802" s="25"/>
       <c r="D802" s="25"/>
     </row>
-    <row r="803" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A803" s="8">
         <v>44265</v>
       </c>
@@ -13078,7 +13078,7 @@
       <c r="C803" s="25"/>
       <c r="D803" s="25"/>
     </row>
-    <row r="804" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="804" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A804" s="8">
         <v>44266</v>
       </c>
@@ -13086,7 +13086,7 @@
       <c r="C804" s="25"/>
       <c r="D804" s="25"/>
     </row>
-    <row r="805" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="805" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A805" s="8">
         <v>44267</v>
       </c>
@@ -13094,15 +13094,24 @@
       <c r="C805" s="25"/>
       <c r="D805" s="25"/>
     </row>
-    <row r="806" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A806" s="8">
         <v>44268</v>
       </c>
       <c r="B806" s="25"/>
       <c r="C806" s="25"/>
       <c r="D806" s="25"/>
-    </row>
-    <row r="807" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E806" s="21">
+        <v>3.02</v>
+      </c>
+      <c r="F806" s="21">
+        <v>2.96</v>
+      </c>
+      <c r="G806" s="21">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="807" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A807" s="8">
         <v>44269</v>
       </c>
@@ -13110,7 +13119,7 @@
       <c r="C807" s="25"/>
       <c r="D807" s="25"/>
     </row>
-    <row r="808" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="808" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A808" s="8">
         <v>44270</v>
       </c>
@@ -13118,7 +13127,7 @@
       <c r="C808" s="25"/>
       <c r="D808" s="25"/>
     </row>
-    <row r="809" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A809" s="8">
         <v>44271</v>
       </c>
@@ -13126,7 +13135,7 @@
       <c r="C809" s="25"/>
       <c r="D809" s="25"/>
     </row>
-    <row r="810" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="810" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A810" s="8">
         <v>44272</v>
       </c>
@@ -13134,7 +13143,7 @@
       <c r="C810" s="25"/>
       <c r="D810" s="25"/>
     </row>
-    <row r="811" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="811" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A811" s="8">
         <v>44273</v>
       </c>
@@ -13142,7 +13151,7 @@
       <c r="C811" s="25"/>
       <c r="D811" s="25"/>
     </row>
-    <row r="812" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="812" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A812" s="8">
         <v>44274</v>
       </c>
@@ -13150,15 +13159,24 @@
       <c r="C812" s="25"/>
       <c r="D812" s="25"/>
     </row>
-    <row r="813" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="813" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A813" s="8">
         <v>44275</v>
       </c>
       <c r="B813" s="25"/>
       <c r="C813" s="25"/>
       <c r="D813" s="25"/>
-    </row>
-    <row r="814" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E813">
+        <v>3.18</v>
+      </c>
+      <c r="F813">
+        <v>3.11</v>
+      </c>
+      <c r="G813">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="814" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A814" s="8">
         <v>44276</v>
       </c>
@@ -13166,7 +13184,7 @@
       <c r="C814" s="25"/>
       <c r="D814" s="25"/>
     </row>
-    <row r="815" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A815" s="8">
         <v>44277</v>
       </c>
@@ -13174,7 +13192,7 @@
       <c r="C815" s="25"/>
       <c r="D815" s="25"/>
     </row>
-    <row r="816" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A816" s="8">
         <v>44278</v>
       </c>
@@ -13333,6 +13351,62 @@
       <c r="B835" s="25"/>
       <c r="C835" s="25"/>
       <c r="D835" s="25"/>
+    </row>
+    <row r="836" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A836" s="8">
+        <v>44298</v>
+      </c>
+      <c r="B836" s="25"/>
+      <c r="C836" s="25"/>
+      <c r="D836" s="25"/>
+    </row>
+    <row r="837" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A837" s="8">
+        <v>44299</v>
+      </c>
+      <c r="B837" s="25"/>
+      <c r="C837" s="25"/>
+      <c r="D837" s="25"/>
+    </row>
+    <row r="838" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A838" s="8">
+        <v>44300</v>
+      </c>
+      <c r="B838" s="25"/>
+      <c r="C838" s="25"/>
+      <c r="D838" s="25"/>
+    </row>
+    <row r="839" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A839" s="8">
+        <v>44301</v>
+      </c>
+      <c r="B839" s="25"/>
+      <c r="C839" s="25"/>
+      <c r="D839" s="25"/>
+    </row>
+    <row r="840" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A840" s="8">
+        <v>44302</v>
+      </c>
+      <c r="B840" s="25"/>
+      <c r="C840" s="25"/>
+      <c r="D840" s="25"/>
+    </row>
+    <row r="841" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A841" s="8">
+        <v>44303</v>
+      </c>
+      <c r="B841" s="25"/>
+      <c r="C841" s="25"/>
+      <c r="D841" s="25"/>
+    </row>
+    <row r="842" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A842" s="8">
+        <v>44304</v>
+      </c>
+      <c r="B842" s="25"/>
+      <c r="C842" s="25"/>
+      <c r="D842" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -13356,7 +13430,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-10-2021 00-30-45
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1510" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2A52EE1C-2D67-485A-A5C4-5EDA7FB80758}"/>
+  <xr:revisionPtr revIDLastSave="1511" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9E0D2880-6FC3-44F6-9C17-B5A17BCE2EDE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13101,15 +13101,6 @@
       <c r="B806" s="25"/>
       <c r="C806" s="25"/>
       <c r="D806" s="25"/>
-      <c r="E806" s="21">
-        <v>3.02</v>
-      </c>
-      <c r="F806" s="21">
-        <v>2.96</v>
-      </c>
-      <c r="G806" s="21">
-        <v>2.61</v>
-      </c>
     </row>
     <row r="807" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A807" s="8">
@@ -13118,6 +13109,15 @@
       <c r="B807" s="25"/>
       <c r="C807" s="25"/>
       <c r="D807" s="25"/>
+      <c r="E807" s="21">
+        <v>3.02</v>
+      </c>
+      <c r="F807" s="21">
+        <v>2.96</v>
+      </c>
+      <c r="G807" s="21">
+        <v>2.61</v>
+      </c>
     </row>
     <row r="808" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A808" s="8">
@@ -13166,15 +13166,6 @@
       <c r="B813" s="25"/>
       <c r="C813" s="25"/>
       <c r="D813" s="25"/>
-      <c r="E813">
-        <v>3.18</v>
-      </c>
-      <c r="F813">
-        <v>3.11</v>
-      </c>
-      <c r="G813">
-        <v>2.69</v>
-      </c>
     </row>
     <row r="814" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A814" s="8">
@@ -13183,6 +13174,15 @@
       <c r="B814" s="25"/>
       <c r="C814" s="25"/>
       <c r="D814" s="25"/>
+      <c r="E814">
+        <v>3.18</v>
+      </c>
+      <c r="F814">
+        <v>3.11</v>
+      </c>
+      <c r="G814">
+        <v>2.69</v>
+      </c>
     </row>
     <row r="815" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A815" s="8">
@@ -13430,7 +13430,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-14-2021 00-31-11
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1511" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9E0D2880-6FC3-44F6-9C17-B5A17BCE2EDE}"/>
+  <xr:revisionPtr revIDLastSave="1514" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B8897AF5-24C3-4877-B854-53239F2944D9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H842" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H842" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H849" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H849" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W842"/>
+  <dimension ref="A1:W849"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A827" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B842" sqref="B842"/>
+      <pane ySplit="3" topLeftCell="A834" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B849" sqref="B849"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13408,6 +13408,62 @@
       <c r="C842" s="25"/>
       <c r="D842" s="25"/>
     </row>
+    <row r="843" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A843" s="8">
+        <v>44305</v>
+      </c>
+      <c r="B843" s="25"/>
+      <c r="C843" s="25"/>
+      <c r="D843" s="25"/>
+    </row>
+    <row r="844" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A844" s="8">
+        <v>44306</v>
+      </c>
+      <c r="B844" s="25"/>
+      <c r="C844" s="25"/>
+      <c r="D844" s="25"/>
+    </row>
+    <row r="845" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A845" s="8">
+        <v>44307</v>
+      </c>
+      <c r="B845" s="25"/>
+      <c r="C845" s="25"/>
+      <c r="D845" s="25"/>
+    </row>
+    <row r="846" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A846" s="8">
+        <v>44308</v>
+      </c>
+      <c r="B846" s="25"/>
+      <c r="C846" s="25"/>
+      <c r="D846" s="25"/>
+    </row>
+    <row r="847" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A847" s="8">
+        <v>44309</v>
+      </c>
+      <c r="B847" s="25"/>
+      <c r="C847" s="25"/>
+      <c r="D847" s="25"/>
+    </row>
+    <row r="848" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A848" s="8">
+        <v>44310</v>
+      </c>
+      <c r="B848" s="25"/>
+      <c r="C848" s="25"/>
+      <c r="D848" s="25"/>
+    </row>
+    <row r="849" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A849" s="8">
+        <v>44311</v>
+      </c>
+      <c r="B849" s="25"/>
+      <c r="C849" s="25"/>
+      <c r="D849" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -13430,7 +13486,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-16-2021 22-30-29
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1514" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B8897AF5-24C3-4877-B854-53239F2944D9}"/>
+  <xr:revisionPtr revIDLastSave="1521" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2FAD7F33-3FD0-4A22-9871-1717A20BB505}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3914,7 +3914,7 @@
         <v>241506.179</v>
       </c>
       <c r="O52" s="2">
-        <v>672024</v>
+        <v>672023.848</v>
       </c>
       <c r="P52" s="2">
         <v>362.07</v>
@@ -3953,7 +3953,9 @@
       <c r="N53" s="2">
         <v>238513.94700000004</v>
       </c>
-      <c r="O53" s="2"/>
+      <c r="O53" s="2">
+        <v>752477.07500000007</v>
+      </c>
       <c r="P53" s="2">
         <v>361.48</v>
       </c>
@@ -13200,7 +13202,7 @@
       <c r="C816" s="25"/>
       <c r="D816" s="25"/>
     </row>
-    <row r="817" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A817" s="8">
         <v>44279</v>
       </c>
@@ -13208,7 +13210,7 @@
       <c r="C817" s="25"/>
       <c r="D817" s="25"/>
     </row>
-    <row r="818" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A818" s="8">
         <v>44280</v>
       </c>
@@ -13216,7 +13218,7 @@
       <c r="C818" s="25"/>
       <c r="D818" s="25"/>
     </row>
-    <row r="819" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="819" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A819" s="8">
         <v>44281</v>
       </c>
@@ -13224,7 +13226,7 @@
       <c r="C819" s="25"/>
       <c r="D819" s="25"/>
     </row>
-    <row r="820" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A820" s="8">
         <v>44282</v>
       </c>
@@ -13232,15 +13234,24 @@
       <c r="C820" s="25"/>
       <c r="D820" s="25"/>
     </row>
-    <row r="821" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A821" s="8">
         <v>44283</v>
       </c>
       <c r="B821" s="25"/>
       <c r="C821" s="25"/>
       <c r="D821" s="25"/>
-    </row>
-    <row r="822" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E821">
+        <v>3.18</v>
+      </c>
+      <c r="F821">
+        <v>3.11</v>
+      </c>
+      <c r="G821">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="822" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A822" s="8">
         <v>44284</v>
       </c>
@@ -13248,7 +13259,7 @@
       <c r="C822" s="25"/>
       <c r="D822" s="25"/>
     </row>
-    <row r="823" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="823" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A823" s="8">
         <v>44285</v>
       </c>
@@ -13256,7 +13267,7 @@
       <c r="C823" s="25"/>
       <c r="D823" s="25"/>
     </row>
-    <row r="824" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="824" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A824" s="8">
         <v>44286</v>
       </c>
@@ -13264,7 +13275,7 @@
       <c r="C824" s="25"/>
       <c r="D824" s="25"/>
     </row>
-    <row r="825" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="825" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A825" s="8">
         <v>44287</v>
       </c>
@@ -13272,7 +13283,7 @@
       <c r="C825" s="25"/>
       <c r="D825" s="25"/>
     </row>
-    <row r="826" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="826" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A826" s="8">
         <v>44288</v>
       </c>
@@ -13280,7 +13291,7 @@
       <c r="C826" s="25"/>
       <c r="D826" s="25"/>
     </row>
-    <row r="827" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="827" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A827" s="8">
         <v>44289</v>
       </c>
@@ -13288,15 +13299,24 @@
       <c r="C827" s="25"/>
       <c r="D827" s="25"/>
     </row>
-    <row r="828" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="828" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A828" s="8">
         <v>44290</v>
       </c>
       <c r="B828" s="25"/>
       <c r="C828" s="25"/>
       <c r="D828" s="25"/>
-    </row>
-    <row r="829" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E828">
+        <v>3.23</v>
+      </c>
+      <c r="F828">
+        <v>3.17</v>
+      </c>
+      <c r="G828">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="829" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A829" s="8">
         <v>44291</v>
       </c>
@@ -13304,7 +13324,7 @@
       <c r="C829" s="25"/>
       <c r="D829" s="25"/>
     </row>
-    <row r="830" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="830" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A830" s="8">
         <v>44292</v>
       </c>
@@ -13312,7 +13332,7 @@
       <c r="C830" s="25"/>
       <c r="D830" s="25"/>
     </row>
-    <row r="831" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="831" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A831" s="8">
         <v>44293</v>
       </c>
@@ -13320,7 +13340,7 @@
       <c r="C831" s="25"/>
       <c r="D831" s="25"/>
     </row>
-    <row r="832" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A832" s="8">
         <v>44294</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-21-2021 00-31-06
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1521" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2FAD7F33-3FD0-4A22-9871-1717A20BB505}"/>
+  <xr:revisionPtr revIDLastSave="1525" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{42D950BA-64A5-4EBE-91E1-3E4050B6BE2E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H849" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H849" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H856" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H856" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W849"/>
+  <dimension ref="A1:W856"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A834" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B849" sqref="B849"/>
+      <pane ySplit="3" topLeftCell="A841" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B856" sqref="B856"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13348,7 +13348,7 @@
       <c r="C832" s="25"/>
       <c r="D832" s="25"/>
     </row>
-    <row r="833" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A833" s="8">
         <v>44295</v>
       </c>
@@ -13356,7 +13356,7 @@
       <c r="C833" s="25"/>
       <c r="D833" s="25"/>
     </row>
-    <row r="834" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="834" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A834" s="8">
         <v>44296</v>
       </c>
@@ -13364,15 +13364,24 @@
       <c r="C834" s="25"/>
       <c r="D834" s="25"/>
     </row>
-    <row r="835" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A835" s="8">
         <v>44297</v>
       </c>
       <c r="B835" s="25"/>
       <c r="C835" s="25"/>
       <c r="D835" s="25"/>
-    </row>
-    <row r="836" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E835">
+        <v>3.19</v>
+      </c>
+      <c r="F835">
+        <v>3.11</v>
+      </c>
+      <c r="G835">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="836" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A836" s="8">
         <v>44298</v>
       </c>
@@ -13380,7 +13389,7 @@
       <c r="C836" s="25"/>
       <c r="D836" s="25"/>
     </row>
-    <row r="837" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A837" s="8">
         <v>44299</v>
       </c>
@@ -13388,7 +13397,7 @@
       <c r="C837" s="25"/>
       <c r="D837" s="25"/>
     </row>
-    <row r="838" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A838" s="8">
         <v>44300</v>
       </c>
@@ -13396,7 +13405,7 @@
       <c r="C838" s="25"/>
       <c r="D838" s="25"/>
     </row>
-    <row r="839" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A839" s="8">
         <v>44301</v>
       </c>
@@ -13404,7 +13413,7 @@
       <c r="C839" s="25"/>
       <c r="D839" s="25"/>
     </row>
-    <row r="840" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="840" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A840" s="8">
         <v>44302</v>
       </c>
@@ -13412,7 +13421,7 @@
       <c r="C840" s="25"/>
       <c r="D840" s="25"/>
     </row>
-    <row r="841" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A841" s="8">
         <v>44303</v>
       </c>
@@ -13420,7 +13429,7 @@
       <c r="C841" s="25"/>
       <c r="D841" s="25"/>
     </row>
-    <row r="842" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A842" s="8">
         <v>44304</v>
       </c>
@@ -13428,7 +13437,7 @@
       <c r="C842" s="25"/>
       <c r="D842" s="25"/>
     </row>
-    <row r="843" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A843" s="8">
         <v>44305</v>
       </c>
@@ -13436,7 +13445,7 @@
       <c r="C843" s="25"/>
       <c r="D843" s="25"/>
     </row>
-    <row r="844" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A844" s="8">
         <v>44306</v>
       </c>
@@ -13444,7 +13453,7 @@
       <c r="C844" s="25"/>
       <c r="D844" s="25"/>
     </row>
-    <row r="845" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A845" s="8">
         <v>44307</v>
       </c>
@@ -13452,7 +13461,7 @@
       <c r="C845" s="25"/>
       <c r="D845" s="25"/>
     </row>
-    <row r="846" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A846" s="8">
         <v>44308</v>
       </c>
@@ -13460,7 +13469,7 @@
       <c r="C846" s="25"/>
       <c r="D846" s="25"/>
     </row>
-    <row r="847" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A847" s="8">
         <v>44309</v>
       </c>
@@ -13468,7 +13477,7 @@
       <c r="C847" s="25"/>
       <c r="D847" s="25"/>
     </row>
-    <row r="848" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="848" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A848" s="8">
         <v>44310</v>
       </c>
@@ -13483,6 +13492,62 @@
       <c r="B849" s="25"/>
       <c r="C849" s="25"/>
       <c r="D849" s="25"/>
+    </row>
+    <row r="850" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A850" s="8">
+        <v>44312</v>
+      </c>
+      <c r="B850" s="25"/>
+      <c r="C850" s="25"/>
+      <c r="D850" s="25"/>
+    </row>
+    <row r="851" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A851" s="8">
+        <v>44313</v>
+      </c>
+      <c r="B851" s="25"/>
+      <c r="C851" s="25"/>
+      <c r="D851" s="25"/>
+    </row>
+    <row r="852" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A852" s="8">
+        <v>44314</v>
+      </c>
+      <c r="B852" s="25"/>
+      <c r="C852" s="25"/>
+      <c r="D852" s="25"/>
+    </row>
+    <row r="853" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A853" s="8">
+        <v>44315</v>
+      </c>
+      <c r="B853" s="25"/>
+      <c r="C853" s="25"/>
+      <c r="D853" s="25"/>
+    </row>
+    <row r="854" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A854" s="8">
+        <v>44316</v>
+      </c>
+      <c r="B854" s="25"/>
+      <c r="C854" s="25"/>
+      <c r="D854" s="25"/>
+    </row>
+    <row r="855" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A855" s="8">
+        <v>44317</v>
+      </c>
+      <c r="B855" s="25"/>
+      <c r="C855" s="25"/>
+      <c r="D855" s="25"/>
+    </row>
+    <row r="856" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A856" s="8">
+        <v>44318</v>
+      </c>
+      <c r="B856" s="25"/>
+      <c r="C856" s="25"/>
+      <c r="D856" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-24-2021 00-30-40
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1525" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{42D950BA-64A5-4EBE-91E1-3E4050B6BE2E}"/>
+  <xr:revisionPtr revIDLastSave="1529" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{332B6DAA-97A5-4408-8D28-7D9DCBA86A6C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H856" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H856" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H863" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H863" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W856"/>
+  <dimension ref="A1:W863"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A841" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B856" sqref="B856"/>
+      <pane ySplit="3" topLeftCell="A849" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B863" sqref="B863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3908,7 +3908,7 @@
         <v>Enero, 2021</v>
       </c>
       <c r="M52" s="24">
-        <v>295.15693645642841</v>
+        <v>295.15693645642801</v>
       </c>
       <c r="N52" s="2">
         <v>241506.179</v>
@@ -3949,7 +3949,9 @@
         <f>+K53&amp;", "&amp;J53</f>
         <v>Febrero, 2021</v>
       </c>
-      <c r="M53" s="24"/>
+      <c r="M53" s="24">
+        <v>305.77029949946126</v>
+      </c>
       <c r="N53" s="2">
         <v>238513.94700000004</v>
       </c>
@@ -13549,6 +13551,62 @@
       <c r="C856" s="25"/>
       <c r="D856" s="25"/>
     </row>
+    <row r="857" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A857" s="8">
+        <v>44319</v>
+      </c>
+      <c r="B857" s="25"/>
+      <c r="C857" s="25"/>
+      <c r="D857" s="25"/>
+    </row>
+    <row r="858" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A858" s="8">
+        <v>44320</v>
+      </c>
+      <c r="B858" s="25"/>
+      <c r="C858" s="25"/>
+      <c r="D858" s="25"/>
+    </row>
+    <row r="859" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A859" s="8">
+        <v>44321</v>
+      </c>
+      <c r="B859" s="25"/>
+      <c r="C859" s="25"/>
+      <c r="D859" s="25"/>
+    </row>
+    <row r="860" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A860" s="8">
+        <v>44322</v>
+      </c>
+      <c r="B860" s="25"/>
+      <c r="C860" s="25"/>
+      <c r="D860" s="25"/>
+    </row>
+    <row r="861" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A861" s="8">
+        <v>44323</v>
+      </c>
+      <c r="B861" s="25"/>
+      <c r="C861" s="25"/>
+      <c r="D861" s="25"/>
+    </row>
+    <row r="862" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A862" s="8">
+        <v>44324</v>
+      </c>
+      <c r="B862" s="25"/>
+      <c r="C862" s="25"/>
+      <c r="D862" s="25"/>
+    </row>
+    <row r="863" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A863" s="8">
+        <v>44325</v>
+      </c>
+      <c r="B863" s="25"/>
+      <c r="C863" s="25"/>
+      <c r="D863" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -13571,7 +13629,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-28-2021 00-30-33
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1529" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{332B6DAA-97A5-4408-8D28-7D9DCBA86A6C}"/>
+  <xr:revisionPtr revIDLastSave="1531" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AADA3B73-B9FA-40F2-AE66-B11973912878}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1651,8 +1651,8 @@
   <dimension ref="A1:W863"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A849" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B863" sqref="B863"/>
+      <pane ySplit="3" topLeftCell="A848" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C863" sqref="C863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13629,7 +13629,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 04-30-2021 22-30-29
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1531" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AADA3B73-B9FA-40F2-AE66-B11973912878}"/>
+  <xr:revisionPtr revIDLastSave="1532" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BFFDE024-C41D-47D7-9273-450C84154BF7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H863" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H863" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H870" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H870" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W863"/>
+  <dimension ref="A1:W870"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A848" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C863" sqref="C863"/>
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13607,6 +13607,62 @@
       <c r="C863" s="25"/>
       <c r="D863" s="25"/>
     </row>
+    <row r="864" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A864" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B864" s="25"/>
+      <c r="C864" s="25"/>
+      <c r="D864" s="25"/>
+    </row>
+    <row r="865" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A865" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B865" s="25"/>
+      <c r="C865" s="25"/>
+      <c r="D865" s="25"/>
+    </row>
+    <row r="866" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A866" s="8">
+        <v>44328</v>
+      </c>
+      <c r="B866" s="25"/>
+      <c r="C866" s="25"/>
+      <c r="D866" s="25"/>
+    </row>
+    <row r="867" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A867" s="8">
+        <v>44329</v>
+      </c>
+      <c r="B867" s="25"/>
+      <c r="C867" s="25"/>
+      <c r="D867" s="25"/>
+    </row>
+    <row r="868" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A868" s="8">
+        <v>44330</v>
+      </c>
+      <c r="B868" s="25"/>
+      <c r="C868" s="25"/>
+      <c r="D868" s="25"/>
+    </row>
+    <row r="869" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A869" s="8">
+        <v>44331</v>
+      </c>
+      <c r="B869" s="25"/>
+      <c r="C869" s="25"/>
+      <c r="D869" s="25"/>
+    </row>
+    <row r="870" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A870" s="8">
+        <v>44332</v>
+      </c>
+      <c r="B870" s="25"/>
+      <c r="C870" s="25"/>
+      <c r="D870" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -13625,11 +13681,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB840748-361D-4458-B100-AAECA785CA65}">
   <dimension ref="A1:Y959"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-05-2021 00-30-54
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1532" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BFFDE024-C41D-47D7-9273-450C84154BF7}"/>
+  <xr:revisionPtr revIDLastSave="1538" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FFAEC99E-3C83-4E29-9F28-9E145F591658}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1333,8 +1333,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R56" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R56" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R57" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R57" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
@@ -1650,9 +1650,9 @@
   </sheetPr>
   <dimension ref="A1:W870"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M54" sqref="M54"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A855" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B870" sqref="B870"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,13 +4089,20 @@
       </c>
       <c r="H57" s="21"/>
       <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="21"/>
+      <c r="J57" s="9">
+        <v>2021</v>
+      </c>
+      <c r="K57" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L57" s="9" t="str">
+        <f>+K57&amp;", "&amp;J57</f>
+        <v>Junio, 2021</v>
+      </c>
       <c r="M57" s="21"/>
-      <c r="N57" s="21"/>
-      <c r="O57" s="21"/>
-      <c r="P57" s="21"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
       <c r="Q57" s="21"/>
       <c r="R57" s="21"/>
       <c r="S57" s="21"/>
@@ -13438,6 +13445,15 @@
       <c r="B842" s="25"/>
       <c r="C842" s="25"/>
       <c r="D842" s="25"/>
+      <c r="E842" s="21">
+        <v>3.19</v>
+      </c>
+      <c r="F842" s="21">
+        <v>3.11</v>
+      </c>
+      <c r="G842" s="21">
+        <v>2.59</v>
+      </c>
     </row>
     <row r="843" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A843" s="8">
@@ -13487,15 +13503,24 @@
       <c r="C848" s="25"/>
       <c r="D848" s="25"/>
     </row>
-    <row r="849" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="849" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A849" s="8">
         <v>44311</v>
       </c>
       <c r="B849" s="25"/>
       <c r="C849" s="25"/>
       <c r="D849" s="25"/>
-    </row>
-    <row r="850" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E849">
+        <v>3.23</v>
+      </c>
+      <c r="F849">
+        <v>3.14</v>
+      </c>
+      <c r="G849">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="850" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A850" s="8">
         <v>44312</v>
       </c>
@@ -13503,7 +13528,7 @@
       <c r="C850" s="25"/>
       <c r="D850" s="25"/>
     </row>
-    <row r="851" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="851" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A851" s="8">
         <v>44313</v>
       </c>
@@ -13511,7 +13536,7 @@
       <c r="C851" s="25"/>
       <c r="D851" s="25"/>
     </row>
-    <row r="852" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="852" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A852" s="8">
         <v>44314</v>
       </c>
@@ -13519,7 +13544,7 @@
       <c r="C852" s="25"/>
       <c r="D852" s="25"/>
     </row>
-    <row r="853" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="853" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A853" s="8">
         <v>44315</v>
       </c>
@@ -13527,7 +13552,7 @@
       <c r="C853" s="25"/>
       <c r="D853" s="25"/>
     </row>
-    <row r="854" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="854" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A854" s="8">
         <v>44316</v>
       </c>
@@ -13535,7 +13560,7 @@
       <c r="C854" s="25"/>
       <c r="D854" s="25"/>
     </row>
-    <row r="855" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="855" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A855" s="8">
         <v>44317</v>
       </c>
@@ -13543,7 +13568,7 @@
       <c r="C855" s="25"/>
       <c r="D855" s="25"/>
     </row>
-    <row r="856" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="856" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A856" s="8">
         <v>44318</v>
       </c>
@@ -13551,7 +13576,7 @@
       <c r="C856" s="25"/>
       <c r="D856" s="25"/>
     </row>
-    <row r="857" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="857" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A857" s="8">
         <v>44319</v>
       </c>
@@ -13559,7 +13584,7 @@
       <c r="C857" s="25"/>
       <c r="D857" s="25"/>
     </row>
-    <row r="858" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="858" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A858" s="8">
         <v>44320</v>
       </c>
@@ -13567,7 +13592,7 @@
       <c r="C858" s="25"/>
       <c r="D858" s="25"/>
     </row>
-    <row r="859" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="859" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A859" s="8">
         <v>44321</v>
       </c>
@@ -13575,7 +13600,7 @@
       <c r="C859" s="25"/>
       <c r="D859" s="25"/>
     </row>
-    <row r="860" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="860" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A860" s="8">
         <v>44322</v>
       </c>
@@ -13583,7 +13608,7 @@
       <c r="C860" s="25"/>
       <c r="D860" s="25"/>
     </row>
-    <row r="861" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="861" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A861" s="8">
         <v>44323</v>
       </c>
@@ -13591,7 +13616,7 @@
       <c r="C861" s="25"/>
       <c r="D861" s="25"/>
     </row>
-    <row r="862" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="862" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A862" s="8">
         <v>44324</v>
       </c>
@@ -13599,7 +13624,7 @@
       <c r="C862" s="25"/>
       <c r="D862" s="25"/>
     </row>
-    <row r="863" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="863" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A863" s="8">
         <v>44325</v>
       </c>
@@ -13607,7 +13632,7 @@
       <c r="C863" s="25"/>
       <c r="D863" s="25"/>
     </row>
-    <row r="864" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="864" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A864" s="8">
         <v>44326</v>
       </c>
@@ -13681,11 +13706,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB840748-361D-4458-B100-AAECA785CA65}">
   <dimension ref="A1:Y959"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-07-2021 22-31-03
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1538" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FFAEC99E-3C83-4E29-9F28-9E145F591658}"/>
+  <xr:revisionPtr revIDLastSave="1539" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CEA7C911-1845-4A3A-992A-100CEC6264E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H870" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H870" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H877" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H877" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W870"/>
+  <dimension ref="A1:W877"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A855" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B870" sqref="B870"/>
+      <pane ySplit="3" topLeftCell="A817" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C824" sqref="C824"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13687,6 +13687,62 @@
       <c r="B870" s="25"/>
       <c r="C870" s="25"/>
       <c r="D870" s="25"/>
+    </row>
+    <row r="871" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A871" s="8">
+        <v>44333</v>
+      </c>
+      <c r="B871" s="25"/>
+      <c r="C871" s="25"/>
+      <c r="D871" s="25"/>
+    </row>
+    <row r="872" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A872" s="8">
+        <v>44334</v>
+      </c>
+      <c r="B872" s="25"/>
+      <c r="C872" s="25"/>
+      <c r="D872" s="25"/>
+    </row>
+    <row r="873" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A873" s="8">
+        <v>44335</v>
+      </c>
+      <c r="B873" s="25"/>
+      <c r="C873" s="25"/>
+      <c r="D873" s="25"/>
+    </row>
+    <row r="874" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A874" s="8">
+        <v>44336</v>
+      </c>
+      <c r="B874" s="25"/>
+      <c r="C874" s="25"/>
+      <c r="D874" s="25"/>
+    </row>
+    <row r="875" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A875" s="8">
+        <v>44337</v>
+      </c>
+      <c r="B875" s="25"/>
+      <c r="C875" s="25"/>
+      <c r="D875" s="25"/>
+    </row>
+    <row r="876" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A876" s="8">
+        <v>44338</v>
+      </c>
+      <c r="B876" s="25"/>
+      <c r="C876" s="25"/>
+      <c r="D876" s="25"/>
+    </row>
+    <row r="877" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A877" s="8">
+        <v>44339</v>
+      </c>
+      <c r="B877" s="25"/>
+      <c r="C877" s="25"/>
+      <c r="D877" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-08-2021 00-31-16
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1539" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CEA7C911-1845-4A3A-992A-100CEC6264E4}"/>
+  <xr:revisionPtr revIDLastSave="1547" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C1D39D28-9BD7-4534-9271-B0F82D62FAC2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1651,8 +1651,8 @@
   <dimension ref="A1:W877"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A817" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C824" sqref="C824"/>
+      <pane ySplit="3" topLeftCell="A862" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B877" sqref="B877"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3387,7 +3387,7 @@
         <v>345.72501531547721</v>
       </c>
       <c r="N40" s="2">
-        <v>157509.239</v>
+        <v>200483.24100000004</v>
       </c>
       <c r="O40" s="2">
         <v>913121.64899999998</v>
@@ -3429,7 +3429,7 @@
         <v>338.73174736590823</v>
       </c>
       <c r="N41" s="2">
-        <v>184085.48300000001</v>
+        <v>232012.64700000003</v>
       </c>
       <c r="O41" s="2">
         <v>750772.66500000004</v>
@@ -3471,7 +3471,7 @@
         <v>364.78145538603928</v>
       </c>
       <c r="N42" s="2">
-        <v>181206.992</v>
+        <v>275901.41500000004</v>
       </c>
       <c r="O42" s="2">
         <v>787744.87100000004</v>
@@ -3911,7 +3911,7 @@
         <v>295.15693645642801</v>
       </c>
       <c r="N52" s="2">
-        <v>241506.179</v>
+        <v>220466.29799999998</v>
       </c>
       <c r="O52" s="2">
         <v>672023.848</v>
@@ -3953,7 +3953,7 @@
         <v>305.77029949946126</v>
       </c>
       <c r="N53" s="2">
-        <v>238513.94700000004</v>
+        <v>236572.63099999999</v>
       </c>
       <c r="O53" s="2">
         <v>752477.07500000007</v>
@@ -3992,9 +3992,13 @@
         <v>Marzo, 2021</v>
       </c>
       <c r="M54" s="24"/>
-      <c r="N54" s="2"/>
+      <c r="N54" s="2">
+        <v>320846.07300000003</v>
+      </c>
       <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
+      <c r="P54" s="2">
+        <v>368.69</v>
+      </c>
       <c r="Q54" s="21"/>
       <c r="R54" s="21"/>
       <c r="S54" s="21"/>
@@ -13575,6 +13579,9 @@
       <c r="B856" s="25"/>
       <c r="C856" s="25"/>
       <c r="D856" s="25"/>
+      <c r="E856" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="857" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A857" s="8">
@@ -13766,7 +13773,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-12-2021 00-30-49
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1547" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C1D39D28-9BD7-4534-9271-B0F82D62FAC2}"/>
+  <xr:revisionPtr revIDLastSave="1552" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1C298968-8845-4E3C-BABC-B4D9B54FA9CF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1652,7 +1652,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A862" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B877" sqref="B877"/>
+      <selection pane="bottomLeft" activeCell="C877" sqref="C877"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13285,8 +13285,12 @@
         <v>44286</v>
       </c>
       <c r="B824" s="25"/>
-      <c r="C824" s="25"/>
-      <c r="D824" s="25"/>
+      <c r="C824" s="25">
+        <v>1.23</v>
+      </c>
+      <c r="D824" s="23">
+        <v>1475.78</v>
+      </c>
     </row>
     <row r="825" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A825" s="8">
@@ -13579,8 +13583,14 @@
       <c r="B856" s="25"/>
       <c r="C856" s="25"/>
       <c r="D856" s="25"/>
-      <c r="E856" t="s">
-        <v>31</v>
+      <c r="E856">
+        <v>3.23</v>
+      </c>
+      <c r="F856" s="21">
+        <v>3.14</v>
+      </c>
+      <c r="G856" s="21">
+        <v>2.64</v>
       </c>
     </row>
     <row r="857" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-15-2021 00-30-53
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1552" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1C298968-8845-4E3C-BABC-B4D9B54FA9CF}"/>
+  <xr:revisionPtr revIDLastSave="1555" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{60815BDD-6E10-4775-A956-2A325857F9C5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H877" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H877" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H884" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H884" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W877"/>
+  <dimension ref="A1:W884"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A862" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C877" sqref="C877"/>
+      <pane ySplit="3" topLeftCell="A869" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B884" sqref="B884"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13761,6 +13761,62 @@
       <c r="C877" s="25"/>
       <c r="D877" s="25"/>
     </row>
+    <row r="878" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A878" s="8">
+        <v>44340</v>
+      </c>
+      <c r="B878" s="25"/>
+      <c r="C878" s="25"/>
+      <c r="D878" s="25"/>
+    </row>
+    <row r="879" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A879" s="8">
+        <v>44341</v>
+      </c>
+      <c r="B879" s="25"/>
+      <c r="C879" s="25"/>
+      <c r="D879" s="25"/>
+    </row>
+    <row r="880" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A880" s="8">
+        <v>44342</v>
+      </c>
+      <c r="B880" s="25"/>
+      <c r="C880" s="25"/>
+      <c r="D880" s="25"/>
+    </row>
+    <row r="881" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A881" s="8">
+        <v>44343</v>
+      </c>
+      <c r="B881" s="25"/>
+      <c r="C881" s="25"/>
+      <c r="D881" s="25"/>
+    </row>
+    <row r="882" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A882" s="8">
+        <v>44344</v>
+      </c>
+      <c r="B882" s="25"/>
+      <c r="C882" s="25"/>
+      <c r="D882" s="25"/>
+    </row>
+    <row r="883" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A883" s="8">
+        <v>44345</v>
+      </c>
+      <c r="B883" s="25"/>
+      <c r="C883" s="25"/>
+      <c r="D883" s="25"/>
+    </row>
+    <row r="884" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A884" s="8">
+        <v>44346</v>
+      </c>
+      <c r="B884" s="25"/>
+      <c r="C884" s="25"/>
+      <c r="D884" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -13783,7 +13839,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-19-2021 17-07-54
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1555" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{60815BDD-6E10-4775-A956-2A325857F9C5}"/>
+  <xr:revisionPtr revIDLastSave="1564" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{38C9D45B-636E-4A76-B1DA-F143AE93459B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3390,7 +3390,7 @@
         <v>200483.24100000004</v>
       </c>
       <c r="O40" s="2">
-        <v>913121.64899999998</v>
+        <v>913121.64900000009</v>
       </c>
       <c r="P40" s="2">
         <v>457.59</v>
@@ -3474,7 +3474,7 @@
         <v>275901.41500000004</v>
       </c>
       <c r="O42" s="2">
-        <v>787744.87100000004</v>
+        <v>787744.87099999993</v>
       </c>
       <c r="P42" s="2">
         <v>425.56</v>
@@ -3995,7 +3995,9 @@
       <c r="N54" s="2">
         <v>320846.07300000003</v>
       </c>
-      <c r="O54" s="2"/>
+      <c r="O54" s="2">
+        <v>967545.10200000007</v>
+      </c>
       <c r="P54" s="2">
         <v>368.69</v>
       </c>
@@ -13565,8 +13567,12 @@
         <v>44316</v>
       </c>
       <c r="B854" s="25"/>
-      <c r="C854" s="25"/>
-      <c r="D854" s="25"/>
+      <c r="C854" s="25">
+        <v>1.23</v>
+      </c>
+      <c r="D854" s="23">
+        <v>1485.48</v>
+      </c>
     </row>
     <row r="855" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A855" s="8">
@@ -13648,6 +13654,15 @@
       <c r="B863" s="25"/>
       <c r="C863" s="25"/>
       <c r="D863" s="25"/>
+      <c r="E863">
+        <v>3.27</v>
+      </c>
+      <c r="F863">
+        <v>3.17</v>
+      </c>
+      <c r="G863">
+        <v>2.71</v>
+      </c>
     </row>
     <row r="864" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A864" s="8">

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-21-2021 00-30-44
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1564" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{38C9D45B-636E-4A76-B1DA-F143AE93459B}"/>
+  <xr:revisionPtr revIDLastSave="1569" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F05F08E0-3202-4F77-A0F3-B35CB25E8031}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1651,8 +1651,8 @@
   <dimension ref="A1:W884"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A869" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B884" sqref="B884"/>
+      <pane ySplit="3" topLeftCell="A872" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C884" sqref="C884"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3996,7 +3996,7 @@
         <v>320846.07300000003</v>
       </c>
       <c r="O54" s="2">
-        <v>967545.10200000007</v>
+        <v>967545.10199999996</v>
       </c>
       <c r="P54" s="2">
         <v>368.69</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 05-25-2021 22-31-02
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1569" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F05F08E0-3202-4F77-A0F3-B35CB25E8031}"/>
+  <xr:revisionPtr revIDLastSave="1571" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1B94A25E-879A-48FC-AB4E-73067B8E52DE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
     <sheet name="Fuentes" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1651,7 +1651,7 @@
   <dimension ref="A1:W884"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A872" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A871" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C884" sqref="C884"/>
     </sheetView>
   </sheetViews>
@@ -13854,7 +13854,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-06-2021 18-24-07
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1582" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AA31DFF-5FEA-4815-A606-E81A59CF8A71}"/>
+  <xr:revisionPtr revIDLastSave="1583" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9858598-99B7-4CCD-99B7-931AE7B040FE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H898" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H898" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H905" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H905" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W898"/>
+  <dimension ref="A1:W905"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A883" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B898" sqref="B898"/>
+      <pane ySplit="3" topLeftCell="A890" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B905" sqref="B905"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13971,6 +13971,62 @@
       <c r="C898" s="25"/>
       <c r="D898" s="25"/>
     </row>
+    <row r="899" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A899" s="8">
+        <v>44361</v>
+      </c>
+      <c r="B899" s="25"/>
+      <c r="C899" s="25"/>
+      <c r="D899" s="25"/>
+    </row>
+    <row r="900" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A900" s="8">
+        <v>44362</v>
+      </c>
+      <c r="B900" s="25"/>
+      <c r="C900" s="25"/>
+      <c r="D900" s="25"/>
+    </row>
+    <row r="901" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A901" s="8">
+        <v>44363</v>
+      </c>
+      <c r="B901" s="25"/>
+      <c r="C901" s="25"/>
+      <c r="D901" s="25"/>
+    </row>
+    <row r="902" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A902" s="8">
+        <v>44364</v>
+      </c>
+      <c r="B902" s="25"/>
+      <c r="C902" s="25"/>
+      <c r="D902" s="25"/>
+    </row>
+    <row r="903" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A903" s="8">
+        <v>44365</v>
+      </c>
+      <c r="B903" s="25"/>
+      <c r="C903" s="25"/>
+      <c r="D903" s="25"/>
+    </row>
+    <row r="904" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A904" s="8">
+        <v>44366</v>
+      </c>
+      <c r="B904" s="25"/>
+      <c r="C904" s="25"/>
+      <c r="D904" s="25"/>
+    </row>
+    <row r="905" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A905" s="8">
+        <v>44367</v>
+      </c>
+      <c r="B905" s="25"/>
+      <c r="C905" s="25"/>
+      <c r="D905" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -13990,10 +14046,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-10-2021 01-35-42
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1583" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9858598-99B7-4CCD-99B7-931AE7B040FE}"/>
+  <xr:revisionPtr revIDLastSave="1585" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AD3D4CE-C06B-4EF0-A0D7-7A003A1852A8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1651,8 +1651,8 @@
   <dimension ref="A1:W905"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A890" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B905" sqref="B905"/>
+      <pane ySplit="3" topLeftCell="A891" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B906" sqref="B906"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14023,7 +14023,6 @@
       <c r="A905" s="8">
         <v>44367</v>
       </c>
-      <c r="B905" s="25"/>
       <c r="C905" s="25"/>
       <c r="D905" s="25"/>
     </row>
@@ -14049,7 +14048,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-12-2021 00-30-50
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1585" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AD3D4CE-C06B-4EF0-A0D7-7A003A1852A8}"/>
+  <xr:revisionPtr revIDLastSave="1590" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE4B0195-89A6-4C77-ACE2-982373BB84A1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H905" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H905" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H912" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H912" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W905"/>
+  <dimension ref="A1:W912"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A891" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B906" sqref="B906"/>
+      <pane ySplit="3" topLeftCell="A898" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B913" sqref="B913"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3387,7 +3387,7 @@
         <v>345.72501531547721</v>
       </c>
       <c r="N40" s="2">
-        <v>200483.24100000004</v>
+        <v>157509.23899999997</v>
       </c>
       <c r="O40" s="2">
         <v>913121.64900000009</v>
@@ -3429,7 +3429,7 @@
         <v>338.73174736590823</v>
       </c>
       <c r="N41" s="2">
-        <v>232012.64700000003</v>
+        <v>184085.48299999998</v>
       </c>
       <c r="O41" s="2">
         <v>750772.66500000004</v>
@@ -3471,7 +3471,7 @@
         <v>364.78145538603928</v>
       </c>
       <c r="N42" s="2">
-        <v>275901.41500000004</v>
+        <v>181206.992</v>
       </c>
       <c r="O42" s="2">
         <v>787744.87099999993</v>
@@ -3911,7 +3911,7 @@
         <v>295.15693645642801</v>
       </c>
       <c r="N52" s="2">
-        <v>220466.29799999998</v>
+        <v>241506.179</v>
       </c>
       <c r="O52" s="2">
         <v>672023.848</v>
@@ -3953,7 +3953,7 @@
         <v>305.77029949946126</v>
       </c>
       <c r="N53" s="2">
-        <v>236572.63099999999</v>
+        <v>238513.94700000004</v>
       </c>
       <c r="O53" s="2">
         <v>752477.07500000007</v>
@@ -3995,10 +3995,10 @@
         <v>342.80006038760365</v>
       </c>
       <c r="N54" s="2">
-        <v>320846.07300000003</v>
+        <v>326246.35299999989</v>
       </c>
       <c r="O54" s="2">
-        <v>967545.10199999996</v>
+        <v>967545.10200000007</v>
       </c>
       <c r="P54" s="2">
         <v>368.69</v>
@@ -4036,7 +4036,9 @@
       <c r="M55" s="24"/>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
+      <c r="P55" s="2">
+        <v>374.79</v>
+      </c>
       <c r="Q55" s="21"/>
       <c r="R55" s="21"/>
       <c r="S55" s="21"/>
@@ -14026,6 +14028,62 @@
       <c r="C905" s="25"/>
       <c r="D905" s="25"/>
     </row>
+    <row r="906" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A906" s="8">
+        <v>44368</v>
+      </c>
+      <c r="B906" s="25"/>
+      <c r="C906" s="25"/>
+      <c r="D906" s="25"/>
+    </row>
+    <row r="907" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A907" s="8">
+        <v>44369</v>
+      </c>
+      <c r="B907" s="25"/>
+      <c r="C907" s="25"/>
+      <c r="D907" s="25"/>
+    </row>
+    <row r="908" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A908" s="8">
+        <v>44370</v>
+      </c>
+      <c r="B908" s="25"/>
+      <c r="C908" s="25"/>
+      <c r="D908" s="25"/>
+    </row>
+    <row r="909" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A909" s="8">
+        <v>44371</v>
+      </c>
+      <c r="B909" s="25"/>
+      <c r="C909" s="25"/>
+      <c r="D909" s="25"/>
+    </row>
+    <row r="910" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A910" s="8">
+        <v>44372</v>
+      </c>
+      <c r="B910" s="25"/>
+      <c r="C910" s="25"/>
+      <c r="D910" s="25"/>
+    </row>
+    <row r="911" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A911" s="8">
+        <v>44373</v>
+      </c>
+      <c r="B911" s="25"/>
+      <c r="C911" s="25"/>
+      <c r="D911" s="25"/>
+    </row>
+    <row r="912" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A912" s="8">
+        <v>44374</v>
+      </c>
+      <c r="B912" s="25"/>
+      <c r="C912" s="25"/>
+      <c r="D912" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -14048,7 +14106,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-16-2021 00-30-50
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1590" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE4B0195-89A6-4C77-ACE2-982373BB84A1}"/>
+  <xr:revisionPtr revIDLastSave="1601" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{564B5351-82DD-4D20-8E35-6E159C2378A4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="13920" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1652,7 +1652,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A898" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B913" sqref="B913"/>
+      <selection pane="bottomLeft" activeCell="C913" sqref="C913"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4034,8 +4034,12 @@
         <v>Abril, 2021</v>
       </c>
       <c r="M55" s="24"/>
-      <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
+      <c r="N55" s="2">
+        <v>279712.50599999999</v>
+      </c>
+      <c r="O55" s="2">
+        <v>887233.929</v>
+      </c>
       <c r="P55" s="2">
         <v>374.79</v>
       </c>
@@ -13582,7 +13586,7 @@
         <v>1.23</v>
       </c>
       <c r="D854" s="23">
-        <v>1485.48</v>
+        <v>1487.25</v>
       </c>
     </row>
     <row r="855" spans="1:7" x14ac:dyDescent="0.25">
@@ -13866,8 +13870,12 @@
         <v>44347</v>
       </c>
       <c r="B885" s="25"/>
-      <c r="C885" s="25"/>
-      <c r="D885" s="25"/>
+      <c r="C885" s="25">
+        <v>1.23</v>
+      </c>
+      <c r="D885" s="23">
+        <v>1513.23</v>
+      </c>
     </row>
     <row r="886" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A886" s="8">
@@ -14103,10 +14111,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-18-2021 22-30-34
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1601" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{564B5351-82DD-4D20-8E35-6E159C2378A4}"/>
+  <xr:revisionPtr revIDLastSave="1608" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4583E476-22B7-40D7-9B76-4F3F8DBCF03E}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="13920" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="585" windowWidth="12975" windowHeight="10335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H912" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H912" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H919" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H919" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W912"/>
+  <dimension ref="A1:W919"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A898" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C913" sqref="C913"/>
+      <pane ySplit="3" topLeftCell="A905" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B920" sqref="B920"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13833,7 +13833,7 @@
       <c r="C880" s="25"/>
       <c r="D880" s="25"/>
     </row>
-    <row r="881" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A881" s="8">
         <v>44343</v>
       </c>
@@ -13841,7 +13841,7 @@
       <c r="C881" s="25"/>
       <c r="D881" s="25"/>
     </row>
-    <row r="882" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="882" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A882" s="8">
         <v>44344</v>
       </c>
@@ -13849,7 +13849,7 @@
       <c r="C882" s="25"/>
       <c r="D882" s="25"/>
     </row>
-    <row r="883" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="883" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A883" s="8">
         <v>44345</v>
       </c>
@@ -13857,15 +13857,24 @@
       <c r="C883" s="25"/>
       <c r="D883" s="25"/>
     </row>
-    <row r="884" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="884" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A884" s="8">
         <v>44346</v>
       </c>
       <c r="B884" s="25"/>
       <c r="C884" s="25"/>
       <c r="D884" s="25"/>
-    </row>
-    <row r="885" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E884" s="21">
+        <v>3.36</v>
+      </c>
+      <c r="F884" s="21">
+        <v>3.25</v>
+      </c>
+      <c r="G884" s="21">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="885" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A885" s="8">
         <v>44347</v>
       </c>
@@ -13877,7 +13886,7 @@
         <v>1513.23</v>
       </c>
     </row>
-    <row r="886" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A886" s="8">
         <v>44348</v>
       </c>
@@ -13885,7 +13894,7 @@
       <c r="C886" s="25"/>
       <c r="D886" s="25"/>
     </row>
-    <row r="887" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="887" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A887" s="8">
         <v>44349</v>
       </c>
@@ -13893,7 +13902,7 @@
       <c r="C887" s="25"/>
       <c r="D887" s="25"/>
     </row>
-    <row r="888" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="888" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A888" s="8">
         <v>44350</v>
       </c>
@@ -13901,7 +13910,7 @@
       <c r="C888" s="25"/>
       <c r="D888" s="25"/>
     </row>
-    <row r="889" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="889" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A889" s="8">
         <v>44351</v>
       </c>
@@ -13909,7 +13918,7 @@
       <c r="C889" s="25"/>
       <c r="D889" s="25"/>
     </row>
-    <row r="890" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="890" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A890" s="8">
         <v>44352</v>
       </c>
@@ -13917,15 +13926,24 @@
       <c r="C890" s="25"/>
       <c r="D890" s="25"/>
     </row>
-    <row r="891" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A891" s="8">
         <v>44353</v>
       </c>
       <c r="B891" s="25"/>
       <c r="C891" s="25"/>
       <c r="D891" s="25"/>
-    </row>
-    <row r="892" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E891" s="21">
+        <v>3.32</v>
+      </c>
+      <c r="F891" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="G891" s="21">
+        <v>2.82</v>
+      </c>
+    </row>
+    <row r="892" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A892" s="8">
         <v>44354</v>
       </c>
@@ -13933,7 +13951,7 @@
       <c r="C892" s="25"/>
       <c r="D892" s="25"/>
     </row>
-    <row r="893" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A893" s="8">
         <v>44355</v>
       </c>
@@ -13941,7 +13959,7 @@
       <c r="C893" s="25"/>
       <c r="D893" s="25"/>
     </row>
-    <row r="894" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A894" s="8">
         <v>44356</v>
       </c>
@@ -13949,7 +13967,7 @@
       <c r="C894" s="25"/>
       <c r="D894" s="25"/>
     </row>
-    <row r="895" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A895" s="8">
         <v>44357</v>
       </c>
@@ -13957,7 +13975,7 @@
       <c r="C895" s="25"/>
       <c r="D895" s="25"/>
     </row>
-    <row r="896" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A896" s="8">
         <v>44358</v>
       </c>
@@ -14091,6 +14109,62 @@
       <c r="B912" s="25"/>
       <c r="C912" s="25"/>
       <c r="D912" s="25"/>
+    </row>
+    <row r="913" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A913" s="8">
+        <v>44375</v>
+      </c>
+      <c r="B913" s="25"/>
+      <c r="C913" s="25"/>
+      <c r="D913" s="25"/>
+    </row>
+    <row r="914" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A914" s="8">
+        <v>44376</v>
+      </c>
+      <c r="B914" s="25"/>
+      <c r="C914" s="25"/>
+      <c r="D914" s="25"/>
+    </row>
+    <row r="915" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A915" s="8">
+        <v>44377</v>
+      </c>
+      <c r="B915" s="25"/>
+      <c r="C915" s="25"/>
+      <c r="D915" s="25"/>
+    </row>
+    <row r="916" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A916" s="8">
+        <v>44378</v>
+      </c>
+      <c r="B916" s="25"/>
+      <c r="C916" s="25"/>
+      <c r="D916" s="25"/>
+    </row>
+    <row r="917" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A917" s="8">
+        <v>44379</v>
+      </c>
+      <c r="B917" s="25"/>
+      <c r="C917" s="25"/>
+      <c r="D917" s="25"/>
+    </row>
+    <row r="918" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A918" s="8">
+        <v>44380</v>
+      </c>
+      <c r="B918" s="25"/>
+      <c r="C918" s="25"/>
+      <c r="D918" s="25"/>
+    </row>
+    <row r="919" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A919" s="8">
+        <v>44381</v>
+      </c>
+      <c r="B919" s="25"/>
+      <c r="C919" s="25"/>
+      <c r="D919" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -14114,7 +14188,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-26-2021 00-30-49
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1608" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4583E476-22B7-40D7-9B76-4F3F8DBCF03E}"/>
+  <xr:revisionPtr revIDLastSave="1618" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63E0EE72-7759-428C-B53D-A5E746B0D333}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="585" windowWidth="12975" windowHeight="10335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H919" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H919" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H926" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H926" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1333,8 +1333,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R58" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R58" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R59" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R59" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W919"/>
+  <dimension ref="A1:W926"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A905" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B920" sqref="B920"/>
+      <pane ySplit="3" topLeftCell="A912" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B927" sqref="B927"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3908,7 +3908,7 @@
         <v>Enero, 2021</v>
       </c>
       <c r="M52" s="24">
-        <v>295.15693645642801</v>
+        <v>295.15693645642841</v>
       </c>
       <c r="N52" s="2">
         <v>241506.179</v>
@@ -4033,7 +4033,9 @@
         <f>+K55&amp;", "&amp;J55</f>
         <v>Abril, 2021</v>
       </c>
-      <c r="M55" s="24"/>
+      <c r="M55" s="24">
+        <v>277.07312193278085</v>
+      </c>
       <c r="N55" s="2">
         <v>279712.50599999999</v>
       </c>
@@ -4171,13 +4173,20 @@
       <c r="G59" s="21"/>
       <c r="H59" s="21"/>
       <c r="I59" s="21"/>
-      <c r="J59" s="21"/>
-      <c r="K59" s="21"/>
-      <c r="L59" s="21"/>
+      <c r="J59" s="9">
+        <v>2021</v>
+      </c>
+      <c r="K59" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L59" s="9" t="str">
+        <f>+K59&amp;", "&amp;J59</f>
+        <v>Agosto, 2021</v>
+      </c>
       <c r="M59" s="21"/>
-      <c r="N59" s="21"/>
-      <c r="O59" s="21"/>
-      <c r="P59" s="21"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
       <c r="Q59" s="21"/>
       <c r="R59" s="21"/>
       <c r="S59" s="21"/>
@@ -13983,7 +13992,7 @@
       <c r="C896" s="25"/>
       <c r="D896" s="25"/>
     </row>
-    <row r="897" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A897" s="8">
         <v>44359</v>
       </c>
@@ -13991,15 +14000,24 @@
       <c r="C897" s="25"/>
       <c r="D897" s="25"/>
     </row>
-    <row r="898" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A898" s="8">
         <v>44360</v>
       </c>
       <c r="B898" s="25"/>
       <c r="C898" s="25"/>
       <c r="D898" s="25"/>
-    </row>
-    <row r="899" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E898" s="21">
+        <v>3.32</v>
+      </c>
+      <c r="F898" s="21">
+        <v>3.2</v>
+      </c>
+      <c r="G898" s="21">
+        <v>2.82</v>
+      </c>
+    </row>
+    <row r="899" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A899" s="8">
         <v>44361</v>
       </c>
@@ -14007,7 +14025,7 @@
       <c r="C899" s="25"/>
       <c r="D899" s="25"/>
     </row>
-    <row r="900" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="900" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A900" s="8">
         <v>44362</v>
       </c>
@@ -14015,7 +14033,7 @@
       <c r="C900" s="25"/>
       <c r="D900" s="25"/>
     </row>
-    <row r="901" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="901" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A901" s="8">
         <v>44363</v>
       </c>
@@ -14023,7 +14041,7 @@
       <c r="C901" s="25"/>
       <c r="D901" s="25"/>
     </row>
-    <row r="902" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A902" s="8">
         <v>44364</v>
       </c>
@@ -14031,7 +14049,7 @@
       <c r="C902" s="25"/>
       <c r="D902" s="25"/>
     </row>
-    <row r="903" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="903" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A903" s="8">
         <v>44365</v>
       </c>
@@ -14039,7 +14057,7 @@
       <c r="C903" s="25"/>
       <c r="D903" s="25"/>
     </row>
-    <row r="904" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="904" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A904" s="8">
         <v>44366</v>
       </c>
@@ -14047,14 +14065,23 @@
       <c r="C904" s="25"/>
       <c r="D904" s="25"/>
     </row>
-    <row r="905" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="905" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A905" s="8">
         <v>44367</v>
       </c>
       <c r="C905" s="25"/>
       <c r="D905" s="25"/>
-    </row>
-    <row r="906" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E905">
+        <v>3.41</v>
+      </c>
+      <c r="F905">
+        <v>3.29</v>
+      </c>
+      <c r="G905">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="906" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A906" s="8">
         <v>44368</v>
       </c>
@@ -14062,7 +14089,7 @@
       <c r="C906" s="25"/>
       <c r="D906" s="25"/>
     </row>
-    <row r="907" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="907" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A907" s="8">
         <v>44369</v>
       </c>
@@ -14070,7 +14097,7 @@
       <c r="C907" s="25"/>
       <c r="D907" s="25"/>
     </row>
-    <row r="908" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="908" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A908" s="8">
         <v>44370</v>
       </c>
@@ -14078,7 +14105,7 @@
       <c r="C908" s="25"/>
       <c r="D908" s="25"/>
     </row>
-    <row r="909" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="909" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A909" s="8">
         <v>44371</v>
       </c>
@@ -14086,7 +14113,7 @@
       <c r="C909" s="25"/>
       <c r="D909" s="25"/>
     </row>
-    <row r="910" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A910" s="8">
         <v>44372</v>
       </c>
@@ -14094,7 +14121,7 @@
       <c r="C910" s="25"/>
       <c r="D910" s="25"/>
     </row>
-    <row r="911" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A911" s="8">
         <v>44373</v>
       </c>
@@ -14102,7 +14129,7 @@
       <c r="C911" s="25"/>
       <c r="D911" s="25"/>
     </row>
-    <row r="912" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A912" s="8">
         <v>44374</v>
       </c>
@@ -14165,6 +14192,62 @@
       <c r="B919" s="25"/>
       <c r="C919" s="25"/>
       <c r="D919" s="25"/>
+    </row>
+    <row r="920" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A920" s="8">
+        <v>44382</v>
+      </c>
+      <c r="B920" s="25"/>
+      <c r="C920" s="25"/>
+      <c r="D920" s="25"/>
+    </row>
+    <row r="921" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A921" s="8">
+        <v>44383</v>
+      </c>
+      <c r="B921" s="25"/>
+      <c r="C921" s="25"/>
+      <c r="D921" s="25"/>
+    </row>
+    <row r="922" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A922" s="8">
+        <v>44384</v>
+      </c>
+      <c r="B922" s="25"/>
+      <c r="C922" s="25"/>
+      <c r="D922" s="25"/>
+    </row>
+    <row r="923" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A923" s="8">
+        <v>44385</v>
+      </c>
+      <c r="B923" s="25"/>
+      <c r="C923" s="25"/>
+      <c r="D923" s="25"/>
+    </row>
+    <row r="924" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A924" s="8">
+        <v>44386</v>
+      </c>
+      <c r="B924" s="25"/>
+      <c r="C924" s="25"/>
+      <c r="D924" s="25"/>
+    </row>
+    <row r="925" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A925" s="8">
+        <v>44387</v>
+      </c>
+      <c r="B925" s="25"/>
+      <c r="C925" s="25"/>
+      <c r="D925" s="25"/>
+    </row>
+    <row r="926" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A926" s="8">
+        <v>44388</v>
+      </c>
+      <c r="B926" s="25"/>
+      <c r="C926" s="25"/>
+      <c r="D926" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
@@ -14188,7 +14271,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-07-2021 00-31-30
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1638" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B525315-2A38-4420-82DD-A9D0C2779791}"/>
+  <xr:revisionPtr revIDLastSave="1640" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30699541-DE82-4E0E-A9CB-8EAD3417C5F7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12990" windowHeight="10335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
@@ -386,11 +386,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -937,7 +937,7 @@
   </borders>
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -981,15 +981,15 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="18" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="18" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -997,7 +997,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="18" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1026,7 +1026,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="46">
@@ -1111,7 +1111,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1130,7 +1130,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1149,7 +1149,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1213,7 +1213,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1244,7 +1244,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="169" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1651,8 +1651,8 @@
   <dimension ref="A1:W933"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A919" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B934" sqref="B934"/>
+      <pane ySplit="3" topLeftCell="A918" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B933" sqref="B933"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14329,7 +14329,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-10-2021 00-30-50
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1640" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30699541-DE82-4E0E-A9CB-8EAD3417C5F7}"/>
+  <xr:revisionPtr revIDLastSave="1644" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A45E4075-5B0D-4262-BA84-09F37ABB1222}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H933" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H933" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H940" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H940" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W933"/>
+  <dimension ref="A1:W940"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A918" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B933" sqref="B933"/>
+      <pane ySplit="3" topLeftCell="A926" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B941" sqref="B941"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3878,7 +3878,9 @@
         <v>356.39</v>
       </c>
       <c r="Q51" s="21"/>
-      <c r="R51" s="21"/>
+      <c r="R51" s="21">
+        <v>246.1</v>
+      </c>
       <c r="S51" s="21"/>
       <c r="T51" s="21"/>
       <c r="U51" s="21"/>
@@ -14307,6 +14309,62 @@
       <c r="C933" s="25"/>
       <c r="D933" s="25"/>
     </row>
+    <row r="934" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A934" s="8">
+        <v>44396</v>
+      </c>
+      <c r="B934" s="25"/>
+      <c r="C934" s="25"/>
+      <c r="D934" s="25"/>
+    </row>
+    <row r="935" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A935" s="8">
+        <v>44397</v>
+      </c>
+      <c r="B935" s="25"/>
+      <c r="C935" s="25"/>
+      <c r="D935" s="25"/>
+    </row>
+    <row r="936" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A936" s="8">
+        <v>44398</v>
+      </c>
+      <c r="B936" s="25"/>
+      <c r="C936" s="25"/>
+      <c r="D936" s="25"/>
+    </row>
+    <row r="937" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A937" s="8">
+        <v>44399</v>
+      </c>
+      <c r="B937" s="25"/>
+      <c r="C937" s="25"/>
+      <c r="D937" s="25"/>
+    </row>
+    <row r="938" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A938" s="8">
+        <v>44400</v>
+      </c>
+      <c r="B938" s="25"/>
+      <c r="C938" s="25"/>
+      <c r="D938" s="25"/>
+    </row>
+    <row r="939" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A939" s="8">
+        <v>44401</v>
+      </c>
+      <c r="B939" s="25"/>
+      <c r="C939" s="25"/>
+      <c r="D939" s="25"/>
+    </row>
+    <row r="940" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A940" s="8">
+        <v>44402</v>
+      </c>
+      <c r="B940" s="25"/>
+      <c r="C940" s="25"/>
+      <c r="D940" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -14329,7 +14387,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-14-2021 00-30-33
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1644" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A45E4075-5B0D-4262-BA84-09F37ABB1222}"/>
+  <xr:revisionPtr revIDLastSave="1649" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{171966F3-F39B-4BAC-9F48-5879888C7102}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14140,8 +14140,17 @@
       <c r="B912" s="25"/>
       <c r="C912" s="25"/>
       <c r="D912" s="25"/>
-    </row>
-    <row r="913" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E912" s="21">
+        <v>3.41</v>
+      </c>
+      <c r="F912" s="21">
+        <v>3.29</v>
+      </c>
+      <c r="G912" s="21">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="913" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A913" s="8">
         <v>44375</v>
       </c>
@@ -14149,7 +14158,7 @@
       <c r="C913" s="25"/>
       <c r="D913" s="25"/>
     </row>
-    <row r="914" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A914" s="8">
         <v>44376</v>
       </c>
@@ -14157,7 +14166,7 @@
       <c r="C914" s="25"/>
       <c r="D914" s="25"/>
     </row>
-    <row r="915" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A915" s="8">
         <v>44377</v>
       </c>
@@ -14165,7 +14174,7 @@
       <c r="C915" s="25"/>
       <c r="D915" s="25"/>
     </row>
-    <row r="916" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A916" s="8">
         <v>44378</v>
       </c>
@@ -14173,7 +14182,7 @@
       <c r="C916" s="25"/>
       <c r="D916" s="25"/>
     </row>
-    <row r="917" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A917" s="8">
         <v>44379</v>
       </c>
@@ -14181,7 +14190,7 @@
       <c r="C917" s="25"/>
       <c r="D917" s="25"/>
     </row>
-    <row r="918" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A918" s="8">
         <v>44380</v>
       </c>
@@ -14189,15 +14198,24 @@
       <c r="C918" s="25"/>
       <c r="D918" s="25"/>
     </row>
-    <row r="919" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A919" s="8">
         <v>44381</v>
       </c>
       <c r="B919" s="25"/>
       <c r="C919" s="25"/>
       <c r="D919" s="25"/>
-    </row>
-    <row r="920" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E919">
+        <v>3.45</v>
+      </c>
+      <c r="F919">
+        <v>3.32</v>
+      </c>
+      <c r="G919">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="920" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A920" s="8">
         <v>44382</v>
       </c>
@@ -14205,7 +14223,7 @@
       <c r="C920" s="25"/>
       <c r="D920" s="25"/>
     </row>
-    <row r="921" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A921" s="8">
         <v>44383</v>
       </c>
@@ -14213,7 +14231,7 @@
       <c r="C921" s="25"/>
       <c r="D921" s="25"/>
     </row>
-    <row r="922" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A922" s="8">
         <v>44384</v>
       </c>
@@ -14221,7 +14239,7 @@
       <c r="C922" s="25"/>
       <c r="D922" s="25"/>
     </row>
-    <row r="923" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A923" s="8">
         <v>44385</v>
       </c>
@@ -14229,7 +14247,7 @@
       <c r="C923" s="25"/>
       <c r="D923" s="25"/>
     </row>
-    <row r="924" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A924" s="8">
         <v>44386</v>
       </c>
@@ -14237,7 +14255,7 @@
       <c r="C924" s="25"/>
       <c r="D924" s="25"/>
     </row>
-    <row r="925" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A925" s="8">
         <v>44387</v>
       </c>
@@ -14245,7 +14263,7 @@
       <c r="C925" s="25"/>
       <c r="D925" s="25"/>
     </row>
-    <row r="926" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A926" s="8">
         <v>44388</v>
       </c>
@@ -14253,7 +14271,7 @@
       <c r="C926" s="25"/>
       <c r="D926" s="25"/>
     </row>
-    <row r="927" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A927" s="8">
         <v>44389</v>
       </c>
@@ -14261,7 +14279,7 @@
       <c r="C927" s="25"/>
       <c r="D927" s="25"/>
     </row>
-    <row r="928" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A928" s="8">
         <v>44390</v>
       </c>
@@ -14387,7 +14405,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-17-2021 00-12-20
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1649" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{171966F3-F39B-4BAC-9F48-5879888C7102}"/>
+  <xr:revisionPtr revIDLastSave="1660" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F0F28C7-8B6B-49B7-BA2E-3C887B067722}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H940" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H940" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H947" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H947" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W940"/>
+  <dimension ref="A1:W947"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A926" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B941" sqref="B941"/>
+      <pane ySplit="3" topLeftCell="A934" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B948" sqref="B948"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3524,7 +3524,7 @@
         <v>89167.92</v>
       </c>
       <c r="O43" s="2">
-        <v>533206.505</v>
+        <v>533206.50500000012</v>
       </c>
       <c r="P43" s="2">
         <v>403.34</v>
@@ -3563,7 +3563,7 @@
         <v>228.29929707050536</v>
       </c>
       <c r="N44" s="2">
-        <v>78383.501999999993</v>
+        <v>78383.502000000008</v>
       </c>
       <c r="O44" s="2">
         <v>493292.21799999999</v>
@@ -4039,7 +4039,7 @@
         <v>277.07312193278085</v>
       </c>
       <c r="N55" s="2">
-        <v>279712.50599999999</v>
+        <v>279642.43900000001</v>
       </c>
       <c r="O55" s="2">
         <v>887233.929</v>
@@ -4078,8 +4078,12 @@
         <v>Mayo, 2021</v>
       </c>
       <c r="M56" s="21"/>
-      <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
+      <c r="N56" s="2">
+        <v>158647.59099999999</v>
+      </c>
+      <c r="O56" s="2">
+        <v>987069.89500000002</v>
+      </c>
       <c r="P56" s="2">
         <v>374.07</v>
       </c>
@@ -14382,6 +14386,62 @@
       <c r="B940" s="25"/>
       <c r="C940" s="25"/>
       <c r="D940" s="25"/>
+    </row>
+    <row r="941" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A941" s="8">
+        <v>44403</v>
+      </c>
+      <c r="B941" s="25"/>
+      <c r="C941" s="25"/>
+      <c r="D941" s="25"/>
+    </row>
+    <row r="942" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A942" s="8">
+        <v>44404</v>
+      </c>
+      <c r="B942" s="25"/>
+      <c r="C942" s="25"/>
+      <c r="D942" s="25"/>
+    </row>
+    <row r="943" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A943" s="8">
+        <v>44405</v>
+      </c>
+      <c r="B943" s="25"/>
+      <c r="C943" s="25"/>
+      <c r="D943" s="25"/>
+    </row>
+    <row r="944" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A944" s="8">
+        <v>44406</v>
+      </c>
+      <c r="B944" s="25"/>
+      <c r="C944" s="25"/>
+      <c r="D944" s="25"/>
+    </row>
+    <row r="945" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A945" s="8">
+        <v>44407</v>
+      </c>
+      <c r="B945" s="25"/>
+      <c r="C945" s="25"/>
+      <c r="D945" s="25"/>
+    </row>
+    <row r="946" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A946" s="8">
+        <v>44408</v>
+      </c>
+      <c r="B946" s="25"/>
+      <c r="C946" s="25"/>
+      <c r="D946" s="25"/>
+    </row>
+    <row r="947" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A947" s="8">
+        <v>44409</v>
+      </c>
+      <c r="B947" s="25"/>
+      <c r="C947" s="25"/>
+      <c r="D947" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-21-2021 02-00-41
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1660" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F0F28C7-8B6B-49B7-BA2E-3C887B067722}"/>
+  <xr:revisionPtr revIDLastSave="1664" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2B46B0C-74D8-4D47-931E-C07E4E49DE4F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1651,7 +1651,7 @@
   <dimension ref="A1:W947"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A934" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A933" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B948" sqref="B948"/>
     </sheetView>
   </sheetViews>
@@ -14175,8 +14175,12 @@
         <v>44377</v>
       </c>
       <c r="B915" s="25"/>
-      <c r="C915" s="25"/>
-      <c r="D915" s="25"/>
+      <c r="C915" s="25">
+        <v>1.23</v>
+      </c>
+      <c r="D915" s="23">
+        <v>1505.35</v>
+      </c>
     </row>
     <row r="916" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A916" s="8">
@@ -14274,6 +14278,15 @@
       <c r="B926" s="25"/>
       <c r="C926" s="25"/>
       <c r="D926" s="25"/>
+      <c r="E926" s="21">
+        <v>3.45</v>
+      </c>
+      <c r="F926" s="21">
+        <v>3.32</v>
+      </c>
+      <c r="G926" s="21">
+        <v>2.91</v>
+      </c>
     </row>
     <row r="927" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A927" s="8">
@@ -14465,7 +14478,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-23-2021 22-31-32
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1664" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2B46B0C-74D8-4D47-931E-C07E4E49DE4F}"/>
+  <xr:revisionPtr revIDLastSave="1667" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A02DE5C2-4CBD-43E3-918E-D24059D0457E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1651,7 +1651,7 @@
   <dimension ref="A1:W947"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A933" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A934" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B948" sqref="B948"/>
     </sheetView>
   </sheetViews>
@@ -4077,7 +4077,9 @@
         <f t="shared" ref="L56" si="7">+K56&amp;", "&amp;J56</f>
         <v>Mayo, 2021</v>
       </c>
-      <c r="M56" s="21"/>
+      <c r="M56" s="24">
+        <v>275.68849948928772</v>
+      </c>
       <c r="N56" s="2">
         <v>158647.59099999999</v>
       </c>
@@ -4123,7 +4125,7 @@
         <f>+K57&amp;", "&amp;J57</f>
         <v>Junio, 2021</v>
       </c>
-      <c r="M57" s="21"/>
+      <c r="M57" s="24"/>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
@@ -14478,7 +14480,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-24-2021 00-30-49
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1667" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A02DE5C2-4CBD-43E3-918E-D24059D0457E}"/>
+  <xr:revisionPtr revIDLastSave="1668" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0FFF703-0437-4E69-8BD9-686EECF5AB00}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="PANAMA" sheetId="2" r:id="rId1"/>
     <sheet name="Fuentes" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H947" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H947" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H954" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H954" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W947"/>
+  <dimension ref="A1:W954"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A934" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B948" sqref="B948"/>
+      <pane ySplit="3" topLeftCell="A943" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A946" sqref="A946:A954"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14457,6 +14457,62 @@
       <c r="B947" s="25"/>
       <c r="C947" s="25"/>
       <c r="D947" s="25"/>
+    </row>
+    <row r="948" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A948" s="8">
+        <v>44410</v>
+      </c>
+      <c r="B948" s="25"/>
+      <c r="C948" s="25"/>
+      <c r="D948" s="25"/>
+    </row>
+    <row r="949" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A949" s="8">
+        <v>44411</v>
+      </c>
+      <c r="B949" s="25"/>
+      <c r="C949" s="25"/>
+      <c r="D949" s="25"/>
+    </row>
+    <row r="950" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A950" s="8">
+        <v>44412</v>
+      </c>
+      <c r="B950" s="25"/>
+      <c r="C950" s="25"/>
+      <c r="D950" s="25"/>
+    </row>
+    <row r="951" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A951" s="8">
+        <v>44413</v>
+      </c>
+      <c r="B951" s="25"/>
+      <c r="C951" s="25"/>
+      <c r="D951" s="25"/>
+    </row>
+    <row r="952" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A952" s="8">
+        <v>44414</v>
+      </c>
+      <c r="B952" s="25"/>
+      <c r="C952" s="25"/>
+      <c r="D952" s="25"/>
+    </row>
+    <row r="953" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A953" s="8">
+        <v>44415</v>
+      </c>
+      <c r="B953" s="25"/>
+      <c r="C953" s="25"/>
+      <c r="D953" s="25"/>
+    </row>
+    <row r="954" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A954" s="8">
+        <v>44416</v>
+      </c>
+      <c r="B954" s="25"/>
+      <c r="C954" s="25"/>
+      <c r="D954" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-24-2021 02-00-47
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1651,8 +1651,8 @@
   <dimension ref="A1:W954"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A943" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A946" sqref="A946:A954"/>
+      <pane ySplit="3" topLeftCell="A940" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B955" sqref="B955"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-28-2021 00-30-37
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1668" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0FFF703-0437-4E69-8BD9-686EECF5AB00}"/>
+  <xr:revisionPtr revIDLastSave="1671" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72FB842B-0C8F-4BD0-8B18-EB735BBE63A0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14306,7 +14306,7 @@
       <c r="C928" s="25"/>
       <c r="D928" s="25"/>
     </row>
-    <row r="929" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="929" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A929" s="8">
         <v>44391</v>
       </c>
@@ -14314,7 +14314,7 @@
       <c r="C929" s="25"/>
       <c r="D929" s="25"/>
     </row>
-    <row r="930" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="930" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A930" s="8">
         <v>44392</v>
       </c>
@@ -14322,7 +14322,7 @@
       <c r="C930" s="25"/>
       <c r="D930" s="25"/>
     </row>
-    <row r="931" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="931" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A931" s="8">
         <v>44393</v>
       </c>
@@ -14330,7 +14330,7 @@
       <c r="C931" s="25"/>
       <c r="D931" s="25"/>
     </row>
-    <row r="932" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="932" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A932" s="8">
         <v>44394</v>
       </c>
@@ -14338,15 +14338,24 @@
       <c r="C932" s="25"/>
       <c r="D932" s="25"/>
     </row>
-    <row r="933" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="933" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A933" s="8">
         <v>44395</v>
       </c>
       <c r="B933" s="25"/>
       <c r="C933" s="25"/>
       <c r="D933" s="25"/>
-    </row>
-    <row r="934" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E933">
+        <v>3.55</v>
+      </c>
+      <c r="F933">
+        <v>3.4</v>
+      </c>
+      <c r="G933">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="934" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A934" s="8">
         <v>44396</v>
       </c>
@@ -14354,7 +14363,7 @@
       <c r="C934" s="25"/>
       <c r="D934" s="25"/>
     </row>
-    <row r="935" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="935" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A935" s="8">
         <v>44397</v>
       </c>
@@ -14362,7 +14371,7 @@
       <c r="C935" s="25"/>
       <c r="D935" s="25"/>
     </row>
-    <row r="936" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="936" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A936" s="8">
         <v>44398</v>
       </c>
@@ -14370,7 +14379,7 @@
       <c r="C936" s="25"/>
       <c r="D936" s="25"/>
     </row>
-    <row r="937" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="937" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A937" s="8">
         <v>44399</v>
       </c>
@@ -14378,7 +14387,7 @@
       <c r="C937" s="25"/>
       <c r="D937" s="25"/>
     </row>
-    <row r="938" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="938" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A938" s="8">
         <v>44400</v>
       </c>
@@ -14386,7 +14395,7 @@
       <c r="C938" s="25"/>
       <c r="D938" s="25"/>
     </row>
-    <row r="939" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="939" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A939" s="8">
         <v>44401</v>
       </c>
@@ -14394,7 +14403,7 @@
       <c r="C939" s="25"/>
       <c r="D939" s="25"/>
     </row>
-    <row r="940" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="940" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A940" s="8">
         <v>44402</v>
       </c>
@@ -14402,7 +14411,7 @@
       <c r="C940" s="25"/>
       <c r="D940" s="25"/>
     </row>
-    <row r="941" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A941" s="8">
         <v>44403</v>
       </c>
@@ -14410,7 +14419,7 @@
       <c r="C941" s="25"/>
       <c r="D941" s="25"/>
     </row>
-    <row r="942" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="942" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A942" s="8">
         <v>44404</v>
       </c>
@@ -14418,7 +14427,7 @@
       <c r="C942" s="25"/>
       <c r="D942" s="25"/>
     </row>
-    <row r="943" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="943" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A943" s="8">
         <v>44405</v>
       </c>
@@ -14426,7 +14435,7 @@
       <c r="C943" s="25"/>
       <c r="D943" s="25"/>
     </row>
-    <row r="944" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="944" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A944" s="8">
         <v>44406</v>
       </c>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-31-2021 00-30-59
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1671" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72FB842B-0C8F-4BD0-8B18-EB735BBE63A0}"/>
+  <xr:revisionPtr revIDLastSave="1673" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90C47DDF-77A7-4902-86B0-4F414964BF8A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="104">
   <si>
     <t>Indicadores diarios</t>
   </si>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H954" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H954" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H961" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H961" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1333,8 +1333,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R59" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
-  <autoFilter ref="J3:R59" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361D6DB9-DB5F-41DB-A2B1-3827A7E68BA3}" name="Indicadores_mes_PN" displayName="Indicadores_mes_PN" ref="J3:R60" totalsRowShown="0" headerRowDxfId="8" headerRowCellStyle="Millares">
+  <autoFilter ref="J3:R60" xr:uid="{3CCA25B4-1DC8-4605-9570-70ABC518C188}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{07F4ADCA-FED6-473F-B251-F3879D4D00F0}" name="Año" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{D9E356F9-F5BF-4968-8B4E-9432BA68AA6E}" name="Mes" dataDxfId="6"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W954"/>
+  <dimension ref="A1:W961"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A940" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B955" sqref="B955"/>
+      <pane ySplit="3" topLeftCell="A947" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B962" sqref="B962"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4217,13 +4217,20 @@
       <c r="G60" s="21"/>
       <c r="H60" s="21"/>
       <c r="I60" s="21"/>
-      <c r="J60" s="21"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="21"/>
+      <c r="J60" s="9">
+        <v>2021</v>
+      </c>
+      <c r="K60" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L60" s="9" t="str">
+        <f t="shared" ref="L60" si="9">+K60&amp;", "&amp;J60</f>
+        <v>Septiembre, 2021</v>
+      </c>
       <c r="M60" s="21"/>
-      <c r="N60" s="21"/>
-      <c r="O60" s="21"/>
-      <c r="P60" s="21"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
       <c r="Q60" s="21"/>
       <c r="R60" s="21"/>
       <c r="S60" s="21"/>
@@ -14523,6 +14530,62 @@
       <c r="C954" s="25"/>
       <c r="D954" s="25"/>
     </row>
+    <row r="955" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A955" s="8">
+        <v>44417</v>
+      </c>
+      <c r="B955" s="25"/>
+      <c r="C955" s="25"/>
+      <c r="D955" s="25"/>
+    </row>
+    <row r="956" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A956" s="8">
+        <v>44418</v>
+      </c>
+      <c r="B956" s="25"/>
+      <c r="C956" s="25"/>
+      <c r="D956" s="25"/>
+    </row>
+    <row r="957" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A957" s="8">
+        <v>44419</v>
+      </c>
+      <c r="B957" s="25"/>
+      <c r="C957" s="25"/>
+      <c r="D957" s="25"/>
+    </row>
+    <row r="958" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A958" s="8">
+        <v>44420</v>
+      </c>
+      <c r="B958" s="25"/>
+      <c r="C958" s="25"/>
+      <c r="D958" s="25"/>
+    </row>
+    <row r="959" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A959" s="8">
+        <v>44421</v>
+      </c>
+      <c r="B959" s="25"/>
+      <c r="C959" s="25"/>
+      <c r="D959" s="25"/>
+    </row>
+    <row r="960" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A960" s="8">
+        <v>44422</v>
+      </c>
+      <c r="B960" s="25"/>
+      <c r="C960" s="25"/>
+      <c r="D960" s="25"/>
+    </row>
+    <row r="961" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A961" s="8">
+        <v>44423</v>
+      </c>
+      <c r="B961" s="25"/>
+      <c r="C961" s="25"/>
+      <c r="D961" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -14545,7 +14608,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-04-2021 02-00-53
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1673" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90C47DDF-77A7-4902-86B0-4F414964BF8A}"/>
+  <xr:revisionPtr revIDLastSave="1686" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1B918D1-1E76-4F68-A169-7210813F1724}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3605,7 +3605,7 @@
         <v>243.00656400193247</v>
       </c>
       <c r="N45" s="2">
-        <v>107559.02800000001</v>
+        <v>107559.02799999998</v>
       </c>
       <c r="O45" s="2">
         <v>523101.42599999998</v>
@@ -4081,7 +4081,7 @@
         <v>275.68849948928772</v>
       </c>
       <c r="N56" s="2">
-        <v>158647.59099999999</v>
+        <v>158647.59100000001</v>
       </c>
       <c r="O56" s="2">
         <v>987069.89500000002</v>
@@ -4126,9 +4126,13 @@
         <v>Junio, 2021</v>
       </c>
       <c r="M57" s="24"/>
-      <c r="N57" s="2"/>
+      <c r="N57" s="2">
+        <v>420338.06900000002</v>
+      </c>
       <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
+      <c r="P57" s="2">
+        <v>379.77</v>
+      </c>
       <c r="Q57" s="21"/>
       <c r="R57" s="21"/>
       <c r="S57" s="21"/>
@@ -14417,6 +14421,15 @@
       <c r="B940" s="25"/>
       <c r="C940" s="25"/>
       <c r="D940" s="25"/>
+      <c r="E940" s="21">
+        <v>3.55</v>
+      </c>
+      <c r="F940" s="21">
+        <v>3.4</v>
+      </c>
+      <c r="G940" s="21">
+        <v>2.93</v>
+      </c>
     </row>
     <row r="941" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A941" s="8">
@@ -14608,7 +14621,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-07-2021 00-30-27
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1686" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1B918D1-1E76-4F68-A169-7210813F1724}"/>
+  <xr:revisionPtr revIDLastSave="1687" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0F7E0A2-7822-4846-A3B7-461597C7EB50}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H961" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H961" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H968" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H968" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W961"/>
+  <dimension ref="A1:W968"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A947" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B962" sqref="B962"/>
+      <pane ySplit="3" topLeftCell="A954" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B969" sqref="B969"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14598,6 +14598,62 @@
       <c r="B961" s="25"/>
       <c r="C961" s="25"/>
       <c r="D961" s="25"/>
+    </row>
+    <row r="962" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A962" s="8">
+        <v>44424</v>
+      </c>
+      <c r="B962" s="25"/>
+      <c r="C962" s="25"/>
+      <c r="D962" s="25"/>
+    </row>
+    <row r="963" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A963" s="8">
+        <v>44425</v>
+      </c>
+      <c r="B963" s="25"/>
+      <c r="C963" s="25"/>
+      <c r="D963" s="25"/>
+    </row>
+    <row r="964" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A964" s="8">
+        <v>44426</v>
+      </c>
+      <c r="B964" s="25"/>
+      <c r="C964" s="25"/>
+      <c r="D964" s="25"/>
+    </row>
+    <row r="965" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A965" s="8">
+        <v>44427</v>
+      </c>
+      <c r="B965" s="25"/>
+      <c r="C965" s="25"/>
+      <c r="D965" s="25"/>
+    </row>
+    <row r="966" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A966" s="8">
+        <v>44428</v>
+      </c>
+      <c r="B966" s="25"/>
+      <c r="C966" s="25"/>
+      <c r="D966" s="25"/>
+    </row>
+    <row r="967" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A967" s="8">
+        <v>44429</v>
+      </c>
+      <c r="B967" s="25"/>
+      <c r="C967" s="25"/>
+      <c r="D967" s="25"/>
+    </row>
+    <row r="968" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A968" s="8">
+        <v>44430</v>
+      </c>
+      <c r="B968" s="25"/>
+      <c r="C968" s="25"/>
+      <c r="D968" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-11-2021 00-30-57
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1687" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0F7E0A2-7822-4846-A3B7-461597C7EB50}"/>
+  <xr:revisionPtr revIDLastSave="1690" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7C1B3D6-A871-44E0-BD13-1ED9B99C128A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14463,7 +14463,7 @@
       <c r="C944" s="25"/>
       <c r="D944" s="25"/>
     </row>
-    <row r="945" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="945" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A945" s="8">
         <v>44407</v>
       </c>
@@ -14471,7 +14471,7 @@
       <c r="C945" s="25"/>
       <c r="D945" s="25"/>
     </row>
-    <row r="946" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="946" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A946" s="8">
         <v>44408</v>
       </c>
@@ -14479,15 +14479,24 @@
       <c r="C946" s="25"/>
       <c r="D946" s="25"/>
     </row>
-    <row r="947" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="947" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A947" s="8">
         <v>44409</v>
       </c>
       <c r="B947" s="25"/>
       <c r="C947" s="25"/>
       <c r="D947" s="25"/>
-    </row>
-    <row r="948" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E947">
+        <v>3.53</v>
+      </c>
+      <c r="F947">
+        <v>3.4</v>
+      </c>
+      <c r="G947">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="948" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A948" s="8">
         <v>44410</v>
       </c>
@@ -14495,7 +14504,7 @@
       <c r="C948" s="25"/>
       <c r="D948" s="25"/>
     </row>
-    <row r="949" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A949" s="8">
         <v>44411</v>
       </c>
@@ -14503,7 +14512,7 @@
       <c r="C949" s="25"/>
       <c r="D949" s="25"/>
     </row>
-    <row r="950" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="950" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A950" s="8">
         <v>44412</v>
       </c>
@@ -14511,7 +14520,7 @@
       <c r="C950" s="25"/>
       <c r="D950" s="25"/>
     </row>
-    <row r="951" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="951" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A951" s="8">
         <v>44413</v>
       </c>
@@ -14519,7 +14528,7 @@
       <c r="C951" s="25"/>
       <c r="D951" s="25"/>
     </row>
-    <row r="952" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="952" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A952" s="8">
         <v>44414</v>
       </c>
@@ -14527,7 +14536,7 @@
       <c r="C952" s="25"/>
       <c r="D952" s="25"/>
     </row>
-    <row r="953" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="953" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A953" s="8">
         <v>44415</v>
       </c>
@@ -14535,7 +14544,7 @@
       <c r="C953" s="25"/>
       <c r="D953" s="25"/>
     </row>
-    <row r="954" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="954" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A954" s="8">
         <v>44416</v>
       </c>
@@ -14543,7 +14552,7 @@
       <c r="C954" s="25"/>
       <c r="D954" s="25"/>
     </row>
-    <row r="955" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="955" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A955" s="8">
         <v>44417</v>
       </c>
@@ -14551,7 +14560,7 @@
       <c r="C955" s="25"/>
       <c r="D955" s="25"/>
     </row>
-    <row r="956" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="956" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A956" s="8">
         <v>44418</v>
       </c>
@@ -14559,7 +14568,7 @@
       <c r="C956" s="25"/>
       <c r="D956" s="25"/>
     </row>
-    <row r="957" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="957" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A957" s="8">
         <v>44419</v>
       </c>
@@ -14567,7 +14576,7 @@
       <c r="C957" s="25"/>
       <c r="D957" s="25"/>
     </row>
-    <row r="958" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="958" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A958" s="8">
         <v>44420</v>
       </c>
@@ -14575,7 +14584,7 @@
       <c r="C958" s="25"/>
       <c r="D958" s="25"/>
     </row>
-    <row r="959" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="959" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A959" s="8">
         <v>44421</v>
       </c>
@@ -14583,7 +14592,7 @@
       <c r="C959" s="25"/>
       <c r="D959" s="25"/>
     </row>
-    <row r="960" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="960" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A960" s="8">
         <v>44422</v>
       </c>
@@ -14677,7 +14686,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-14-2021 18-36-32
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1690" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7C1B3D6-A871-44E0-BD13-1ED9B99C128A}"/>
+  <xr:revisionPtr revIDLastSave="1693" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32981164-A1B8-433E-91EE-93683E4CFE6F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H968" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H968" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H975" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H975" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W968"/>
+  <dimension ref="A1:W975"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A954" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B969" sqref="B969"/>
+      <pane ySplit="3" topLeftCell="A961" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B976" sqref="B976"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="Q51" s="21"/>
       <c r="R51" s="21">
-        <v>246.1</v>
+        <v>-31.6</v>
       </c>
       <c r="S51" s="21"/>
       <c r="T51" s="21"/>
@@ -4006,7 +4006,9 @@
         <v>368.69</v>
       </c>
       <c r="Q54" s="21"/>
-      <c r="R54" s="21"/>
+      <c r="R54" s="21">
+        <v>-26.7</v>
+      </c>
       <c r="S54" s="21"/>
       <c r="T54" s="21"/>
       <c r="U54" s="21"/>
@@ -14664,6 +14666,62 @@
       <c r="C968" s="25"/>
       <c r="D968" s="25"/>
     </row>
+    <row r="969" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A969" s="8">
+        <v>44431</v>
+      </c>
+      <c r="B969" s="25"/>
+      <c r="C969" s="25"/>
+      <c r="D969" s="25"/>
+    </row>
+    <row r="970" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A970" s="8">
+        <v>44432</v>
+      </c>
+      <c r="B970" s="25"/>
+      <c r="C970" s="25"/>
+      <c r="D970" s="25"/>
+    </row>
+    <row r="971" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A971" s="8">
+        <v>44433</v>
+      </c>
+      <c r="B971" s="25"/>
+      <c r="C971" s="25"/>
+      <c r="D971" s="25"/>
+    </row>
+    <row r="972" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A972" s="8">
+        <v>44434</v>
+      </c>
+      <c r="B972" s="25"/>
+      <c r="C972" s="25"/>
+      <c r="D972" s="25"/>
+    </row>
+    <row r="973" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A973" s="8">
+        <v>44435</v>
+      </c>
+      <c r="B973" s="25"/>
+      <c r="C973" s="25"/>
+      <c r="D973" s="25"/>
+    </row>
+    <row r="974" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A974" s="8">
+        <v>44436</v>
+      </c>
+      <c r="B974" s="25"/>
+      <c r="C974" s="25"/>
+      <c r="D974" s="25"/>
+    </row>
+    <row r="975" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A975" s="8">
+        <v>44437</v>
+      </c>
+      <c r="B975" s="25"/>
+      <c r="C975" s="25"/>
+      <c r="D975" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -14686,7 +14744,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-18-2021 00-30-55
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1693" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32981164-A1B8-433E-91EE-93683E4CFE6F}"/>
+  <xr:revisionPtr revIDLastSave="1698" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C813A4C-5144-443A-8A9F-555E541CCCAB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4131,7 +4131,9 @@
       <c r="N57" s="2">
         <v>420338.06900000002</v>
       </c>
-      <c r="O57" s="2"/>
+      <c r="O57" s="2">
+        <v>896354.11399999994</v>
+      </c>
       <c r="P57" s="2">
         <v>379.77</v>
       </c>
@@ -14492,10 +14494,10 @@
         <v>3.53</v>
       </c>
       <c r="F947">
-        <v>3.4</v>
+        <v>3.37</v>
       </c>
       <c r="G947">
-        <v>2.93</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="948" spans="1:7" x14ac:dyDescent="0.25">
@@ -14553,6 +14555,15 @@
       <c r="B954" s="25"/>
       <c r="C954" s="25"/>
       <c r="D954" s="25"/>
+      <c r="E954" s="21">
+        <v>3.53</v>
+      </c>
+      <c r="F954" s="21">
+        <v>3.37</v>
+      </c>
+      <c r="G954" s="21">
+        <v>2.89</v>
+      </c>
     </row>
     <row r="955" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A955" s="8">

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-21-2021 00-30-29
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1698" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C813A4C-5144-443A-8A9F-555E541CCCAB}"/>
+  <xr:revisionPtr revIDLastSave="1699" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B53D9B86-AE0B-4843-9B39-A3EEC68FD8C8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H975" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H975" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H982" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H982" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W975"/>
+  <dimension ref="A1:W982"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A961" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B976" sqref="B976"/>
+      <pane ySplit="3" topLeftCell="A968" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A983" sqref="A983"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14733,6 +14733,62 @@
       <c r="C975" s="25"/>
       <c r="D975" s="25"/>
     </row>
+    <row r="976" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A976" s="8">
+        <v>44438</v>
+      </c>
+      <c r="B976" s="25"/>
+      <c r="C976" s="25"/>
+      <c r="D976" s="25"/>
+    </row>
+    <row r="977" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A977" s="8">
+        <v>44439</v>
+      </c>
+      <c r="B977" s="25"/>
+      <c r="C977" s="25"/>
+      <c r="D977" s="25"/>
+    </row>
+    <row r="978" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A978" s="8">
+        <v>44440</v>
+      </c>
+      <c r="B978" s="25"/>
+      <c r="C978" s="25"/>
+      <c r="D978" s="25"/>
+    </row>
+    <row r="979" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A979" s="8">
+        <v>44441</v>
+      </c>
+      <c r="B979" s="25"/>
+      <c r="C979" s="25"/>
+      <c r="D979" s="25"/>
+    </row>
+    <row r="980" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A980" s="8">
+        <v>44442</v>
+      </c>
+      <c r="B980" s="25"/>
+      <c r="C980" s="25"/>
+      <c r="D980" s="25"/>
+    </row>
+    <row r="981" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A981" s="8">
+        <v>44443</v>
+      </c>
+      <c r="B981" s="25"/>
+      <c r="C981" s="25"/>
+      <c r="D981" s="25"/>
+    </row>
+    <row r="982" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A982" s="8">
+        <v>44444</v>
+      </c>
+      <c r="B982" s="25"/>
+      <c r="C982" s="25"/>
+      <c r="D982" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -14755,7 +14811,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-25-2021 00-31-11
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1699" documentId="8_{21879485-51D3-4BBD-9EB2-06C996039B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B53D9B86-AE0B-4843-9B39-A3EEC68FD8C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{C6B00F64-2DA6-484C-A47B-41EFCC98D386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1650,9 +1650,9 @@
   </sheetPr>
   <dimension ref="A1:W982"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A968" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A983" sqref="A983"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N57" sqref="N57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4038,7 +4038,7 @@
         <v>Abril, 2021</v>
       </c>
       <c r="M55" s="24">
-        <v>277.07312193278085</v>
+        <v>299.76761457852291</v>
       </c>
       <c r="N55" s="2">
         <v>279642.43900000001</v>
@@ -4080,7 +4080,7 @@
         <v>Mayo, 2021</v>
       </c>
       <c r="M56" s="24">
-        <v>275.68849948928772</v>
+        <v>306.40588728828141</v>
       </c>
       <c r="N56" s="2">
         <v>158647.59100000001</v>
@@ -4127,7 +4127,9 @@
         <f>+K57&amp;", "&amp;J57</f>
         <v>Junio, 2021</v>
       </c>
-      <c r="M57" s="24"/>
+      <c r="M57" s="24">
+        <v>303.54009691207443</v>
+      </c>
       <c r="N57" s="2">
         <v>420338.06900000002</v>
       </c>
@@ -14480,8 +14482,12 @@
         <v>44408</v>
       </c>
       <c r="B946" s="25"/>
-      <c r="C946" s="25"/>
-      <c r="D946" s="25"/>
+      <c r="C946" s="25">
+        <v>1.23</v>
+      </c>
+      <c r="D946" s="23">
+        <v>1502.65</v>
+      </c>
     </row>
     <row r="947" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A947" s="8">
@@ -14613,15 +14619,24 @@
       <c r="C960" s="25"/>
       <c r="D960" s="25"/>
     </row>
-    <row r="961" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="961" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A961" s="8">
         <v>44423</v>
       </c>
       <c r="B961" s="25"/>
       <c r="C961" s="25"/>
       <c r="D961" s="25"/>
-    </row>
-    <row r="962" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E961">
+        <v>3.55</v>
+      </c>
+      <c r="F961">
+        <v>3.42</v>
+      </c>
+      <c r="G961">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="962" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A962" s="8">
         <v>44424</v>
       </c>
@@ -14629,7 +14644,7 @@
       <c r="C962" s="25"/>
       <c r="D962" s="25"/>
     </row>
-    <row r="963" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="963" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A963" s="8">
         <v>44425</v>
       </c>
@@ -14637,7 +14652,7 @@
       <c r="C963" s="25"/>
       <c r="D963" s="25"/>
     </row>
-    <row r="964" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="964" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A964" s="8">
         <v>44426</v>
       </c>
@@ -14645,7 +14660,7 @@
       <c r="C964" s="25"/>
       <c r="D964" s="25"/>
     </row>
-    <row r="965" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="965" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A965" s="8">
         <v>44427</v>
       </c>
@@ -14653,7 +14668,7 @@
       <c r="C965" s="25"/>
       <c r="D965" s="25"/>
     </row>
-    <row r="966" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="966" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A966" s="8">
         <v>44428</v>
       </c>
@@ -14661,7 +14676,7 @@
       <c r="C966" s="25"/>
       <c r="D966" s="25"/>
     </row>
-    <row r="967" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="967" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A967" s="8">
         <v>44429</v>
       </c>
@@ -14669,7 +14684,7 @@
       <c r="C967" s="25"/>
       <c r="D967" s="25"/>
     </row>
-    <row r="968" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="968" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A968" s="8">
         <v>44430</v>
       </c>
@@ -14677,7 +14692,7 @@
       <c r="C968" s="25"/>
       <c r="D968" s="25"/>
     </row>
-    <row r="969" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="969" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A969" s="8">
         <v>44431</v>
       </c>
@@ -14685,7 +14700,7 @@
       <c r="C969" s="25"/>
       <c r="D969" s="25"/>
     </row>
-    <row r="970" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="970" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A970" s="8">
         <v>44432</v>
       </c>
@@ -14693,7 +14708,7 @@
       <c r="C970" s="25"/>
       <c r="D970" s="25"/>
     </row>
-    <row r="971" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="971" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A971" s="8">
         <v>44433</v>
       </c>
@@ -14701,7 +14716,7 @@
       <c r="C971" s="25"/>
       <c r="D971" s="25"/>
     </row>
-    <row r="972" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="972" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A972" s="8">
         <v>44434</v>
       </c>
@@ -14709,7 +14724,7 @@
       <c r="C972" s="25"/>
       <c r="D972" s="25"/>
     </row>
-    <row r="973" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="973" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A973" s="8">
         <v>44435</v>
       </c>
@@ -14717,7 +14732,7 @@
       <c r="C973" s="25"/>
       <c r="D973" s="25"/>
     </row>
-    <row r="974" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="974" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A974" s="8">
         <v>44436</v>
       </c>
@@ -14725,7 +14740,7 @@
       <c r="C974" s="25"/>
       <c r="D974" s="25"/>
     </row>
-    <row r="975" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="975" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A975" s="8">
         <v>44437</v>
       </c>
@@ -14733,7 +14748,7 @@
       <c r="C975" s="25"/>
       <c r="D975" s="25"/>
     </row>
-    <row r="976" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="976" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A976" s="8">
         <v>44438</v>
       </c>
@@ -14808,10 +14823,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-28-2021 02-01-16
</commit_message>
<xml_diff>
--- a/datacovidpa/ECONOMICOS PN.xlsx
+++ b/datacovidpa/ECONOMICOS PN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{C6B00F64-2DA6-484C-A47B-41EFCC98D386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="14_{C6B00F64-2DA6-484C-A47B-41EFCC98D386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4204ABF-D51F-462D-AE27-5E6E032FFDC5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H982" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A3:H982" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71A19996-DC22-486D-BF8D-97EBA5C503C7}" name="Indicadores_dia_PN" displayName="Indicadores_dia_PN" ref="A3:H989" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:H989" xr:uid="{6D71C6AD-D385-42F5-9CD8-B1007F6F3A09}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F490BF3E-829C-4C70-9AA3-B512D80A1FB4}" name="Fecha" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{5D7EFC02-0FC9-44AC-A1B8-577CBA91C59C}" name="Columna1" dataDxfId="11"/>
@@ -1648,11 +1648,11 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:W982"/>
+  <dimension ref="A1:W989"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N57" sqref="N57"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A975" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B990" sqref="B990"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14804,6 +14804,62 @@
       <c r="C982" s="25"/>
       <c r="D982" s="25"/>
     </row>
+    <row r="983" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A983" s="8">
+        <v>44445</v>
+      </c>
+      <c r="B983" s="25"/>
+      <c r="C983" s="25"/>
+      <c r="D983" s="25"/>
+    </row>
+    <row r="984" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A984" s="8">
+        <v>44446</v>
+      </c>
+      <c r="B984" s="25"/>
+      <c r="C984" s="25"/>
+      <c r="D984" s="25"/>
+    </row>
+    <row r="985" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A985" s="8">
+        <v>44447</v>
+      </c>
+      <c r="B985" s="25"/>
+      <c r="C985" s="25"/>
+      <c r="D985" s="25"/>
+    </row>
+    <row r="986" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A986" s="8">
+        <v>44448</v>
+      </c>
+      <c r="B986" s="25"/>
+      <c r="C986" s="25"/>
+      <c r="D986" s="25"/>
+    </row>
+    <row r="987" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A987" s="8">
+        <v>44449</v>
+      </c>
+      <c r="B987" s="25"/>
+      <c r="C987" s="25"/>
+      <c r="D987" s="25"/>
+    </row>
+    <row r="988" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A988" s="8">
+        <v>44450</v>
+      </c>
+      <c r="B988" s="25"/>
+      <c r="C988" s="25"/>
+      <c r="D988" s="25"/>
+    </row>
+    <row r="989" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A989" s="8">
+        <v>44451</v>
+      </c>
+      <c r="B989" s="25"/>
+      <c r="C989" s="25"/>
+      <c r="D989" s="25"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R16:X27">
     <sortCondition ref="S16:S27"/>
@@ -14823,10 +14879,10 @@
   <dimension ref="A1:Y959"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>